<commit_message>
Corrigir duplicação de +Milionária no menu da landing page
</commit_message>
<xml_diff>
--- a/LoteriasExcel/Lotofacil_edt2.xlsx
+++ b/LoteriasExcel/Lotofacil_edt2.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\Dropbox\! 000 ByPass\Pessoal\99_Loterias\0 - Loterias-Inteligentes\LoteriasExcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F21D250-C897-447A-A770-A64B71EB9FAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD606A7A-1238-4159-9464-BF4FE03A2A0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57930" yWindow="0" windowWidth="25005" windowHeight="10515" tabRatio="876" xr2:uid="{2663372B-AA50-4721-AD6B-5F0B8186ACF5}"/>
+    <workbookView xWindow="66615" yWindow="0" windowWidth="26610" windowHeight="11850" tabRatio="876" xr2:uid="{2663372B-AA50-4721-AD6B-5F0B8186ACF5}"/>
   </bookViews>
   <sheets>
     <sheet name="LOTOFÁCIL" sheetId="3" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -455,10 +455,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69BEFC42-DD13-4DE0-B2AD-D0F44AF8189C}">
-  <dimension ref="A1:P402"/>
+  <dimension ref="A1:P417"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A385" workbookViewId="0">
-      <selection activeCell="A402" sqref="A402:XFD402"/>
+      <selection activeCell="G404" sqref="G404"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -20569,18 +20569,769 @@
         <v>25</v>
       </c>
     </row>
+    <row r="403" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A403">
+        <v>3473</v>
+      </c>
+      <c r="B403">
+        <v>2</v>
+      </c>
+      <c r="C403">
+        <v>3</v>
+      </c>
+      <c r="D403">
+        <v>4</v>
+      </c>
+      <c r="E403">
+        <v>5</v>
+      </c>
+      <c r="F403">
+        <v>6</v>
+      </c>
+      <c r="G403">
+        <v>7</v>
+      </c>
+      <c r="H403">
+        <v>9</v>
+      </c>
+      <c r="I403">
+        <v>12</v>
+      </c>
+      <c r="J403">
+        <v>13</v>
+      </c>
+      <c r="K403">
+        <v>14</v>
+      </c>
+      <c r="L403">
+        <v>17</v>
+      </c>
+      <c r="M403">
+        <v>18</v>
+      </c>
+      <c r="N403">
+        <v>19</v>
+      </c>
+      <c r="O403">
+        <v>23</v>
+      </c>
+      <c r="P403">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="404" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A404">
+        <v>3474</v>
+      </c>
+      <c r="B404">
+        <v>1</v>
+      </c>
+      <c r="C404">
+        <v>4</v>
+      </c>
+      <c r="D404">
+        <v>6</v>
+      </c>
+      <c r="E404">
+        <v>8</v>
+      </c>
+      <c r="F404">
+        <v>9</v>
+      </c>
+      <c r="G404">
+        <v>10</v>
+      </c>
+      <c r="H404">
+        <v>12</v>
+      </c>
+      <c r="I404">
+        <v>13</v>
+      </c>
+      <c r="J404">
+        <v>14</v>
+      </c>
+      <c r="K404">
+        <v>15</v>
+      </c>
+      <c r="L404">
+        <v>18</v>
+      </c>
+      <c r="M404">
+        <v>19</v>
+      </c>
+      <c r="N404">
+        <v>20</v>
+      </c>
+      <c r="O404">
+        <v>21</v>
+      </c>
+      <c r="P404">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="405" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A405">
+        <v>3475</v>
+      </c>
+      <c r="B405">
+        <v>1</v>
+      </c>
+      <c r="C405">
+        <v>3</v>
+      </c>
+      <c r="D405">
+        <v>4</v>
+      </c>
+      <c r="E405">
+        <v>5</v>
+      </c>
+      <c r="F405">
+        <v>6</v>
+      </c>
+      <c r="G405">
+        <v>11</v>
+      </c>
+      <c r="H405">
+        <v>14</v>
+      </c>
+      <c r="I405">
+        <v>15</v>
+      </c>
+      <c r="J405">
+        <v>18</v>
+      </c>
+      <c r="K405">
+        <v>20</v>
+      </c>
+      <c r="L405">
+        <v>21</v>
+      </c>
+      <c r="M405">
+        <v>22</v>
+      </c>
+      <c r="N405">
+        <v>23</v>
+      </c>
+      <c r="O405">
+        <v>24</v>
+      </c>
+      <c r="P405">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="406" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A406">
+        <v>3476</v>
+      </c>
+      <c r="B406">
+        <v>3</v>
+      </c>
+      <c r="C406">
+        <v>5</v>
+      </c>
+      <c r="D406">
+        <v>6</v>
+      </c>
+      <c r="E406">
+        <v>7</v>
+      </c>
+      <c r="F406">
+        <v>8</v>
+      </c>
+      <c r="G406">
+        <v>10</v>
+      </c>
+      <c r="H406">
+        <v>12</v>
+      </c>
+      <c r="I406">
+        <v>15</v>
+      </c>
+      <c r="J406">
+        <v>16</v>
+      </c>
+      <c r="K406">
+        <v>17</v>
+      </c>
+      <c r="L406">
+        <v>19</v>
+      </c>
+      <c r="M406">
+        <v>20</v>
+      </c>
+      <c r="N406">
+        <v>23</v>
+      </c>
+      <c r="O406">
+        <v>24</v>
+      </c>
+      <c r="P406">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="407" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A407">
+        <v>3477</v>
+      </c>
+      <c r="B407">
+        <v>2</v>
+      </c>
+      <c r="C407">
+        <v>3</v>
+      </c>
+      <c r="D407">
+        <v>5</v>
+      </c>
+      <c r="E407">
+        <v>6</v>
+      </c>
+      <c r="F407">
+        <v>8</v>
+      </c>
+      <c r="G407">
+        <v>12</v>
+      </c>
+      <c r="H407">
+        <v>15</v>
+      </c>
+      <c r="I407">
+        <v>16</v>
+      </c>
+      <c r="J407">
+        <v>17</v>
+      </c>
+      <c r="K407">
+        <v>18</v>
+      </c>
+      <c r="L407">
+        <v>20</v>
+      </c>
+      <c r="M407">
+        <v>21</v>
+      </c>
+      <c r="N407">
+        <v>23</v>
+      </c>
+      <c r="O407">
+        <v>24</v>
+      </c>
+      <c r="P407">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="408" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A408">
+        <v>3478</v>
+      </c>
+      <c r="B408">
+        <v>1</v>
+      </c>
+      <c r="C408">
+        <v>4</v>
+      </c>
+      <c r="D408">
+        <v>5</v>
+      </c>
+      <c r="E408">
+        <v>6</v>
+      </c>
+      <c r="F408">
+        <v>7</v>
+      </c>
+      <c r="G408">
+        <v>8</v>
+      </c>
+      <c r="H408">
+        <v>9</v>
+      </c>
+      <c r="I408">
+        <v>10</v>
+      </c>
+      <c r="J408">
+        <v>12</v>
+      </c>
+      <c r="K408">
+        <v>14</v>
+      </c>
+      <c r="L408">
+        <v>15</v>
+      </c>
+      <c r="M408">
+        <v>17</v>
+      </c>
+      <c r="N408">
+        <v>21</v>
+      </c>
+      <c r="O408">
+        <v>22</v>
+      </c>
+      <c r="P408">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="409" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A409">
+        <v>3479</v>
+      </c>
+      <c r="B409">
+        <v>1</v>
+      </c>
+      <c r="C409">
+        <v>5</v>
+      </c>
+      <c r="D409">
+        <v>6</v>
+      </c>
+      <c r="E409">
+        <v>8</v>
+      </c>
+      <c r="F409">
+        <v>9</v>
+      </c>
+      <c r="G409">
+        <v>10</v>
+      </c>
+      <c r="H409">
+        <v>12</v>
+      </c>
+      <c r="I409">
+        <v>13</v>
+      </c>
+      <c r="J409">
+        <v>15</v>
+      </c>
+      <c r="K409">
+        <v>16</v>
+      </c>
+      <c r="L409">
+        <v>18</v>
+      </c>
+      <c r="M409">
+        <v>19</v>
+      </c>
+      <c r="N409">
+        <v>23</v>
+      </c>
+      <c r="O409">
+        <v>24</v>
+      </c>
+      <c r="P409">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="410" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A410">
+        <v>3480</v>
+      </c>
+      <c r="B410">
+        <v>3</v>
+      </c>
+      <c r="C410">
+        <v>5</v>
+      </c>
+      <c r="D410">
+        <v>6</v>
+      </c>
+      <c r="E410">
+        <v>8</v>
+      </c>
+      <c r="F410">
+        <v>9</v>
+      </c>
+      <c r="G410">
+        <v>12</v>
+      </c>
+      <c r="H410">
+        <v>13</v>
+      </c>
+      <c r="I410">
+        <v>14</v>
+      </c>
+      <c r="J410">
+        <v>15</v>
+      </c>
+      <c r="K410">
+        <v>16</v>
+      </c>
+      <c r="L410">
+        <v>17</v>
+      </c>
+      <c r="M410">
+        <v>20</v>
+      </c>
+      <c r="N410">
+        <v>21</v>
+      </c>
+      <c r="O410">
+        <v>22</v>
+      </c>
+      <c r="P410">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="411" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A411">
+        <v>3481</v>
+      </c>
+      <c r="B411">
+        <v>1</v>
+      </c>
+      <c r="C411">
+        <v>2</v>
+      </c>
+      <c r="D411">
+        <v>3</v>
+      </c>
+      <c r="E411">
+        <v>4</v>
+      </c>
+      <c r="F411">
+        <v>5</v>
+      </c>
+      <c r="G411">
+        <v>7</v>
+      </c>
+      <c r="H411">
+        <v>9</v>
+      </c>
+      <c r="I411">
+        <v>10</v>
+      </c>
+      <c r="J411">
+        <v>13</v>
+      </c>
+      <c r="K411">
+        <v>14</v>
+      </c>
+      <c r="L411">
+        <v>19</v>
+      </c>
+      <c r="M411">
+        <v>21</v>
+      </c>
+      <c r="N411">
+        <v>22</v>
+      </c>
+      <c r="O411">
+        <v>23</v>
+      </c>
+      <c r="P411">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="412" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A412">
+        <v>3482</v>
+      </c>
+      <c r="B412">
+        <v>1</v>
+      </c>
+      <c r="C412">
+        <v>2</v>
+      </c>
+      <c r="D412">
+        <v>4</v>
+      </c>
+      <c r="E412">
+        <v>5</v>
+      </c>
+      <c r="F412">
+        <v>9</v>
+      </c>
+      <c r="G412">
+        <v>10</v>
+      </c>
+      <c r="H412">
+        <v>13</v>
+      </c>
+      <c r="I412">
+        <v>14</v>
+      </c>
+      <c r="J412">
+        <v>15</v>
+      </c>
+      <c r="K412">
+        <v>17</v>
+      </c>
+      <c r="L412">
+        <v>19</v>
+      </c>
+      <c r="M412">
+        <v>20</v>
+      </c>
+      <c r="N412">
+        <v>22</v>
+      </c>
+      <c r="O412">
+        <v>24</v>
+      </c>
+      <c r="P412">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="413" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A413">
+        <v>3483</v>
+      </c>
+      <c r="B413">
+        <v>2</v>
+      </c>
+      <c r="C413">
+        <v>4</v>
+      </c>
+      <c r="D413">
+        <v>7</v>
+      </c>
+      <c r="E413">
+        <v>8</v>
+      </c>
+      <c r="F413">
+        <v>9</v>
+      </c>
+      <c r="G413">
+        <v>12</v>
+      </c>
+      <c r="H413">
+        <v>13</v>
+      </c>
+      <c r="I413">
+        <v>14</v>
+      </c>
+      <c r="J413">
+        <v>15</v>
+      </c>
+      <c r="K413">
+        <v>17</v>
+      </c>
+      <c r="L413">
+        <v>18</v>
+      </c>
+      <c r="M413">
+        <v>20</v>
+      </c>
+      <c r="N413">
+        <v>22</v>
+      </c>
+      <c r="O413">
+        <v>24</v>
+      </c>
+      <c r="P413">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="414" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A414">
+        <v>3484</v>
+      </c>
+      <c r="B414">
+        <v>1</v>
+      </c>
+      <c r="C414">
+        <v>3</v>
+      </c>
+      <c r="D414">
+        <v>4</v>
+      </c>
+      <c r="E414">
+        <v>5</v>
+      </c>
+      <c r="F414">
+        <v>7</v>
+      </c>
+      <c r="G414">
+        <v>8</v>
+      </c>
+      <c r="H414">
+        <v>9</v>
+      </c>
+      <c r="I414">
+        <v>11</v>
+      </c>
+      <c r="J414">
+        <v>13</v>
+      </c>
+      <c r="K414">
+        <v>14</v>
+      </c>
+      <c r="L414">
+        <v>15</v>
+      </c>
+      <c r="M414">
+        <v>17</v>
+      </c>
+      <c r="N414">
+        <v>23</v>
+      </c>
+      <c r="O414">
+        <v>24</v>
+      </c>
+      <c r="P414">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="415" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A415">
+        <v>3485</v>
+      </c>
+      <c r="B415">
+        <v>2</v>
+      </c>
+      <c r="C415">
+        <v>3</v>
+      </c>
+      <c r="D415">
+        <v>4</v>
+      </c>
+      <c r="E415">
+        <v>5</v>
+      </c>
+      <c r="F415">
+        <v>6</v>
+      </c>
+      <c r="G415">
+        <v>9</v>
+      </c>
+      <c r="H415">
+        <v>10</v>
+      </c>
+      <c r="I415">
+        <v>11</v>
+      </c>
+      <c r="J415">
+        <v>12</v>
+      </c>
+      <c r="K415">
+        <v>13</v>
+      </c>
+      <c r="L415">
+        <v>15</v>
+      </c>
+      <c r="M415">
+        <v>18</v>
+      </c>
+      <c r="N415">
+        <v>20</v>
+      </c>
+      <c r="O415">
+        <v>22</v>
+      </c>
+      <c r="P415">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="416" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A416">
+        <v>3486</v>
+      </c>
+      <c r="B416">
+        <v>2</v>
+      </c>
+      <c r="C416">
+        <v>6</v>
+      </c>
+      <c r="D416">
+        <v>7</v>
+      </c>
+      <c r="E416">
+        <v>8</v>
+      </c>
+      <c r="F416">
+        <v>9</v>
+      </c>
+      <c r="G416">
+        <v>10</v>
+      </c>
+      <c r="H416">
+        <v>11</v>
+      </c>
+      <c r="I416">
+        <v>12</v>
+      </c>
+      <c r="J416">
+        <v>16</v>
+      </c>
+      <c r="K416">
+        <v>17</v>
+      </c>
+      <c r="L416">
+        <v>18</v>
+      </c>
+      <c r="M416">
+        <v>19</v>
+      </c>
+      <c r="N416">
+        <v>22</v>
+      </c>
+      <c r="O416">
+        <v>24</v>
+      </c>
+      <c r="P416">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="417" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A417">
+        <v>3487</v>
+      </c>
+      <c r="B417">
+        <v>2</v>
+      </c>
+      <c r="C417">
+        <v>4</v>
+      </c>
+      <c r="D417">
+        <v>5</v>
+      </c>
+      <c r="E417">
+        <v>7</v>
+      </c>
+      <c r="F417">
+        <v>10</v>
+      </c>
+      <c r="G417">
+        <v>12</v>
+      </c>
+      <c r="H417">
+        <v>13</v>
+      </c>
+      <c r="I417">
+        <v>15</v>
+      </c>
+      <c r="J417">
+        <v>16</v>
+      </c>
+      <c r="K417">
+        <v>17</v>
+      </c>
+      <c r="L417">
+        <v>18</v>
+      </c>
+      <c r="M417">
+        <v>19</v>
+      </c>
+      <c r="N417">
+        <v>21</v>
+      </c>
+      <c r="O417">
+        <v>22</v>
+      </c>
+      <c r="P417">
+        <v>23</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <PublishingExpirationDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <PublishingStartDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <AtualizadoPeloTimerJobEm xmlns="4455b8ba-124f-46d5-aaaa-9813efd83d1e">2025-08-17T04:03:58+00:00</AtualizadoPeloTimerJobEm>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -20752,19 +21503,21 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <PublishingExpirationDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <PublishingStartDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <AtualizadoPeloTimerJobEm xmlns="4455b8ba-124f-46d5-aaaa-9813efd83d1e">2025-08-17T04:03:58+00:00</AtualizadoPeloTimerJobEm>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{82B637BD-743B-452C-A85E-33AF8B93F052}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0328C38C-FE97-4791-8469-4B5D9CCC5D08}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="4455b8ba-124f-46d5-aaaa-9813efd83d1e"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -20790,12 +21543,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0328C38C-FE97-4791-8469-4B5D9CCC5D08}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{82B637BD-743B-452C-A85E-33AF8B93F052}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="4455b8ba-124f-46d5-aaaa-9813efd83d1e"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
📊 Update: Atualizar dados das loterias nos arquivos Excel
- Update: Lotofacil_edt2.xlsx - Novos dados e estatísticas
- Update: Lotomania_edt.xlsx - Atualizações de resultados
- Update: MegaSena_edt.xlsx - Dados mais recentes
- Update: Milionária_edt.xlsx - Informações atualizadas
- Update: Quina_edt.xlsx - Novos sorteios e análises
- Update: carrossel_Dados.csv - Dados do carrossel atualizados

Todos os arquivos Excel das loterias foram atualizados com os dados mais recentes.
</commit_message>
<xml_diff>
--- a/LoteriasExcel/Lotofacil_edt2.xlsx
+++ b/LoteriasExcel/Lotofacil_edt2.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\Dropbox\! 000 ByPass\Pessoal\99_Loterias\0 - Loterias-Inteligentes\LoteriasExcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD606A7A-1238-4159-9464-BF4FE03A2A0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79F76C1E-D133-4EBD-BD88-FD65E9E0164C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="66615" yWindow="0" windowWidth="26610" windowHeight="11850" tabRatio="876" xr2:uid="{2663372B-AA50-4721-AD6B-5F0B8186ACF5}"/>
+    <workbookView xWindow="57645" yWindow="90" windowWidth="33525" windowHeight="15630" tabRatio="876" xr2:uid="{2663372B-AA50-4721-AD6B-5F0B8186ACF5}"/>
   </bookViews>
   <sheets>
     <sheet name="LOTOFÁCIL" sheetId="3" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -455,10 +455,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69BEFC42-DD13-4DE0-B2AD-D0F44AF8189C}">
-  <dimension ref="A1:P417"/>
+  <dimension ref="A1:P422"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A385" workbookViewId="0">
-      <selection activeCell="G404" sqref="G404"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A395" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F420" sqref="F420"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -21319,22 +21320,262 @@
         <v>23</v>
       </c>
     </row>
+    <row r="418" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A418">
+        <v>3488</v>
+      </c>
+      <c r="B418">
+        <v>1</v>
+      </c>
+      <c r="C418">
+        <v>3</v>
+      </c>
+      <c r="D418">
+        <v>4</v>
+      </c>
+      <c r="E418">
+        <v>5</v>
+      </c>
+      <c r="F418">
+        <v>6</v>
+      </c>
+      <c r="G418">
+        <v>8</v>
+      </c>
+      <c r="H418">
+        <v>9</v>
+      </c>
+      <c r="I418">
+        <v>11</v>
+      </c>
+      <c r="J418">
+        <v>12</v>
+      </c>
+      <c r="K418">
+        <v>13</v>
+      </c>
+      <c r="L418">
+        <v>14</v>
+      </c>
+      <c r="M418">
+        <v>15</v>
+      </c>
+      <c r="N418">
+        <v>17</v>
+      </c>
+      <c r="O418">
+        <v>22</v>
+      </c>
+      <c r="P418">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="419" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A419">
+        <v>3489</v>
+      </c>
+      <c r="B419">
+        <v>1</v>
+      </c>
+      <c r="C419">
+        <v>2</v>
+      </c>
+      <c r="D419">
+        <v>5</v>
+      </c>
+      <c r="E419">
+        <v>8</v>
+      </c>
+      <c r="F419">
+        <v>9</v>
+      </c>
+      <c r="G419">
+        <v>11</v>
+      </c>
+      <c r="H419">
+        <v>14</v>
+      </c>
+      <c r="I419">
+        <v>16</v>
+      </c>
+      <c r="J419">
+        <v>17</v>
+      </c>
+      <c r="K419">
+        <v>20</v>
+      </c>
+      <c r="L419">
+        <v>21</v>
+      </c>
+      <c r="M419">
+        <v>22</v>
+      </c>
+      <c r="N419">
+        <v>23</v>
+      </c>
+      <c r="O419">
+        <v>24</v>
+      </c>
+      <c r="P419">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="420" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A420">
+        <v>3490</v>
+      </c>
+      <c r="B420">
+        <v>2</v>
+      </c>
+      <c r="C420">
+        <v>3</v>
+      </c>
+      <c r="D420">
+        <v>4</v>
+      </c>
+      <c r="E420">
+        <v>7</v>
+      </c>
+      <c r="F420">
+        <v>8</v>
+      </c>
+      <c r="G420">
+        <v>11</v>
+      </c>
+      <c r="H420">
+        <v>13</v>
+      </c>
+      <c r="I420">
+        <v>14</v>
+      </c>
+      <c r="J420">
+        <v>15</v>
+      </c>
+      <c r="K420">
+        <v>16</v>
+      </c>
+      <c r="L420">
+        <v>18</v>
+      </c>
+      <c r="M420">
+        <v>19</v>
+      </c>
+      <c r="N420">
+        <v>21</v>
+      </c>
+      <c r="O420">
+        <v>23</v>
+      </c>
+      <c r="P420">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="421" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A421">
+        <v>3491</v>
+      </c>
+      <c r="B421">
+        <v>1</v>
+      </c>
+      <c r="C421">
+        <v>2</v>
+      </c>
+      <c r="D421">
+        <v>4</v>
+      </c>
+      <c r="E421">
+        <v>8</v>
+      </c>
+      <c r="F421">
+        <v>9</v>
+      </c>
+      <c r="G421">
+        <v>10</v>
+      </c>
+      <c r="H421">
+        <v>12</v>
+      </c>
+      <c r="I421">
+        <v>13</v>
+      </c>
+      <c r="J421">
+        <v>15</v>
+      </c>
+      <c r="K421">
+        <v>17</v>
+      </c>
+      <c r="L421">
+        <v>21</v>
+      </c>
+      <c r="M421">
+        <v>22</v>
+      </c>
+      <c r="N421">
+        <v>23</v>
+      </c>
+      <c r="O421">
+        <v>24</v>
+      </c>
+      <c r="P421">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="422" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A422">
+        <v>3492</v>
+      </c>
+      <c r="B422">
+        <v>2</v>
+      </c>
+      <c r="C422">
+        <v>3</v>
+      </c>
+      <c r="D422">
+        <v>4</v>
+      </c>
+      <c r="E422">
+        <v>8</v>
+      </c>
+      <c r="F422">
+        <v>9</v>
+      </c>
+      <c r="G422">
+        <v>10</v>
+      </c>
+      <c r="H422">
+        <v>13</v>
+      </c>
+      <c r="I422">
+        <v>17</v>
+      </c>
+      <c r="J422">
+        <v>18</v>
+      </c>
+      <c r="K422">
+        <v>19</v>
+      </c>
+      <c r="L422">
+        <v>20</v>
+      </c>
+      <c r="M422">
+        <v>21</v>
+      </c>
+      <c r="N422">
+        <v>22</v>
+      </c>
+      <c r="O422">
+        <v>23</v>
+      </c>
+      <c r="P422">
+        <v>25</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <PublishingExpirationDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <PublishingStartDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <AtualizadoPeloTimerJobEm xmlns="4455b8ba-124f-46d5-aaaa-9813efd83d1e">2025-08-17T04:03:58+00:00</AtualizadoPeloTimerJobEm>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100C92CDE8829F3C7438DCCB0991C30EAAE" ma:contentTypeVersion="3" ma:contentTypeDescription="Crie um novo documento." ma:contentTypeScope="" ma:versionID="36cf41eecaf38ba1d849a0c8dd067090">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="3e38fcf2-aa96-4a2c-865b-c3abba01ba51" xmlns:ns3="4455b8ba-124f-46d5-aaaa-9813efd83d1e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="023f68b2d27389a617bf935a3f0e17ad" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -21502,6 +21743,16 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <PublishingExpirationDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <PublishingStartDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <AtualizadoPeloTimerJobEm xmlns="4455b8ba-124f-46d5-aaaa-9813efd83d1e">2025-08-17T04:03:58+00:00</AtualizadoPeloTimerJobEm>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -21512,17 +21763,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0328C38C-FE97-4791-8469-4B5D9CCC5D08}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="4455b8ba-124f-46d5-aaaa-9813efd83d1e"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{46C5B8C5-4575-4105-836C-9C4A6674A14B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -21542,6 +21782,17 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0328C38C-FE97-4791-8469-4B5D9CCC5D08}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="4455b8ba-124f-46d5-aaaa-9813efd83d1e"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{82B637BD-743B-452C-A85E-33AF8B93F052}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
✅ Implementação completa do sistema de termos de uso e restrições do botão CRIAR CONTA
🔧 Funcionalidades implementadas:
- Modal de termos de uso integrado ao fluxo de cadastro
- Checkbox obrigatório destacado em verde lima neon
- Retorno automático ao modal de cadastro após aceitar termos
- Botão CRIAR CONTA com restrições (vermelho desabilitado → verde habilitado)
- Comunicação via iframe entre modais
- Validação dupla de segurança
- Design responsivo e animações

🎯 Fluxo completo:
1. Usuário clica termos → abre iframe
2. Aceita termos → volta ao modal cadastro
3. Botão fica verde e funcional
4. Validação completa → modal confirmação

📁 Arquivos modificados:
- static/js/modal-login-cadastro.js
- static/css/modal-login-cadastro.css
- templates/modal_cadastro_assinatura.html
- app.py (rota /termos-uso)
</commit_message>
<xml_diff>
--- a/LoteriasExcel/Lotofacil_edt2.xlsx
+++ b/LoteriasExcel/Lotofacil_edt2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\Dropbox\! 000 ByPass\Pessoal\99_Loterias\0 - Loterias-Inteligentes\LoteriasExcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79F76C1E-D133-4EBD-BD88-FD65E9E0164C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8464ABFF-0E3C-4A62-B6DA-0A9BAD2D6628}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57645" yWindow="90" windowWidth="33525" windowHeight="15630" tabRatio="876" xr2:uid="{2663372B-AA50-4721-AD6B-5F0B8186ACF5}"/>
+    <workbookView xWindow="76530" yWindow="660" windowWidth="17970" windowHeight="15885" tabRatio="876" xr2:uid="{2663372B-AA50-4721-AD6B-5F0B8186ACF5}"/>
   </bookViews>
   <sheets>
     <sheet name="LOTOFÁCIL" sheetId="3" r:id="rId1"/>
@@ -455,11 +455,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69BEFC42-DD13-4DE0-B2AD-D0F44AF8189C}">
-  <dimension ref="A1:P422"/>
+  <dimension ref="A1:P423"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A395" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F420" sqref="F420"/>
+      <selection pane="bottomLeft" activeCell="Q423" sqref="Q423"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -21570,12 +21570,81 @@
         <v>25</v>
       </c>
     </row>
+    <row r="423" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A423">
+        <v>3493</v>
+      </c>
+      <c r="B423">
+        <v>2</v>
+      </c>
+      <c r="C423">
+        <v>3</v>
+      </c>
+      <c r="D423">
+        <v>4</v>
+      </c>
+      <c r="E423">
+        <v>5</v>
+      </c>
+      <c r="F423">
+        <v>6</v>
+      </c>
+      <c r="G423">
+        <v>10</v>
+      </c>
+      <c r="H423">
+        <v>11</v>
+      </c>
+      <c r="I423">
+        <v>13</v>
+      </c>
+      <c r="J423">
+        <v>15</v>
+      </c>
+      <c r="K423">
+        <v>16</v>
+      </c>
+      <c r="L423">
+        <v>19</v>
+      </c>
+      <c r="M423">
+        <v>20</v>
+      </c>
+      <c r="N423">
+        <v>21</v>
+      </c>
+      <c r="O423">
+        <v>23</v>
+      </c>
+      <c r="P423">
+        <v>24</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <PublishingExpirationDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <PublishingStartDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <AtualizadoPeloTimerJobEm xmlns="4455b8ba-124f-46d5-aaaa-9813efd83d1e">2025-08-17T04:03:58+00:00</AtualizadoPeloTimerJobEm>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100C92CDE8829F3C7438DCCB0991C30EAAE" ma:contentTypeVersion="3" ma:contentTypeDescription="Crie um novo documento." ma:contentTypeScope="" ma:versionID="36cf41eecaf38ba1d849a0c8dd067090">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="3e38fcf2-aa96-4a2c-865b-c3abba01ba51" xmlns:ns3="4455b8ba-124f-46d5-aaaa-9813efd83d1e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="023f68b2d27389a617bf935a3f0e17ad" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -21743,26 +21812,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <PublishingExpirationDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <PublishingStartDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <AtualizadoPeloTimerJobEm xmlns="4455b8ba-124f-46d5-aaaa-9813efd83d1e">2025-08-17T04:03:58+00:00</AtualizadoPeloTimerJobEm>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{82B637BD-743B-452C-A85E-33AF8B93F052}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0328C38C-FE97-4791-8469-4B5D9CCC5D08}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="4455b8ba-124f-46d5-aaaa-9813efd83d1e"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{46C5B8C5-4575-4105-836C-9C4A6674A14B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -21780,23 +21849,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0328C38C-FE97-4791-8469-4B5D9CCC5D08}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="4455b8ba-124f-46d5-aaaa-9813efd83d1e"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{82B637BD-743B-452C-A85E-33AF8B93F052}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
ajustando o modal dos planos das paginas...
</commit_message>
<xml_diff>
--- a/LoteriasExcel/Lotofacil_edt2.xlsx
+++ b/LoteriasExcel/Lotofacil_edt2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\Dropbox\! 000 ByPass\Pessoal\99_Loterias\0 - Loterias-Inteligentes\LoteriasExcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8464ABFF-0E3C-4A62-B6DA-0A9BAD2D6628}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC964802-2475-4A43-A9CC-A3B140130A0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="76530" yWindow="660" windowWidth="17970" windowHeight="15885" tabRatio="876" xr2:uid="{2663372B-AA50-4721-AD6B-5F0B8186ACF5}"/>
+    <workbookView xWindow="77535" yWindow="0" windowWidth="18255" windowHeight="17505" tabRatio="876" xr2:uid="{2663372B-AA50-4721-AD6B-5F0B8186ACF5}"/>
   </bookViews>
   <sheets>
     <sheet name="LOTOFÁCIL" sheetId="3" r:id="rId1"/>
@@ -455,11 +455,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69BEFC42-DD13-4DE0-B2AD-D0F44AF8189C}">
-  <dimension ref="A1:P423"/>
+  <dimension ref="A1:P455"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A395" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q423" sqref="Q423"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A418" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B435" sqref="B435:P455"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -21617,6 +21617,1606 @@
         <v>23</v>
       </c>
       <c r="P423">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="424" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A424">
+        <v>3494</v>
+      </c>
+      <c r="B424">
+        <v>1</v>
+      </c>
+      <c r="C424">
+        <v>4</v>
+      </c>
+      <c r="D424">
+        <v>9</v>
+      </c>
+      <c r="E424">
+        <v>10</v>
+      </c>
+      <c r="F424">
+        <v>11</v>
+      </c>
+      <c r="G424">
+        <v>12</v>
+      </c>
+      <c r="H424">
+        <v>14</v>
+      </c>
+      <c r="I424">
+        <v>15</v>
+      </c>
+      <c r="J424">
+        <v>16</v>
+      </c>
+      <c r="K424">
+        <v>17</v>
+      </c>
+      <c r="L424">
+        <v>19</v>
+      </c>
+      <c r="M424">
+        <v>21</v>
+      </c>
+      <c r="N424">
+        <v>22</v>
+      </c>
+      <c r="O424">
+        <v>24</v>
+      </c>
+      <c r="P424">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="425" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A425">
+        <v>3495</v>
+      </c>
+      <c r="B425">
+        <v>2</v>
+      </c>
+      <c r="C425">
+        <v>3</v>
+      </c>
+      <c r="D425">
+        <v>6</v>
+      </c>
+      <c r="E425">
+        <v>8</v>
+      </c>
+      <c r="F425">
+        <v>9</v>
+      </c>
+      <c r="G425">
+        <v>11</v>
+      </c>
+      <c r="H425">
+        <v>12</v>
+      </c>
+      <c r="I425">
+        <v>15</v>
+      </c>
+      <c r="J425">
+        <v>16</v>
+      </c>
+      <c r="K425">
+        <v>18</v>
+      </c>
+      <c r="L425">
+        <v>19</v>
+      </c>
+      <c r="M425">
+        <v>20</v>
+      </c>
+      <c r="N425">
+        <v>22</v>
+      </c>
+      <c r="O425">
+        <v>23</v>
+      </c>
+      <c r="P425">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="426" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A426">
+        <v>3496</v>
+      </c>
+      <c r="B426">
+        <v>1</v>
+      </c>
+      <c r="C426">
+        <v>4</v>
+      </c>
+      <c r="D426">
+        <v>5</v>
+      </c>
+      <c r="E426">
+        <v>8</v>
+      </c>
+      <c r="F426">
+        <v>9</v>
+      </c>
+      <c r="G426">
+        <v>11</v>
+      </c>
+      <c r="H426">
+        <v>13</v>
+      </c>
+      <c r="I426">
+        <v>14</v>
+      </c>
+      <c r="J426">
+        <v>15</v>
+      </c>
+      <c r="K426">
+        <v>16</v>
+      </c>
+      <c r="L426">
+        <v>17</v>
+      </c>
+      <c r="M426">
+        <v>18</v>
+      </c>
+      <c r="N426">
+        <v>20</v>
+      </c>
+      <c r="O426">
+        <v>23</v>
+      </c>
+      <c r="P426">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="427" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A427">
+        <v>3497</v>
+      </c>
+      <c r="B427">
+        <v>1</v>
+      </c>
+      <c r="C427">
+        <v>2</v>
+      </c>
+      <c r="D427">
+        <v>3</v>
+      </c>
+      <c r="E427">
+        <v>4</v>
+      </c>
+      <c r="F427">
+        <v>6</v>
+      </c>
+      <c r="G427">
+        <v>10</v>
+      </c>
+      <c r="H427">
+        <v>11</v>
+      </c>
+      <c r="I427">
+        <v>12</v>
+      </c>
+      <c r="J427">
+        <v>13</v>
+      </c>
+      <c r="K427">
+        <v>14</v>
+      </c>
+      <c r="L427">
+        <v>15</v>
+      </c>
+      <c r="M427">
+        <v>18</v>
+      </c>
+      <c r="N427">
+        <v>19</v>
+      </c>
+      <c r="O427">
+        <v>21</v>
+      </c>
+      <c r="P427">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="428" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A428">
+        <v>3498</v>
+      </c>
+      <c r="B428">
+        <v>1</v>
+      </c>
+      <c r="C428">
+        <v>2</v>
+      </c>
+      <c r="D428">
+        <v>3</v>
+      </c>
+      <c r="E428">
+        <v>4</v>
+      </c>
+      <c r="F428">
+        <v>5</v>
+      </c>
+      <c r="G428">
+        <v>7</v>
+      </c>
+      <c r="H428">
+        <v>8</v>
+      </c>
+      <c r="I428">
+        <v>9</v>
+      </c>
+      <c r="J428">
+        <v>15</v>
+      </c>
+      <c r="K428">
+        <v>16</v>
+      </c>
+      <c r="L428">
+        <v>17</v>
+      </c>
+      <c r="M428">
+        <v>19</v>
+      </c>
+      <c r="N428">
+        <v>21</v>
+      </c>
+      <c r="O428">
+        <v>22</v>
+      </c>
+      <c r="P428">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="429" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A429">
+        <v>3499</v>
+      </c>
+      <c r="B429">
+        <v>1</v>
+      </c>
+      <c r="C429">
+        <v>5</v>
+      </c>
+      <c r="D429">
+        <v>7</v>
+      </c>
+      <c r="E429">
+        <v>9</v>
+      </c>
+      <c r="F429">
+        <v>10</v>
+      </c>
+      <c r="G429">
+        <v>11</v>
+      </c>
+      <c r="H429">
+        <v>12</v>
+      </c>
+      <c r="I429">
+        <v>13</v>
+      </c>
+      <c r="J429">
+        <v>14</v>
+      </c>
+      <c r="K429">
+        <v>17</v>
+      </c>
+      <c r="L429">
+        <v>18</v>
+      </c>
+      <c r="M429">
+        <v>19</v>
+      </c>
+      <c r="N429">
+        <v>23</v>
+      </c>
+      <c r="O429">
+        <v>24</v>
+      </c>
+      <c r="P429">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="430" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A430">
+        <v>3500</v>
+      </c>
+      <c r="B430">
+        <v>1</v>
+      </c>
+      <c r="C430">
+        <v>2</v>
+      </c>
+      <c r="D430">
+        <v>4</v>
+      </c>
+      <c r="E430">
+        <v>5</v>
+      </c>
+      <c r="F430">
+        <v>6</v>
+      </c>
+      <c r="G430">
+        <v>7</v>
+      </c>
+      <c r="H430">
+        <v>9</v>
+      </c>
+      <c r="I430">
+        <v>10</v>
+      </c>
+      <c r="J430">
+        <v>11</v>
+      </c>
+      <c r="K430">
+        <v>12</v>
+      </c>
+      <c r="L430">
+        <v>14</v>
+      </c>
+      <c r="M430">
+        <v>16</v>
+      </c>
+      <c r="N430">
+        <v>18</v>
+      </c>
+      <c r="O430">
+        <v>19</v>
+      </c>
+      <c r="P430">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="431" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A431">
+        <v>3501</v>
+      </c>
+      <c r="B431">
+        <v>1</v>
+      </c>
+      <c r="C431">
+        <v>3</v>
+      </c>
+      <c r="D431">
+        <v>7</v>
+      </c>
+      <c r="E431">
+        <v>9</v>
+      </c>
+      <c r="F431">
+        <v>11</v>
+      </c>
+      <c r="G431">
+        <v>12</v>
+      </c>
+      <c r="H431">
+        <v>13</v>
+      </c>
+      <c r="I431">
+        <v>15</v>
+      </c>
+      <c r="J431">
+        <v>16</v>
+      </c>
+      <c r="K431">
+        <v>18</v>
+      </c>
+      <c r="L431">
+        <v>19</v>
+      </c>
+      <c r="M431">
+        <v>20</v>
+      </c>
+      <c r="N431">
+        <v>21</v>
+      </c>
+      <c r="O431">
+        <v>22</v>
+      </c>
+      <c r="P431">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="432" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A432">
+        <v>3502</v>
+      </c>
+      <c r="B432">
+        <v>4</v>
+      </c>
+      <c r="C432">
+        <v>5</v>
+      </c>
+      <c r="D432">
+        <v>6</v>
+      </c>
+      <c r="E432">
+        <v>7</v>
+      </c>
+      <c r="F432">
+        <v>8</v>
+      </c>
+      <c r="G432">
+        <v>9</v>
+      </c>
+      <c r="H432">
+        <v>14</v>
+      </c>
+      <c r="I432">
+        <v>15</v>
+      </c>
+      <c r="J432">
+        <v>16</v>
+      </c>
+      <c r="K432">
+        <v>17</v>
+      </c>
+      <c r="L432">
+        <v>18</v>
+      </c>
+      <c r="M432">
+        <v>19</v>
+      </c>
+      <c r="N432">
+        <v>20</v>
+      </c>
+      <c r="O432">
+        <v>21</v>
+      </c>
+      <c r="P432">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="433" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A433">
+        <v>3503</v>
+      </c>
+      <c r="B433">
+        <v>1</v>
+      </c>
+      <c r="C433">
+        <v>4</v>
+      </c>
+      <c r="D433">
+        <v>6</v>
+      </c>
+      <c r="E433">
+        <v>7</v>
+      </c>
+      <c r="F433">
+        <v>8</v>
+      </c>
+      <c r="G433">
+        <v>10</v>
+      </c>
+      <c r="H433">
+        <v>11</v>
+      </c>
+      <c r="I433">
+        <v>12</v>
+      </c>
+      <c r="J433">
+        <v>14</v>
+      </c>
+      <c r="K433">
+        <v>15</v>
+      </c>
+      <c r="L433">
+        <v>16</v>
+      </c>
+      <c r="M433">
+        <v>18</v>
+      </c>
+      <c r="N433">
+        <v>21</v>
+      </c>
+      <c r="O433">
+        <v>24</v>
+      </c>
+      <c r="P433">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="434" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A434">
+        <v>3504</v>
+      </c>
+      <c r="B434">
+        <v>1</v>
+      </c>
+      <c r="C434">
+        <v>2</v>
+      </c>
+      <c r="D434">
+        <v>4</v>
+      </c>
+      <c r="E434">
+        <v>6</v>
+      </c>
+      <c r="F434">
+        <v>7</v>
+      </c>
+      <c r="G434">
+        <v>9</v>
+      </c>
+      <c r="H434">
+        <v>10</v>
+      </c>
+      <c r="I434">
+        <v>12</v>
+      </c>
+      <c r="J434">
+        <v>15</v>
+      </c>
+      <c r="K434">
+        <v>16</v>
+      </c>
+      <c r="L434">
+        <v>17</v>
+      </c>
+      <c r="M434">
+        <v>21</v>
+      </c>
+      <c r="N434">
+        <v>22</v>
+      </c>
+      <c r="O434">
+        <v>23</v>
+      </c>
+      <c r="P434">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="435" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A435">
+        <v>3505</v>
+      </c>
+      <c r="B435">
+        <v>1</v>
+      </c>
+      <c r="C435">
+        <v>2</v>
+      </c>
+      <c r="D435">
+        <v>3</v>
+      </c>
+      <c r="E435">
+        <v>4</v>
+      </c>
+      <c r="F435">
+        <v>6</v>
+      </c>
+      <c r="G435">
+        <v>7</v>
+      </c>
+      <c r="H435">
+        <v>8</v>
+      </c>
+      <c r="I435">
+        <v>9</v>
+      </c>
+      <c r="J435">
+        <v>11</v>
+      </c>
+      <c r="K435">
+        <v>14</v>
+      </c>
+      <c r="L435">
+        <v>16</v>
+      </c>
+      <c r="M435">
+        <v>20</v>
+      </c>
+      <c r="N435">
+        <v>21</v>
+      </c>
+      <c r="O435">
+        <v>23</v>
+      </c>
+      <c r="P435">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="436" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A436">
+        <v>3506</v>
+      </c>
+      <c r="B436">
+        <v>3</v>
+      </c>
+      <c r="C436">
+        <v>4</v>
+      </c>
+      <c r="D436">
+        <v>5</v>
+      </c>
+      <c r="E436">
+        <v>6</v>
+      </c>
+      <c r="F436">
+        <v>8</v>
+      </c>
+      <c r="G436">
+        <v>11</v>
+      </c>
+      <c r="H436">
+        <v>12</v>
+      </c>
+      <c r="I436">
+        <v>13</v>
+      </c>
+      <c r="J436">
+        <v>16</v>
+      </c>
+      <c r="K436">
+        <v>17</v>
+      </c>
+      <c r="L436">
+        <v>18</v>
+      </c>
+      <c r="M436">
+        <v>22</v>
+      </c>
+      <c r="N436">
+        <v>23</v>
+      </c>
+      <c r="O436">
+        <v>24</v>
+      </c>
+      <c r="P436">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="437" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A437">
+        <v>3507</v>
+      </c>
+      <c r="B437">
+        <v>2</v>
+      </c>
+      <c r="C437">
+        <v>3</v>
+      </c>
+      <c r="D437">
+        <v>4</v>
+      </c>
+      <c r="E437">
+        <v>7</v>
+      </c>
+      <c r="F437">
+        <v>9</v>
+      </c>
+      <c r="G437">
+        <v>10</v>
+      </c>
+      <c r="H437">
+        <v>11</v>
+      </c>
+      <c r="I437">
+        <v>12</v>
+      </c>
+      <c r="J437">
+        <v>17</v>
+      </c>
+      <c r="K437">
+        <v>18</v>
+      </c>
+      <c r="L437">
+        <v>19</v>
+      </c>
+      <c r="M437">
+        <v>21</v>
+      </c>
+      <c r="N437">
+        <v>22</v>
+      </c>
+      <c r="O437">
+        <v>24</v>
+      </c>
+      <c r="P437">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="438" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A438">
+        <v>3508</v>
+      </c>
+      <c r="B438">
+        <v>1</v>
+      </c>
+      <c r="C438">
+        <v>3</v>
+      </c>
+      <c r="D438">
+        <v>4</v>
+      </c>
+      <c r="E438">
+        <v>5</v>
+      </c>
+      <c r="F438">
+        <v>6</v>
+      </c>
+      <c r="G438">
+        <v>8</v>
+      </c>
+      <c r="H438">
+        <v>11</v>
+      </c>
+      <c r="I438">
+        <v>13</v>
+      </c>
+      <c r="J438">
+        <v>14</v>
+      </c>
+      <c r="K438">
+        <v>16</v>
+      </c>
+      <c r="L438">
+        <v>17</v>
+      </c>
+      <c r="M438">
+        <v>20</v>
+      </c>
+      <c r="N438">
+        <v>21</v>
+      </c>
+      <c r="O438">
+        <v>22</v>
+      </c>
+      <c r="P438">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="439" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A439">
+        <v>3509</v>
+      </c>
+      <c r="B439">
+        <v>1</v>
+      </c>
+      <c r="C439">
+        <v>3</v>
+      </c>
+      <c r="D439">
+        <v>4</v>
+      </c>
+      <c r="E439">
+        <v>7</v>
+      </c>
+      <c r="F439">
+        <v>9</v>
+      </c>
+      <c r="G439">
+        <v>10</v>
+      </c>
+      <c r="H439">
+        <v>12</v>
+      </c>
+      <c r="I439">
+        <v>14</v>
+      </c>
+      <c r="J439">
+        <v>15</v>
+      </c>
+      <c r="K439">
+        <v>16</v>
+      </c>
+      <c r="L439">
+        <v>19</v>
+      </c>
+      <c r="M439">
+        <v>21</v>
+      </c>
+      <c r="N439">
+        <v>22</v>
+      </c>
+      <c r="O439">
+        <v>24</v>
+      </c>
+      <c r="P439">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="440" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A440">
+        <v>3510</v>
+      </c>
+      <c r="B440">
+        <v>1</v>
+      </c>
+      <c r="C440">
+        <v>2</v>
+      </c>
+      <c r="D440">
+        <v>3</v>
+      </c>
+      <c r="E440">
+        <v>4</v>
+      </c>
+      <c r="F440">
+        <v>5</v>
+      </c>
+      <c r="G440">
+        <v>6</v>
+      </c>
+      <c r="H440">
+        <v>7</v>
+      </c>
+      <c r="I440">
+        <v>8</v>
+      </c>
+      <c r="J440">
+        <v>13</v>
+      </c>
+      <c r="K440">
+        <v>14</v>
+      </c>
+      <c r="L440">
+        <v>15</v>
+      </c>
+      <c r="M440">
+        <v>17</v>
+      </c>
+      <c r="N440">
+        <v>21</v>
+      </c>
+      <c r="O440">
+        <v>22</v>
+      </c>
+      <c r="P440">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="441" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A441">
+        <v>3511</v>
+      </c>
+      <c r="B441">
+        <v>2</v>
+      </c>
+      <c r="C441">
+        <v>3</v>
+      </c>
+      <c r="D441">
+        <v>5</v>
+      </c>
+      <c r="E441">
+        <v>6</v>
+      </c>
+      <c r="F441">
+        <v>7</v>
+      </c>
+      <c r="G441">
+        <v>8</v>
+      </c>
+      <c r="H441">
+        <v>9</v>
+      </c>
+      <c r="I441">
+        <v>12</v>
+      </c>
+      <c r="J441">
+        <v>13</v>
+      </c>
+      <c r="K441">
+        <v>14</v>
+      </c>
+      <c r="L441">
+        <v>15</v>
+      </c>
+      <c r="M441">
+        <v>19</v>
+      </c>
+      <c r="N441">
+        <v>20</v>
+      </c>
+      <c r="O441">
+        <v>23</v>
+      </c>
+      <c r="P441">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="442" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A442">
+        <v>3512</v>
+      </c>
+      <c r="B442">
+        <v>1</v>
+      </c>
+      <c r="C442">
+        <v>2</v>
+      </c>
+      <c r="D442">
+        <v>3</v>
+      </c>
+      <c r="E442">
+        <v>4</v>
+      </c>
+      <c r="F442">
+        <v>5</v>
+      </c>
+      <c r="G442">
+        <v>6</v>
+      </c>
+      <c r="H442">
+        <v>9</v>
+      </c>
+      <c r="I442">
+        <v>12</v>
+      </c>
+      <c r="J442">
+        <v>13</v>
+      </c>
+      <c r="K442">
+        <v>14</v>
+      </c>
+      <c r="L442">
+        <v>15</v>
+      </c>
+      <c r="M442">
+        <v>17</v>
+      </c>
+      <c r="N442">
+        <v>19</v>
+      </c>
+      <c r="O442">
+        <v>20</v>
+      </c>
+      <c r="P442">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="443" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A443">
+        <v>3513</v>
+      </c>
+      <c r="B443">
+        <v>3</v>
+      </c>
+      <c r="C443">
+        <v>4</v>
+      </c>
+      <c r="D443">
+        <v>5</v>
+      </c>
+      <c r="E443">
+        <v>6</v>
+      </c>
+      <c r="F443">
+        <v>7</v>
+      </c>
+      <c r="G443">
+        <v>11</v>
+      </c>
+      <c r="H443">
+        <v>13</v>
+      </c>
+      <c r="I443">
+        <v>14</v>
+      </c>
+      <c r="J443">
+        <v>15</v>
+      </c>
+      <c r="K443">
+        <v>16</v>
+      </c>
+      <c r="L443">
+        <v>18</v>
+      </c>
+      <c r="M443">
+        <v>20</v>
+      </c>
+      <c r="N443">
+        <v>22</v>
+      </c>
+      <c r="O443">
+        <v>23</v>
+      </c>
+      <c r="P443">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="444" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A444">
+        <v>3514</v>
+      </c>
+      <c r="B444">
+        <v>1</v>
+      </c>
+      <c r="C444">
+        <v>3</v>
+      </c>
+      <c r="D444">
+        <v>4</v>
+      </c>
+      <c r="E444">
+        <v>5</v>
+      </c>
+      <c r="F444">
+        <v>6</v>
+      </c>
+      <c r="G444">
+        <v>8</v>
+      </c>
+      <c r="H444">
+        <v>10</v>
+      </c>
+      <c r="I444">
+        <v>12</v>
+      </c>
+      <c r="J444">
+        <v>13</v>
+      </c>
+      <c r="K444">
+        <v>16</v>
+      </c>
+      <c r="L444">
+        <v>17</v>
+      </c>
+      <c r="M444">
+        <v>20</v>
+      </c>
+      <c r="N444">
+        <v>21</v>
+      </c>
+      <c r="O444">
+        <v>23</v>
+      </c>
+      <c r="P444">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="445" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A445">
+        <v>3515</v>
+      </c>
+      <c r="B445">
+        <v>1</v>
+      </c>
+      <c r="C445">
+        <v>2</v>
+      </c>
+      <c r="D445">
+        <v>3</v>
+      </c>
+      <c r="E445">
+        <v>4</v>
+      </c>
+      <c r="F445">
+        <v>5</v>
+      </c>
+      <c r="G445">
+        <v>6</v>
+      </c>
+      <c r="H445">
+        <v>7</v>
+      </c>
+      <c r="I445">
+        <v>9</v>
+      </c>
+      <c r="J445">
+        <v>14</v>
+      </c>
+      <c r="K445">
+        <v>15</v>
+      </c>
+      <c r="L445">
+        <v>16</v>
+      </c>
+      <c r="M445">
+        <v>17</v>
+      </c>
+      <c r="N445">
+        <v>21</v>
+      </c>
+      <c r="O445">
+        <v>23</v>
+      </c>
+      <c r="P445">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="446" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A446">
+        <v>3516</v>
+      </c>
+      <c r="B446">
+        <v>2</v>
+      </c>
+      <c r="C446">
+        <v>3</v>
+      </c>
+      <c r="D446">
+        <v>6</v>
+      </c>
+      <c r="E446">
+        <v>11</v>
+      </c>
+      <c r="F446">
+        <v>12</v>
+      </c>
+      <c r="G446">
+        <v>13</v>
+      </c>
+      <c r="H446">
+        <v>14</v>
+      </c>
+      <c r="I446">
+        <v>15</v>
+      </c>
+      <c r="J446">
+        <v>17</v>
+      </c>
+      <c r="K446">
+        <v>18</v>
+      </c>
+      <c r="L446">
+        <v>19</v>
+      </c>
+      <c r="M446">
+        <v>20</v>
+      </c>
+      <c r="N446">
+        <v>21</v>
+      </c>
+      <c r="O446">
+        <v>23</v>
+      </c>
+      <c r="P446">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="447" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A447">
+        <v>3517</v>
+      </c>
+      <c r="B447">
+        <v>1</v>
+      </c>
+      <c r="C447">
+        <v>2</v>
+      </c>
+      <c r="D447">
+        <v>3</v>
+      </c>
+      <c r="E447">
+        <v>7</v>
+      </c>
+      <c r="F447">
+        <v>8</v>
+      </c>
+      <c r="G447">
+        <v>11</v>
+      </c>
+      <c r="H447">
+        <v>12</v>
+      </c>
+      <c r="I447">
+        <v>14</v>
+      </c>
+      <c r="J447">
+        <v>17</v>
+      </c>
+      <c r="K447">
+        <v>18</v>
+      </c>
+      <c r="L447">
+        <v>19</v>
+      </c>
+      <c r="M447">
+        <v>20</v>
+      </c>
+      <c r="N447">
+        <v>21</v>
+      </c>
+      <c r="O447">
+        <v>22</v>
+      </c>
+      <c r="P447">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="448" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A448">
+        <v>3518</v>
+      </c>
+      <c r="B448">
+        <v>2</v>
+      </c>
+      <c r="C448">
+        <v>5</v>
+      </c>
+      <c r="D448">
+        <v>6</v>
+      </c>
+      <c r="E448">
+        <v>7</v>
+      </c>
+      <c r="F448">
+        <v>11</v>
+      </c>
+      <c r="G448">
+        <v>12</v>
+      </c>
+      <c r="H448">
+        <v>13</v>
+      </c>
+      <c r="I448">
+        <v>14</v>
+      </c>
+      <c r="J448">
+        <v>16</v>
+      </c>
+      <c r="K448">
+        <v>17</v>
+      </c>
+      <c r="L448">
+        <v>19</v>
+      </c>
+      <c r="M448">
+        <v>21</v>
+      </c>
+      <c r="N448">
+        <v>22</v>
+      </c>
+      <c r="O448">
+        <v>24</v>
+      </c>
+      <c r="P448">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="449" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A449">
+        <v>3519</v>
+      </c>
+      <c r="B449">
+        <v>4</v>
+      </c>
+      <c r="C449">
+        <v>5</v>
+      </c>
+      <c r="D449">
+        <v>6</v>
+      </c>
+      <c r="E449">
+        <v>7</v>
+      </c>
+      <c r="F449">
+        <v>8</v>
+      </c>
+      <c r="G449">
+        <v>13</v>
+      </c>
+      <c r="H449">
+        <v>14</v>
+      </c>
+      <c r="I449">
+        <v>16</v>
+      </c>
+      <c r="J449">
+        <v>17</v>
+      </c>
+      <c r="K449">
+        <v>18</v>
+      </c>
+      <c r="L449">
+        <v>20</v>
+      </c>
+      <c r="M449">
+        <v>21</v>
+      </c>
+      <c r="N449">
+        <v>22</v>
+      </c>
+      <c r="O449">
+        <v>23</v>
+      </c>
+      <c r="P449">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="450" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A450">
+        <v>3520</v>
+      </c>
+      <c r="B450">
+        <v>1</v>
+      </c>
+      <c r="C450">
+        <v>3</v>
+      </c>
+      <c r="D450">
+        <v>7</v>
+      </c>
+      <c r="E450">
+        <v>8</v>
+      </c>
+      <c r="F450">
+        <v>10</v>
+      </c>
+      <c r="G450">
+        <v>12</v>
+      </c>
+      <c r="H450">
+        <v>13</v>
+      </c>
+      <c r="I450">
+        <v>15</v>
+      </c>
+      <c r="J450">
+        <v>16</v>
+      </c>
+      <c r="K450">
+        <v>18</v>
+      </c>
+      <c r="L450">
+        <v>19</v>
+      </c>
+      <c r="M450">
+        <v>20</v>
+      </c>
+      <c r="N450">
+        <v>21</v>
+      </c>
+      <c r="O450">
+        <v>22</v>
+      </c>
+      <c r="P450">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="451" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A451">
+        <v>3521</v>
+      </c>
+      <c r="B451">
+        <v>6</v>
+      </c>
+      <c r="C451">
+        <v>7</v>
+      </c>
+      <c r="D451">
+        <v>8</v>
+      </c>
+      <c r="E451">
+        <v>9</v>
+      </c>
+      <c r="F451">
+        <v>10</v>
+      </c>
+      <c r="G451">
+        <v>11</v>
+      </c>
+      <c r="H451">
+        <v>12</v>
+      </c>
+      <c r="I451">
+        <v>13</v>
+      </c>
+      <c r="J451">
+        <v>14</v>
+      </c>
+      <c r="K451">
+        <v>15</v>
+      </c>
+      <c r="L451">
+        <v>19</v>
+      </c>
+      <c r="M451">
+        <v>20</v>
+      </c>
+      <c r="N451">
+        <v>21</v>
+      </c>
+      <c r="O451">
+        <v>22</v>
+      </c>
+      <c r="P451">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="452" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A452">
+        <v>3522</v>
+      </c>
+      <c r="B452">
+        <v>1</v>
+      </c>
+      <c r="C452">
+        <v>2</v>
+      </c>
+      <c r="D452">
+        <v>4</v>
+      </c>
+      <c r="E452">
+        <v>5</v>
+      </c>
+      <c r="F452">
+        <v>7</v>
+      </c>
+      <c r="G452">
+        <v>8</v>
+      </c>
+      <c r="H452">
+        <v>10</v>
+      </c>
+      <c r="I452">
+        <v>11</v>
+      </c>
+      <c r="J452">
+        <v>12</v>
+      </c>
+      <c r="K452">
+        <v>14</v>
+      </c>
+      <c r="L452">
+        <v>15</v>
+      </c>
+      <c r="M452">
+        <v>17</v>
+      </c>
+      <c r="N452">
+        <v>20</v>
+      </c>
+      <c r="O452">
+        <v>22</v>
+      </c>
+      <c r="P452">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="453" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A453">
+        <v>3523</v>
+      </c>
+      <c r="B453">
+        <v>5</v>
+      </c>
+      <c r="C453">
+        <v>6</v>
+      </c>
+      <c r="D453">
+        <v>8</v>
+      </c>
+      <c r="E453">
+        <v>9</v>
+      </c>
+      <c r="F453">
+        <v>10</v>
+      </c>
+      <c r="G453">
+        <v>11</v>
+      </c>
+      <c r="H453">
+        <v>12</v>
+      </c>
+      <c r="I453">
+        <v>14</v>
+      </c>
+      <c r="J453">
+        <v>15</v>
+      </c>
+      <c r="K453">
+        <v>16</v>
+      </c>
+      <c r="L453">
+        <v>17</v>
+      </c>
+      <c r="M453">
+        <v>19</v>
+      </c>
+      <c r="N453">
+        <v>23</v>
+      </c>
+      <c r="O453">
+        <v>24</v>
+      </c>
+      <c r="P453">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="454" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A454">
+        <v>3524</v>
+      </c>
+      <c r="B454">
+        <v>2</v>
+      </c>
+      <c r="C454">
+        <v>3</v>
+      </c>
+      <c r="D454">
+        <v>4</v>
+      </c>
+      <c r="E454">
+        <v>5</v>
+      </c>
+      <c r="F454">
+        <v>7</v>
+      </c>
+      <c r="G454">
+        <v>9</v>
+      </c>
+      <c r="H454">
+        <v>12</v>
+      </c>
+      <c r="I454">
+        <v>13</v>
+      </c>
+      <c r="J454">
+        <v>14</v>
+      </c>
+      <c r="K454">
+        <v>15</v>
+      </c>
+      <c r="L454">
+        <v>16</v>
+      </c>
+      <c r="M454">
+        <v>17</v>
+      </c>
+      <c r="N454">
+        <v>18</v>
+      </c>
+      <c r="O454">
+        <v>22</v>
+      </c>
+      <c r="P454">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="455" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A455">
+        <v>3525</v>
+      </c>
+      <c r="B455">
+        <v>1</v>
+      </c>
+      <c r="C455">
+        <v>2</v>
+      </c>
+      <c r="D455">
+        <v>3</v>
+      </c>
+      <c r="E455">
+        <v>7</v>
+      </c>
+      <c r="F455">
+        <v>10</v>
+      </c>
+      <c r="G455">
+        <v>11</v>
+      </c>
+      <c r="H455">
+        <v>14</v>
+      </c>
+      <c r="I455">
+        <v>15</v>
+      </c>
+      <c r="J455">
+        <v>16</v>
+      </c>
+      <c r="K455">
+        <v>17</v>
+      </c>
+      <c r="L455">
+        <v>18</v>
+      </c>
+      <c r="M455">
+        <v>20</v>
+      </c>
+      <c r="N455">
+        <v>21</v>
+      </c>
+      <c r="O455">
+        <v>23</v>
+      </c>
+      <c r="P455">
         <v>24</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fix: Corrige limpeza de trevos no botao Limpar Tudo - Remove residuo de cor roxa ao resetar estilos inline
</commit_message>
<xml_diff>
--- a/LoteriasExcel/Lotofacil_edt2.xlsx
+++ b/LoteriasExcel/Lotofacil_edt2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\Dropbox\! 000 ByPass\Pessoal\99_Loterias\0 - Loterias-Inteligentes\LoteriasExcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC964802-2475-4A43-A9CC-A3B140130A0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C46F418F-E353-49DA-B6E8-9628CC40E5A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="77535" yWindow="0" windowWidth="18255" windowHeight="17505" tabRatio="876" xr2:uid="{2663372B-AA50-4721-AD6B-5F0B8186ACF5}"/>
+    <workbookView xWindow="61215" yWindow="3540" windowWidth="23685" windowHeight="13800" tabRatio="876" xr2:uid="{2663372B-AA50-4721-AD6B-5F0B8186ACF5}"/>
   </bookViews>
   <sheets>
     <sheet name="LOTOFÁCIL" sheetId="3" r:id="rId1"/>
@@ -130,11 +130,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -455,11 +457,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69BEFC42-DD13-4DE0-B2AD-D0F44AF8189C}">
-  <dimension ref="A1:P455"/>
+  <dimension ref="A1:P463"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A418" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B435" sqref="B435:P455"/>
+      <pane ySplit="1" topLeftCell="A445" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B456" sqref="B456:P463"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -23220,21 +23222,412 @@
         <v>24</v>
       </c>
     </row>
+    <row r="456" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A456" s="2">
+        <v>3526</v>
+      </c>
+      <c r="B456" s="3">
+        <v>1</v>
+      </c>
+      <c r="C456" s="3">
+        <v>3</v>
+      </c>
+      <c r="D456" s="3">
+        <v>7</v>
+      </c>
+      <c r="E456" s="3">
+        <v>8</v>
+      </c>
+      <c r="F456" s="3">
+        <v>10</v>
+      </c>
+      <c r="G456" s="3">
+        <v>12</v>
+      </c>
+      <c r="H456" s="3">
+        <v>14</v>
+      </c>
+      <c r="I456" s="3">
+        <v>15</v>
+      </c>
+      <c r="J456" s="3">
+        <v>17</v>
+      </c>
+      <c r="K456" s="3">
+        <v>18</v>
+      </c>
+      <c r="L456" s="3">
+        <v>19</v>
+      </c>
+      <c r="M456" s="3">
+        <v>20</v>
+      </c>
+      <c r="N456" s="3">
+        <v>21</v>
+      </c>
+      <c r="O456" s="3">
+        <v>22</v>
+      </c>
+      <c r="P456" s="3">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="457" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A457" s="2">
+        <v>3527</v>
+      </c>
+      <c r="B457" s="3">
+        <v>2</v>
+      </c>
+      <c r="C457" s="3">
+        <v>3</v>
+      </c>
+      <c r="D457" s="3">
+        <v>4</v>
+      </c>
+      <c r="E457" s="3">
+        <v>6</v>
+      </c>
+      <c r="F457" s="3">
+        <v>7</v>
+      </c>
+      <c r="G457" s="3">
+        <v>9</v>
+      </c>
+      <c r="H457" s="3">
+        <v>13</v>
+      </c>
+      <c r="I457" s="3">
+        <v>14</v>
+      </c>
+      <c r="J457" s="3">
+        <v>15</v>
+      </c>
+      <c r="K457" s="3">
+        <v>16</v>
+      </c>
+      <c r="L457" s="3">
+        <v>17</v>
+      </c>
+      <c r="M457" s="3">
+        <v>19</v>
+      </c>
+      <c r="N457" s="3">
+        <v>20</v>
+      </c>
+      <c r="O457" s="3">
+        <v>23</v>
+      </c>
+      <c r="P457" s="3">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="458" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A458" s="2">
+        <v>3528</v>
+      </c>
+      <c r="B458" s="3">
+        <v>1</v>
+      </c>
+      <c r="C458" s="3">
+        <v>3</v>
+      </c>
+      <c r="D458" s="3">
+        <v>5</v>
+      </c>
+      <c r="E458" s="3">
+        <v>6</v>
+      </c>
+      <c r="F458" s="3">
+        <v>7</v>
+      </c>
+      <c r="G458" s="3">
+        <v>9</v>
+      </c>
+      <c r="H458" s="3">
+        <v>10</v>
+      </c>
+      <c r="I458" s="3">
+        <v>16</v>
+      </c>
+      <c r="J458" s="3">
+        <v>18</v>
+      </c>
+      <c r="K458" s="3">
+        <v>19</v>
+      </c>
+      <c r="L458" s="3">
+        <v>20</v>
+      </c>
+      <c r="M458" s="3">
+        <v>22</v>
+      </c>
+      <c r="N458" s="3">
+        <v>23</v>
+      </c>
+      <c r="O458" s="3">
+        <v>24</v>
+      </c>
+      <c r="P458" s="3">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="459" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A459" s="2">
+        <v>3529</v>
+      </c>
+      <c r="B459" s="3">
+        <v>1</v>
+      </c>
+      <c r="C459" s="3">
+        <v>7</v>
+      </c>
+      <c r="D459" s="3">
+        <v>8</v>
+      </c>
+      <c r="E459" s="3">
+        <v>10</v>
+      </c>
+      <c r="F459" s="3">
+        <v>11</v>
+      </c>
+      <c r="G459" s="3">
+        <v>12</v>
+      </c>
+      <c r="H459" s="3">
+        <v>14</v>
+      </c>
+      <c r="I459" s="3">
+        <v>15</v>
+      </c>
+      <c r="J459" s="3">
+        <v>16</v>
+      </c>
+      <c r="K459" s="3">
+        <v>17</v>
+      </c>
+      <c r="L459" s="3">
+        <v>18</v>
+      </c>
+      <c r="M459" s="3">
+        <v>19</v>
+      </c>
+      <c r="N459" s="3">
+        <v>20</v>
+      </c>
+      <c r="O459" s="3">
+        <v>22</v>
+      </c>
+      <c r="P459" s="3">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="460" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A460" s="2">
+        <v>3530</v>
+      </c>
+      <c r="B460" s="3">
+        <v>1</v>
+      </c>
+      <c r="C460" s="3">
+        <v>2</v>
+      </c>
+      <c r="D460" s="3">
+        <v>3</v>
+      </c>
+      <c r="E460" s="3">
+        <v>5</v>
+      </c>
+      <c r="F460" s="3">
+        <v>7</v>
+      </c>
+      <c r="G460" s="3">
+        <v>11</v>
+      </c>
+      <c r="H460" s="3">
+        <v>12</v>
+      </c>
+      <c r="I460" s="3">
+        <v>13</v>
+      </c>
+      <c r="J460" s="3">
+        <v>15</v>
+      </c>
+      <c r="K460" s="3">
+        <v>16</v>
+      </c>
+      <c r="L460" s="3">
+        <v>20</v>
+      </c>
+      <c r="M460" s="3">
+        <v>22</v>
+      </c>
+      <c r="N460" s="3">
+        <v>23</v>
+      </c>
+      <c r="O460" s="3">
+        <v>24</v>
+      </c>
+      <c r="P460" s="3">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="461" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A461" s="2">
+        <v>3531</v>
+      </c>
+      <c r="B461" s="3">
+        <v>1</v>
+      </c>
+      <c r="C461" s="3">
+        <v>3</v>
+      </c>
+      <c r="D461" s="3">
+        <v>4</v>
+      </c>
+      <c r="E461" s="3">
+        <v>5</v>
+      </c>
+      <c r="F461" s="3">
+        <v>7</v>
+      </c>
+      <c r="G461" s="3">
+        <v>8</v>
+      </c>
+      <c r="H461" s="3">
+        <v>10</v>
+      </c>
+      <c r="I461" s="3">
+        <v>11</v>
+      </c>
+      <c r="J461" s="3">
+        <v>12</v>
+      </c>
+      <c r="K461" s="3">
+        <v>14</v>
+      </c>
+      <c r="L461" s="3">
+        <v>15</v>
+      </c>
+      <c r="M461" s="3">
+        <v>16</v>
+      </c>
+      <c r="N461" s="3">
+        <v>18</v>
+      </c>
+      <c r="O461" s="3">
+        <v>19</v>
+      </c>
+      <c r="P461" s="3">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="462" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A462" s="2">
+        <v>3532</v>
+      </c>
+      <c r="B462" s="3">
+        <v>2</v>
+      </c>
+      <c r="C462" s="3">
+        <v>3</v>
+      </c>
+      <c r="D462" s="3">
+        <v>4</v>
+      </c>
+      <c r="E462" s="3">
+        <v>5</v>
+      </c>
+      <c r="F462" s="3">
+        <v>6</v>
+      </c>
+      <c r="G462" s="3">
+        <v>7</v>
+      </c>
+      <c r="H462" s="3">
+        <v>8</v>
+      </c>
+      <c r="I462" s="3">
+        <v>10</v>
+      </c>
+      <c r="J462" s="3">
+        <v>11</v>
+      </c>
+      <c r="K462" s="3">
+        <v>12</v>
+      </c>
+      <c r="L462" s="3">
+        <v>14</v>
+      </c>
+      <c r="M462" s="3">
+        <v>15</v>
+      </c>
+      <c r="N462" s="3">
+        <v>17</v>
+      </c>
+      <c r="O462" s="3">
+        <v>23</v>
+      </c>
+      <c r="P462" s="3">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="463" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A463" s="2">
+        <v>3533</v>
+      </c>
+      <c r="B463" s="3">
+        <v>1</v>
+      </c>
+      <c r="C463" s="3">
+        <v>3</v>
+      </c>
+      <c r="D463" s="3">
+        <v>5</v>
+      </c>
+      <c r="E463" s="3">
+        <v>6</v>
+      </c>
+      <c r="F463" s="3">
+        <v>8</v>
+      </c>
+      <c r="G463" s="3">
+        <v>11</v>
+      </c>
+      <c r="H463" s="3">
+        <v>12</v>
+      </c>
+      <c r="I463" s="3">
+        <v>13</v>
+      </c>
+      <c r="J463" s="3">
+        <v>14</v>
+      </c>
+      <c r="K463" s="3">
+        <v>15</v>
+      </c>
+      <c r="L463" s="3">
+        <v>19</v>
+      </c>
+      <c r="M463" s="3">
+        <v>20</v>
+      </c>
+      <c r="N463" s="3">
+        <v>22</v>
+      </c>
+      <c r="O463" s="3">
+        <v>23</v>
+      </c>
+      <c r="P463" s="3">
+        <v>25</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <PublishingExpirationDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
@@ -23242,6 +23635,15 @@
     <AtualizadoPeloTimerJobEm xmlns="4455b8ba-124f-46d5-aaaa-9813efd83d1e">2025-08-17T04:03:58+00:00</AtualizadoPeloTimerJobEm>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -23413,20 +23815,20 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{82B637BD-743B-452C-A85E-33AF8B93F052}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0328C38C-FE97-4791-8469-4B5D9CCC5D08}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
     <ds:schemaRef ds:uri="4455b8ba-124f-46d5-aaaa-9813efd83d1e"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{82B637BD-743B-452C-A85E-33AF8B93F052}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
ImplementaÃ§Ã£o do Google Analytics (G-17YN7Z48QN) e atualizaÃ§Ã£o dos dados das loterias
</commit_message>
<xml_diff>
--- a/LoteriasExcel/Lotofacil_edt2.xlsx
+++ b/LoteriasExcel/Lotofacil_edt2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\Dropbox\! 000 ByPass\Pessoal\99_Loterias\0 - Loterias-Inteligentes\LoteriasExcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C46F418F-E353-49DA-B6E8-9628CC40E5A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8659FFBF-486F-4A90-A8B8-1642BBC24339}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="61215" yWindow="3540" windowWidth="23685" windowHeight="13800" tabRatio="876" xr2:uid="{2663372B-AA50-4721-AD6B-5F0B8186ACF5}"/>
+    <workbookView xWindow="57690" yWindow="420" windowWidth="26025" windowHeight="11475" tabRatio="876" xr2:uid="{2663372B-AA50-4721-AD6B-5F0B8186ACF5}"/>
   </bookViews>
   <sheets>
     <sheet name="LOTOFÁCIL" sheetId="3" r:id="rId1"/>
@@ -130,13 +130,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -457,11 +455,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69BEFC42-DD13-4DE0-B2AD-D0F44AF8189C}">
-  <dimension ref="A1:P463"/>
+  <dimension ref="A1:P466"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A445" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B456" sqref="B456:P463"/>
+      <selection pane="bottomLeft" activeCell="P464" sqref="P464"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -23223,403 +23221,553 @@
       </c>
     </row>
     <row r="456" spans="1:16" x14ac:dyDescent="0.4">
-      <c r="A456" s="2">
+      <c r="A456">
         <v>3526</v>
       </c>
-      <c r="B456" s="3">
-        <v>1</v>
-      </c>
-      <c r="C456" s="3">
-        <v>3</v>
-      </c>
-      <c r="D456" s="3">
-        <v>7</v>
-      </c>
-      <c r="E456" s="3">
-        <v>8</v>
-      </c>
-      <c r="F456" s="3">
-        <v>10</v>
-      </c>
-      <c r="G456" s="3">
-        <v>12</v>
-      </c>
-      <c r="H456" s="3">
-        <v>14</v>
-      </c>
-      <c r="I456" s="3">
-        <v>15</v>
-      </c>
-      <c r="J456" s="3">
-        <v>17</v>
-      </c>
-      <c r="K456" s="3">
-        <v>18</v>
-      </c>
-      <c r="L456" s="3">
-        <v>19</v>
-      </c>
-      <c r="M456" s="3">
-        <v>20</v>
-      </c>
-      <c r="N456" s="3">
-        <v>21</v>
-      </c>
-      <c r="O456" s="3">
-        <v>22</v>
-      </c>
-      <c r="P456" s="3">
+      <c r="B456">
+        <v>1</v>
+      </c>
+      <c r="C456">
+        <v>3</v>
+      </c>
+      <c r="D456">
+        <v>7</v>
+      </c>
+      <c r="E456">
+        <v>8</v>
+      </c>
+      <c r="F456">
+        <v>10</v>
+      </c>
+      <c r="G456">
+        <v>12</v>
+      </c>
+      <c r="H456">
+        <v>14</v>
+      </c>
+      <c r="I456">
+        <v>15</v>
+      </c>
+      <c r="J456">
+        <v>17</v>
+      </c>
+      <c r="K456">
+        <v>18</v>
+      </c>
+      <c r="L456">
+        <v>19</v>
+      </c>
+      <c r="M456">
+        <v>20</v>
+      </c>
+      <c r="N456">
+        <v>21</v>
+      </c>
+      <c r="O456">
+        <v>22</v>
+      </c>
+      <c r="P456">
         <v>23</v>
       </c>
     </row>
     <row r="457" spans="1:16" x14ac:dyDescent="0.4">
-      <c r="A457" s="2">
+      <c r="A457">
         <v>3527</v>
       </c>
-      <c r="B457" s="3">
-        <v>2</v>
-      </c>
-      <c r="C457" s="3">
-        <v>3</v>
-      </c>
-      <c r="D457" s="3">
-        <v>4</v>
-      </c>
-      <c r="E457" s="3">
-        <v>6</v>
-      </c>
-      <c r="F457" s="3">
-        <v>7</v>
-      </c>
-      <c r="G457" s="3">
-        <v>9</v>
-      </c>
-      <c r="H457" s="3">
-        <v>13</v>
-      </c>
-      <c r="I457" s="3">
-        <v>14</v>
-      </c>
-      <c r="J457" s="3">
-        <v>15</v>
-      </c>
-      <c r="K457" s="3">
-        <v>16</v>
-      </c>
-      <c r="L457" s="3">
-        <v>17</v>
-      </c>
-      <c r="M457" s="3">
-        <v>19</v>
-      </c>
-      <c r="N457" s="3">
-        <v>20</v>
-      </c>
-      <c r="O457" s="3">
-        <v>23</v>
-      </c>
-      <c r="P457" s="3">
+      <c r="B457">
+        <v>2</v>
+      </c>
+      <c r="C457">
+        <v>3</v>
+      </c>
+      <c r="D457">
+        <v>4</v>
+      </c>
+      <c r="E457">
+        <v>6</v>
+      </c>
+      <c r="F457">
+        <v>7</v>
+      </c>
+      <c r="G457">
+        <v>9</v>
+      </c>
+      <c r="H457">
+        <v>13</v>
+      </c>
+      <c r="I457">
+        <v>14</v>
+      </c>
+      <c r="J457">
+        <v>15</v>
+      </c>
+      <c r="K457">
+        <v>16</v>
+      </c>
+      <c r="L457">
+        <v>17</v>
+      </c>
+      <c r="M457">
+        <v>19</v>
+      </c>
+      <c r="N457">
+        <v>20</v>
+      </c>
+      <c r="O457">
+        <v>23</v>
+      </c>
+      <c r="P457">
         <v>24</v>
       </c>
     </row>
     <row r="458" spans="1:16" x14ac:dyDescent="0.4">
-      <c r="A458" s="2">
+      <c r="A458">
         <v>3528</v>
       </c>
-      <c r="B458" s="3">
-        <v>1</v>
-      </c>
-      <c r="C458" s="3">
-        <v>3</v>
-      </c>
-      <c r="D458" s="3">
-        <v>5</v>
-      </c>
-      <c r="E458" s="3">
-        <v>6</v>
-      </c>
-      <c r="F458" s="3">
-        <v>7</v>
-      </c>
-      <c r="G458" s="3">
-        <v>9</v>
-      </c>
-      <c r="H458" s="3">
-        <v>10</v>
-      </c>
-      <c r="I458" s="3">
-        <v>16</v>
-      </c>
-      <c r="J458" s="3">
-        <v>18</v>
-      </c>
-      <c r="K458" s="3">
-        <v>19</v>
-      </c>
-      <c r="L458" s="3">
-        <v>20</v>
-      </c>
-      <c r="M458" s="3">
-        <v>22</v>
-      </c>
-      <c r="N458" s="3">
-        <v>23</v>
-      </c>
-      <c r="O458" s="3">
-        <v>24</v>
-      </c>
-      <c r="P458" s="3">
+      <c r="B458">
+        <v>1</v>
+      </c>
+      <c r="C458">
+        <v>3</v>
+      </c>
+      <c r="D458">
+        <v>5</v>
+      </c>
+      <c r="E458">
+        <v>6</v>
+      </c>
+      <c r="F458">
+        <v>7</v>
+      </c>
+      <c r="G458">
+        <v>9</v>
+      </c>
+      <c r="H458">
+        <v>10</v>
+      </c>
+      <c r="I458">
+        <v>16</v>
+      </c>
+      <c r="J458">
+        <v>18</v>
+      </c>
+      <c r="K458">
+        <v>19</v>
+      </c>
+      <c r="L458">
+        <v>20</v>
+      </c>
+      <c r="M458">
+        <v>22</v>
+      </c>
+      <c r="N458">
+        <v>23</v>
+      </c>
+      <c r="O458">
+        <v>24</v>
+      </c>
+      <c r="P458">
         <v>25</v>
       </c>
     </row>
     <row r="459" spans="1:16" x14ac:dyDescent="0.4">
-      <c r="A459" s="2">
+      <c r="A459">
         <v>3529</v>
       </c>
-      <c r="B459" s="3">
-        <v>1</v>
-      </c>
-      <c r="C459" s="3">
-        <v>7</v>
-      </c>
-      <c r="D459" s="3">
-        <v>8</v>
-      </c>
-      <c r="E459" s="3">
-        <v>10</v>
-      </c>
-      <c r="F459" s="3">
-        <v>11</v>
-      </c>
-      <c r="G459" s="3">
-        <v>12</v>
-      </c>
-      <c r="H459" s="3">
-        <v>14</v>
-      </c>
-      <c r="I459" s="3">
-        <v>15</v>
-      </c>
-      <c r="J459" s="3">
-        <v>16</v>
-      </c>
-      <c r="K459" s="3">
-        <v>17</v>
-      </c>
-      <c r="L459" s="3">
-        <v>18</v>
-      </c>
-      <c r="M459" s="3">
-        <v>19</v>
-      </c>
-      <c r="N459" s="3">
-        <v>20</v>
-      </c>
-      <c r="O459" s="3">
-        <v>22</v>
-      </c>
-      <c r="P459" s="3">
+      <c r="B459">
+        <v>1</v>
+      </c>
+      <c r="C459">
+        <v>7</v>
+      </c>
+      <c r="D459">
+        <v>8</v>
+      </c>
+      <c r="E459">
+        <v>10</v>
+      </c>
+      <c r="F459">
+        <v>11</v>
+      </c>
+      <c r="G459">
+        <v>12</v>
+      </c>
+      <c r="H459">
+        <v>14</v>
+      </c>
+      <c r="I459">
+        <v>15</v>
+      </c>
+      <c r="J459">
+        <v>16</v>
+      </c>
+      <c r="K459">
+        <v>17</v>
+      </c>
+      <c r="L459">
+        <v>18</v>
+      </c>
+      <c r="M459">
+        <v>19</v>
+      </c>
+      <c r="N459">
+        <v>20</v>
+      </c>
+      <c r="O459">
+        <v>22</v>
+      </c>
+      <c r="P459">
         <v>24</v>
       </c>
     </row>
     <row r="460" spans="1:16" x14ac:dyDescent="0.4">
-      <c r="A460" s="2">
+      <c r="A460">
         <v>3530</v>
       </c>
-      <c r="B460" s="3">
-        <v>1</v>
-      </c>
-      <c r="C460" s="3">
-        <v>2</v>
-      </c>
-      <c r="D460" s="3">
-        <v>3</v>
-      </c>
-      <c r="E460" s="3">
-        <v>5</v>
-      </c>
-      <c r="F460" s="3">
-        <v>7</v>
-      </c>
-      <c r="G460" s="3">
-        <v>11</v>
-      </c>
-      <c r="H460" s="3">
-        <v>12</v>
-      </c>
-      <c r="I460" s="3">
-        <v>13</v>
-      </c>
-      <c r="J460" s="3">
-        <v>15</v>
-      </c>
-      <c r="K460" s="3">
-        <v>16</v>
-      </c>
-      <c r="L460" s="3">
-        <v>20</v>
-      </c>
-      <c r="M460" s="3">
-        <v>22</v>
-      </c>
-      <c r="N460" s="3">
-        <v>23</v>
-      </c>
-      <c r="O460" s="3">
-        <v>24</v>
-      </c>
-      <c r="P460" s="3">
+      <c r="B460">
+        <v>1</v>
+      </c>
+      <c r="C460">
+        <v>2</v>
+      </c>
+      <c r="D460">
+        <v>3</v>
+      </c>
+      <c r="E460">
+        <v>5</v>
+      </c>
+      <c r="F460">
+        <v>7</v>
+      </c>
+      <c r="G460">
+        <v>11</v>
+      </c>
+      <c r="H460">
+        <v>12</v>
+      </c>
+      <c r="I460">
+        <v>13</v>
+      </c>
+      <c r="J460">
+        <v>15</v>
+      </c>
+      <c r="K460">
+        <v>16</v>
+      </c>
+      <c r="L460">
+        <v>20</v>
+      </c>
+      <c r="M460">
+        <v>22</v>
+      </c>
+      <c r="N460">
+        <v>23</v>
+      </c>
+      <c r="O460">
+        <v>24</v>
+      </c>
+      <c r="P460">
         <v>25</v>
       </c>
     </row>
     <row r="461" spans="1:16" x14ac:dyDescent="0.4">
-      <c r="A461" s="2">
+      <c r="A461">
         <v>3531</v>
       </c>
-      <c r="B461" s="3">
-        <v>1</v>
-      </c>
-      <c r="C461" s="3">
-        <v>3</v>
-      </c>
-      <c r="D461" s="3">
-        <v>4</v>
-      </c>
-      <c r="E461" s="3">
-        <v>5</v>
-      </c>
-      <c r="F461" s="3">
-        <v>7</v>
-      </c>
-      <c r="G461" s="3">
-        <v>8</v>
-      </c>
-      <c r="H461" s="3">
-        <v>10</v>
-      </c>
-      <c r="I461" s="3">
-        <v>11</v>
-      </c>
-      <c r="J461" s="3">
-        <v>12</v>
-      </c>
-      <c r="K461" s="3">
-        <v>14</v>
-      </c>
-      <c r="L461" s="3">
-        <v>15</v>
-      </c>
-      <c r="M461" s="3">
-        <v>16</v>
-      </c>
-      <c r="N461" s="3">
-        <v>18</v>
-      </c>
-      <c r="O461" s="3">
-        <v>19</v>
-      </c>
-      <c r="P461" s="3">
+      <c r="B461">
+        <v>1</v>
+      </c>
+      <c r="C461">
+        <v>3</v>
+      </c>
+      <c r="D461">
+        <v>4</v>
+      </c>
+      <c r="E461">
+        <v>5</v>
+      </c>
+      <c r="F461">
+        <v>7</v>
+      </c>
+      <c r="G461">
+        <v>8</v>
+      </c>
+      <c r="H461">
+        <v>10</v>
+      </c>
+      <c r="I461">
+        <v>11</v>
+      </c>
+      <c r="J461">
+        <v>12</v>
+      </c>
+      <c r="K461">
+        <v>14</v>
+      </c>
+      <c r="L461">
+        <v>15</v>
+      </c>
+      <c r="M461">
+        <v>16</v>
+      </c>
+      <c r="N461">
+        <v>18</v>
+      </c>
+      <c r="O461">
+        <v>19</v>
+      </c>
+      <c r="P461">
         <v>22</v>
       </c>
     </row>
     <row r="462" spans="1:16" x14ac:dyDescent="0.4">
-      <c r="A462" s="2">
+      <c r="A462">
         <v>3532</v>
       </c>
-      <c r="B462" s="3">
-        <v>2</v>
-      </c>
-      <c r="C462" s="3">
-        <v>3</v>
-      </c>
-      <c r="D462" s="3">
-        <v>4</v>
-      </c>
-      <c r="E462" s="3">
-        <v>5</v>
-      </c>
-      <c r="F462" s="3">
-        <v>6</v>
-      </c>
-      <c r="G462" s="3">
-        <v>7</v>
-      </c>
-      <c r="H462" s="3">
-        <v>8</v>
-      </c>
-      <c r="I462" s="3">
-        <v>10</v>
-      </c>
-      <c r="J462" s="3">
-        <v>11</v>
-      </c>
-      <c r="K462" s="3">
-        <v>12</v>
-      </c>
-      <c r="L462" s="3">
-        <v>14</v>
-      </c>
-      <c r="M462" s="3">
-        <v>15</v>
-      </c>
-      <c r="N462" s="3">
-        <v>17</v>
-      </c>
-      <c r="O462" s="3">
-        <v>23</v>
-      </c>
-      <c r="P462" s="3">
+      <c r="B462">
+        <v>2</v>
+      </c>
+      <c r="C462">
+        <v>3</v>
+      </c>
+      <c r="D462">
+        <v>4</v>
+      </c>
+      <c r="E462">
+        <v>5</v>
+      </c>
+      <c r="F462">
+        <v>6</v>
+      </c>
+      <c r="G462">
+        <v>7</v>
+      </c>
+      <c r="H462">
+        <v>8</v>
+      </c>
+      <c r="I462">
+        <v>10</v>
+      </c>
+      <c r="J462">
+        <v>11</v>
+      </c>
+      <c r="K462">
+        <v>12</v>
+      </c>
+      <c r="L462">
+        <v>14</v>
+      </c>
+      <c r="M462">
+        <v>15</v>
+      </c>
+      <c r="N462">
+        <v>17</v>
+      </c>
+      <c r="O462">
+        <v>23</v>
+      </c>
+      <c r="P462">
         <v>25</v>
       </c>
     </row>
     <row r="463" spans="1:16" x14ac:dyDescent="0.4">
-      <c r="A463" s="2">
+      <c r="A463">
         <v>3533</v>
       </c>
-      <c r="B463" s="3">
-        <v>1</v>
-      </c>
-      <c r="C463" s="3">
-        <v>3</v>
-      </c>
-      <c r="D463" s="3">
-        <v>5</v>
-      </c>
-      <c r="E463" s="3">
-        <v>6</v>
-      </c>
-      <c r="F463" s="3">
-        <v>8</v>
-      </c>
-      <c r="G463" s="3">
-        <v>11</v>
-      </c>
-      <c r="H463" s="3">
-        <v>12</v>
-      </c>
-      <c r="I463" s="3">
-        <v>13</v>
-      </c>
-      <c r="J463" s="3">
-        <v>14</v>
-      </c>
-      <c r="K463" s="3">
-        <v>15</v>
-      </c>
-      <c r="L463" s="3">
-        <v>19</v>
-      </c>
-      <c r="M463" s="3">
-        <v>20</v>
-      </c>
-      <c r="N463" s="3">
-        <v>22</v>
-      </c>
-      <c r="O463" s="3">
-        <v>23</v>
-      </c>
-      <c r="P463" s="3">
-        <v>25</v>
+      <c r="B463">
+        <v>1</v>
+      </c>
+      <c r="C463">
+        <v>3</v>
+      </c>
+      <c r="D463">
+        <v>5</v>
+      </c>
+      <c r="E463">
+        <v>6</v>
+      </c>
+      <c r="F463">
+        <v>8</v>
+      </c>
+      <c r="G463">
+        <v>11</v>
+      </c>
+      <c r="H463">
+        <v>12</v>
+      </c>
+      <c r="I463">
+        <v>13</v>
+      </c>
+      <c r="J463">
+        <v>14</v>
+      </c>
+      <c r="K463">
+        <v>15</v>
+      </c>
+      <c r="L463">
+        <v>19</v>
+      </c>
+      <c r="M463">
+        <v>20</v>
+      </c>
+      <c r="N463">
+        <v>22</v>
+      </c>
+      <c r="O463">
+        <v>23</v>
+      </c>
+      <c r="P463">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="464" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A464">
+        <v>3534</v>
+      </c>
+      <c r="B464">
+        <v>1</v>
+      </c>
+      <c r="C464">
+        <v>3</v>
+      </c>
+      <c r="D464">
+        <v>7</v>
+      </c>
+      <c r="E464">
+        <v>9</v>
+      </c>
+      <c r="F464">
+        <v>11</v>
+      </c>
+      <c r="G464">
+        <v>12</v>
+      </c>
+      <c r="H464">
+        <v>13</v>
+      </c>
+      <c r="I464">
+        <v>14</v>
+      </c>
+      <c r="J464">
+        <v>15</v>
+      </c>
+      <c r="K464">
+        <v>16</v>
+      </c>
+      <c r="L464">
+        <v>17</v>
+      </c>
+      <c r="M464">
+        <v>19</v>
+      </c>
+      <c r="N464">
+        <v>20</v>
+      </c>
+      <c r="O464">
+        <v>21</v>
+      </c>
+      <c r="P464">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="465" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A465">
+        <v>3535</v>
+      </c>
+      <c r="B465">
+        <v>2</v>
+      </c>
+      <c r="C465">
+        <v>3</v>
+      </c>
+      <c r="D465">
+        <v>6</v>
+      </c>
+      <c r="E465">
+        <v>7</v>
+      </c>
+      <c r="F465">
+        <v>8</v>
+      </c>
+      <c r="G465">
+        <v>9</v>
+      </c>
+      <c r="H465">
+        <v>11</v>
+      </c>
+      <c r="I465">
+        <v>13</v>
+      </c>
+      <c r="J465">
+        <v>18</v>
+      </c>
+      <c r="K465">
+        <v>19</v>
+      </c>
+      <c r="L465">
+        <v>20</v>
+      </c>
+      <c r="M465">
+        <v>21</v>
+      </c>
+      <c r="N465">
+        <v>22</v>
+      </c>
+      <c r="O465">
+        <v>24</v>
+      </c>
+      <c r="P465">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="466" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A466">
+        <v>3536</v>
+      </c>
+      <c r="B466">
+        <v>1</v>
+      </c>
+      <c r="C466">
+        <v>3</v>
+      </c>
+      <c r="D466">
+        <v>4</v>
+      </c>
+      <c r="E466">
+        <v>6</v>
+      </c>
+      <c r="F466">
+        <v>7</v>
+      </c>
+      <c r="G466">
+        <v>8</v>
+      </c>
+      <c r="H466">
+        <v>9</v>
+      </c>
+      <c r="I466">
+        <v>10</v>
+      </c>
+      <c r="J466">
+        <v>11</v>
+      </c>
+      <c r="K466">
+        <v>15</v>
+      </c>
+      <c r="L466">
+        <v>16</v>
+      </c>
+      <c r="M466">
+        <v>17</v>
+      </c>
+      <c r="N466">
+        <v>18</v>
+      </c>
+      <c r="O466">
+        <v>22</v>
+      </c>
+      <c r="P466">
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -23628,6 +23776,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <PublishingExpirationDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
@@ -23635,15 +23792,6 @@
     <AtualizadoPeloTimerJobEm xmlns="4455b8ba-124f-46d5-aaaa-9813efd83d1e">2025-08-17T04:03:58+00:00</AtualizadoPeloTimerJobEm>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -23815,20 +23963,20 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{82B637BD-743B-452C-A85E-33AF8B93F052}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0328C38C-FE97-4791-8469-4B5D9CCC5D08}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
     <ds:schemaRef ds:uri="4455b8ba-124f-46d5-aaaa-9813efd83d1e"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{82B637BD-743B-452C-A85E-33AF8B93F052}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
AtualizaÃ§Ã£o dos resultados das loterias - LotofÃ¡cil, Lotomania, MegaSena, Quina e carrossel
</commit_message>
<xml_diff>
--- a/LoteriasExcel/Lotofacil_edt2.xlsx
+++ b/LoteriasExcel/Lotofacil_edt2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\Dropbox\! 000 ByPass\Pessoal\99_Loterias\0 - Loterias-Inteligentes\LoteriasExcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8659FFBF-486F-4A90-A8B8-1642BBC24339}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0B5CD55-5ED5-4063-86CE-0E8BE76B318F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57690" yWindow="420" windowWidth="26025" windowHeight="11475" tabRatio="876" xr2:uid="{2663372B-AA50-4721-AD6B-5F0B8186ACF5}"/>
+    <workbookView xWindow="68475" yWindow="1290" windowWidth="28800" windowHeight="15150" tabRatio="876" xr2:uid="{2663372B-AA50-4721-AD6B-5F0B8186ACF5}"/>
   </bookViews>
   <sheets>
     <sheet name="LOTOFÁCIL" sheetId="3" r:id="rId1"/>
@@ -455,11 +455,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69BEFC42-DD13-4DE0-B2AD-D0F44AF8189C}">
-  <dimension ref="A1:P466"/>
+  <dimension ref="A1:P468"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A445" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P464" sqref="P464"/>
+      <selection pane="bottomLeft" activeCell="D472" sqref="D472"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -23770,21 +23770,112 @@
         <v>24</v>
       </c>
     </row>
+    <row r="467" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A467">
+        <v>3537</v>
+      </c>
+      <c r="B467">
+        <v>1</v>
+      </c>
+      <c r="C467">
+        <v>2</v>
+      </c>
+      <c r="D467">
+        <v>3</v>
+      </c>
+      <c r="E467">
+        <v>4</v>
+      </c>
+      <c r="F467">
+        <v>7</v>
+      </c>
+      <c r="G467">
+        <v>9</v>
+      </c>
+      <c r="H467">
+        <v>10</v>
+      </c>
+      <c r="I467">
+        <v>12</v>
+      </c>
+      <c r="J467">
+        <v>15</v>
+      </c>
+      <c r="K467">
+        <v>19</v>
+      </c>
+      <c r="L467">
+        <v>20</v>
+      </c>
+      <c r="M467">
+        <v>21</v>
+      </c>
+      <c r="N467">
+        <v>22</v>
+      </c>
+      <c r="O467">
+        <v>24</v>
+      </c>
+      <c r="P467">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="468" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A468">
+        <v>3538</v>
+      </c>
+      <c r="B468">
+        <v>2</v>
+      </c>
+      <c r="C468">
+        <v>3</v>
+      </c>
+      <c r="D468">
+        <v>5</v>
+      </c>
+      <c r="E468">
+        <v>8</v>
+      </c>
+      <c r="F468">
+        <v>9</v>
+      </c>
+      <c r="G468">
+        <v>10</v>
+      </c>
+      <c r="H468">
+        <v>13</v>
+      </c>
+      <c r="I468">
+        <v>14</v>
+      </c>
+      <c r="J468">
+        <v>17</v>
+      </c>
+      <c r="K468">
+        <v>19</v>
+      </c>
+      <c r="L468">
+        <v>20</v>
+      </c>
+      <c r="M468">
+        <v>21</v>
+      </c>
+      <c r="N468">
+        <v>22</v>
+      </c>
+      <c r="O468">
+        <v>24</v>
+      </c>
+      <c r="P468">
+        <v>25</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <PublishingExpirationDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
@@ -23792,6 +23883,15 @@
     <AtualizadoPeloTimerJobEm xmlns="4455b8ba-124f-46d5-aaaa-9813efd83d1e">2025-08-17T04:03:58+00:00</AtualizadoPeloTimerJobEm>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -23963,20 +24063,20 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{82B637BD-743B-452C-A85E-33AF8B93F052}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0328C38C-FE97-4791-8469-4B5D9CCC5D08}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
     <ds:schemaRef ds:uri="4455b8ba-124f-46d5-aaaa-9813efd83d1e"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{82B637BD-743B-452C-A85E-33AF8B93F052}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
AtualizaÃ§Ã£o dos resultados das loterias - LotofÃ¡cil, Lotomania, MegaSena, +MilionÃ¡ria, Quina e carrossel
</commit_message>
<xml_diff>
--- a/LoteriasExcel/Lotofacil_edt2.xlsx
+++ b/LoteriasExcel/Lotofacil_edt2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\Dropbox\! 000 ByPass\Pessoal\99_Loterias\0 - Loterias-Inteligentes\LoteriasExcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0B5CD55-5ED5-4063-86CE-0E8BE76B318F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{049F7491-E6BA-411A-9FAA-FA016BDB8A0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="68475" yWindow="1290" windowWidth="28800" windowHeight="15150" tabRatio="876" xr2:uid="{2663372B-AA50-4721-AD6B-5F0B8186ACF5}"/>
+    <workbookView xWindow="62925" yWindow="2535" windowWidth="20460" windowHeight="16995" tabRatio="876" xr2:uid="{2663372B-AA50-4721-AD6B-5F0B8186ACF5}"/>
   </bookViews>
   <sheets>
     <sheet name="LOTOFÁCIL" sheetId="3" r:id="rId1"/>
@@ -455,11 +455,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69BEFC42-DD13-4DE0-B2AD-D0F44AF8189C}">
-  <dimension ref="A1:P468"/>
+  <dimension ref="A1:P470"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A445" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D472" sqref="D472"/>
+      <pane ySplit="1" topLeftCell="A442" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D465" sqref="D465"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -23870,31 +23870,112 @@
         <v>25</v>
       </c>
     </row>
+    <row r="469" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A469">
+        <v>3539</v>
+      </c>
+      <c r="B469">
+        <v>1</v>
+      </c>
+      <c r="C469">
+        <v>2</v>
+      </c>
+      <c r="D469">
+        <v>7</v>
+      </c>
+      <c r="E469">
+        <v>8</v>
+      </c>
+      <c r="F469">
+        <v>9</v>
+      </c>
+      <c r="G469">
+        <v>11</v>
+      </c>
+      <c r="H469">
+        <v>12</v>
+      </c>
+      <c r="I469">
+        <v>131</v>
+      </c>
+      <c r="J469">
+        <v>14</v>
+      </c>
+      <c r="K469">
+        <v>16</v>
+      </c>
+      <c r="L469">
+        <v>18</v>
+      </c>
+      <c r="M469">
+        <v>19</v>
+      </c>
+      <c r="N469">
+        <v>20</v>
+      </c>
+      <c r="O469">
+        <v>23</v>
+      </c>
+      <c r="P469">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="470" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A470">
+        <v>3540</v>
+      </c>
+      <c r="B470">
+        <v>1</v>
+      </c>
+      <c r="C470">
+        <v>2</v>
+      </c>
+      <c r="D470">
+        <v>3</v>
+      </c>
+      <c r="E470">
+        <v>5</v>
+      </c>
+      <c r="F470">
+        <v>6</v>
+      </c>
+      <c r="G470">
+        <v>9</v>
+      </c>
+      <c r="H470">
+        <v>10</v>
+      </c>
+      <c r="I470">
+        <v>13</v>
+      </c>
+      <c r="J470">
+        <v>14</v>
+      </c>
+      <c r="K470">
+        <v>15</v>
+      </c>
+      <c r="L470">
+        <v>16</v>
+      </c>
+      <c r="M470">
+        <v>18</v>
+      </c>
+      <c r="N470">
+        <v>22</v>
+      </c>
+      <c r="O470">
+        <v>23</v>
+      </c>
+      <c r="P470">
+        <v>25</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <PublishingExpirationDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <PublishingStartDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <AtualizadoPeloTimerJobEm xmlns="4455b8ba-124f-46d5-aaaa-9813efd83d1e">2025-08-17T04:03:58+00:00</AtualizadoPeloTimerJobEm>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100C92CDE8829F3C7438DCCB0991C30EAAE" ma:contentTypeVersion="3" ma:contentTypeDescription="Crie um novo documento." ma:contentTypeScope="" ma:versionID="36cf41eecaf38ba1d849a0c8dd067090">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="3e38fcf2-aa96-4a2c-865b-c3abba01ba51" xmlns:ns3="4455b8ba-124f-46d5-aaaa-9813efd83d1e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="023f68b2d27389a617bf935a3f0e17ad" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -24062,26 +24143,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0328C38C-FE97-4791-8469-4B5D9CCC5D08}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="4455b8ba-124f-46d5-aaaa-9813efd83d1e"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{82B637BD-743B-452C-A85E-33AF8B93F052}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <PublishingExpirationDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <PublishingStartDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <AtualizadoPeloTimerJobEm xmlns="4455b8ba-124f-46d5-aaaa-9813efd83d1e">2025-08-17T04:03:58+00:00</AtualizadoPeloTimerJobEm>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{46C5B8C5-4575-4105-836C-9C4A6674A14B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -24099,4 +24180,23 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{82B637BD-743B-452C-A85E-33AF8B93F052}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0328C38C-FE97-4791-8469-4B5D9CCC5D08}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="4455b8ba-124f-46d5-aaaa-9813efd83d1e"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
AtualizaÃ§Ã£o dos resultados das loterias da Caixa - dados mais recentes para os usuÃ¡rios
</commit_message>
<xml_diff>
--- a/LoteriasExcel/Lotofacil_edt2.xlsx
+++ b/LoteriasExcel/Lotofacil_edt2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\Dropbox\! 000 ByPass\Pessoal\99_Loterias\0 - Loterias-Inteligentes\LoteriasExcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{049F7491-E6BA-411A-9FAA-FA016BDB8A0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{690614F6-7722-428E-A2A5-5C56CF244FDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="62925" yWindow="2535" windowWidth="20460" windowHeight="16995" tabRatio="876" xr2:uid="{2663372B-AA50-4721-AD6B-5F0B8186ACF5}"/>
+    <workbookView xWindow="69915" yWindow="0" windowWidth="24690" windowHeight="10050" tabRatio="876" xr2:uid="{2663372B-AA50-4721-AD6B-5F0B8186ACF5}"/>
   </bookViews>
   <sheets>
     <sheet name="LOTOFÁCIL" sheetId="3" r:id="rId1"/>
@@ -455,11 +455,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69BEFC42-DD13-4DE0-B2AD-D0F44AF8189C}">
-  <dimension ref="A1:P470"/>
+  <dimension ref="A1:P481"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A442" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D465" sqref="D465"/>
+      <pane ySplit="1" topLeftCell="A463" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B471" sqref="B471:P481"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -23970,12 +23970,571 @@
         <v>25</v>
       </c>
     </row>
+    <row r="471" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A471">
+        <v>3541</v>
+      </c>
+      <c r="B471">
+        <v>1</v>
+      </c>
+      <c r="C471">
+        <v>2</v>
+      </c>
+      <c r="D471">
+        <v>3</v>
+      </c>
+      <c r="E471">
+        <v>4</v>
+      </c>
+      <c r="F471">
+        <v>6</v>
+      </c>
+      <c r="G471">
+        <v>8</v>
+      </c>
+      <c r="H471">
+        <v>13</v>
+      </c>
+      <c r="I471">
+        <v>14</v>
+      </c>
+      <c r="J471">
+        <v>16</v>
+      </c>
+      <c r="K471">
+        <v>17</v>
+      </c>
+      <c r="L471">
+        <v>18</v>
+      </c>
+      <c r="M471">
+        <v>19</v>
+      </c>
+      <c r="N471">
+        <v>21</v>
+      </c>
+      <c r="O471">
+        <v>23</v>
+      </c>
+      <c r="P471">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="472" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A472">
+        <v>3542</v>
+      </c>
+      <c r="B472">
+        <v>1</v>
+      </c>
+      <c r="C472">
+        <v>2</v>
+      </c>
+      <c r="D472">
+        <v>5</v>
+      </c>
+      <c r="E472">
+        <v>8</v>
+      </c>
+      <c r="F472">
+        <v>11</v>
+      </c>
+      <c r="G472">
+        <v>12</v>
+      </c>
+      <c r="H472">
+        <v>13</v>
+      </c>
+      <c r="I472">
+        <v>15</v>
+      </c>
+      <c r="J472">
+        <v>18</v>
+      </c>
+      <c r="K472">
+        <v>19</v>
+      </c>
+      <c r="L472">
+        <v>21</v>
+      </c>
+      <c r="M472">
+        <v>22</v>
+      </c>
+      <c r="N472">
+        <v>23</v>
+      </c>
+      <c r="O472">
+        <v>24</v>
+      </c>
+      <c r="P472">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="473" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A473">
+        <v>3543</v>
+      </c>
+      <c r="B473">
+        <v>1</v>
+      </c>
+      <c r="C473">
+        <v>4</v>
+      </c>
+      <c r="D473">
+        <v>5</v>
+      </c>
+      <c r="E473">
+        <v>6</v>
+      </c>
+      <c r="F473">
+        <v>7</v>
+      </c>
+      <c r="G473">
+        <v>8</v>
+      </c>
+      <c r="H473">
+        <v>9</v>
+      </c>
+      <c r="I473">
+        <v>14</v>
+      </c>
+      <c r="J473">
+        <v>15</v>
+      </c>
+      <c r="K473">
+        <v>16</v>
+      </c>
+      <c r="L473">
+        <v>17</v>
+      </c>
+      <c r="M473">
+        <v>20</v>
+      </c>
+      <c r="N473">
+        <v>21</v>
+      </c>
+      <c r="O473">
+        <v>22</v>
+      </c>
+      <c r="P473">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="474" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A474">
+        <v>3544</v>
+      </c>
+      <c r="B474">
+        <v>1</v>
+      </c>
+      <c r="C474">
+        <v>4</v>
+      </c>
+      <c r="D474">
+        <v>5</v>
+      </c>
+      <c r="E474">
+        <v>6</v>
+      </c>
+      <c r="F474">
+        <v>8</v>
+      </c>
+      <c r="G474">
+        <v>10</v>
+      </c>
+      <c r="H474">
+        <v>11</v>
+      </c>
+      <c r="I474">
+        <v>12</v>
+      </c>
+      <c r="J474">
+        <v>15</v>
+      </c>
+      <c r="K474">
+        <v>17</v>
+      </c>
+      <c r="L474">
+        <v>20</v>
+      </c>
+      <c r="M474">
+        <v>21</v>
+      </c>
+      <c r="N474">
+        <v>22</v>
+      </c>
+      <c r="O474">
+        <v>23</v>
+      </c>
+      <c r="P474">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="475" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A475">
+        <v>3545</v>
+      </c>
+      <c r="B475">
+        <v>1</v>
+      </c>
+      <c r="C475">
+        <v>4</v>
+      </c>
+      <c r="D475">
+        <v>5</v>
+      </c>
+      <c r="E475">
+        <v>6</v>
+      </c>
+      <c r="F475">
+        <v>7</v>
+      </c>
+      <c r="G475">
+        <v>8</v>
+      </c>
+      <c r="H475">
+        <v>11</v>
+      </c>
+      <c r="I475">
+        <v>12</v>
+      </c>
+      <c r="J475">
+        <v>14</v>
+      </c>
+      <c r="K475">
+        <v>17</v>
+      </c>
+      <c r="L475">
+        <v>19</v>
+      </c>
+      <c r="M475">
+        <v>20</v>
+      </c>
+      <c r="N475">
+        <v>21</v>
+      </c>
+      <c r="O475">
+        <v>22</v>
+      </c>
+      <c r="P475">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="476" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A476">
+        <v>3546</v>
+      </c>
+      <c r="B476">
+        <v>2</v>
+      </c>
+      <c r="C476">
+        <v>3</v>
+      </c>
+      <c r="D476">
+        <v>5</v>
+      </c>
+      <c r="E476">
+        <v>7</v>
+      </c>
+      <c r="F476">
+        <v>8</v>
+      </c>
+      <c r="G476">
+        <v>11</v>
+      </c>
+      <c r="H476">
+        <v>12</v>
+      </c>
+      <c r="I476">
+        <v>13</v>
+      </c>
+      <c r="J476">
+        <v>18</v>
+      </c>
+      <c r="K476">
+        <v>19</v>
+      </c>
+      <c r="L476">
+        <v>20</v>
+      </c>
+      <c r="M476">
+        <v>22</v>
+      </c>
+      <c r="N476">
+        <v>23</v>
+      </c>
+      <c r="O476">
+        <v>24</v>
+      </c>
+      <c r="P476">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="477" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A477">
+        <v>3547</v>
+      </c>
+      <c r="B477">
+        <v>2</v>
+      </c>
+      <c r="C477">
+        <v>5</v>
+      </c>
+      <c r="D477">
+        <v>6</v>
+      </c>
+      <c r="E477">
+        <v>7</v>
+      </c>
+      <c r="F477">
+        <v>9</v>
+      </c>
+      <c r="G477">
+        <v>10</v>
+      </c>
+      <c r="H477">
+        <v>14</v>
+      </c>
+      <c r="I477">
+        <v>15</v>
+      </c>
+      <c r="J477">
+        <v>17</v>
+      </c>
+      <c r="K477">
+        <v>18</v>
+      </c>
+      <c r="L477">
+        <v>19</v>
+      </c>
+      <c r="M477">
+        <v>20</v>
+      </c>
+      <c r="N477">
+        <v>21</v>
+      </c>
+      <c r="O477">
+        <v>24</v>
+      </c>
+      <c r="P477">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="478" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A478">
+        <v>3548</v>
+      </c>
+      <c r="B478">
+        <v>4</v>
+      </c>
+      <c r="C478">
+        <v>8</v>
+      </c>
+      <c r="D478">
+        <v>9</v>
+      </c>
+      <c r="E478">
+        <v>10</v>
+      </c>
+      <c r="F478">
+        <v>11</v>
+      </c>
+      <c r="G478">
+        <v>12</v>
+      </c>
+      <c r="H478">
+        <v>13</v>
+      </c>
+      <c r="I478">
+        <v>15</v>
+      </c>
+      <c r="J478">
+        <v>16</v>
+      </c>
+      <c r="K478">
+        <v>17</v>
+      </c>
+      <c r="L478">
+        <v>19</v>
+      </c>
+      <c r="M478">
+        <v>21</v>
+      </c>
+      <c r="N478">
+        <v>23</v>
+      </c>
+      <c r="O478">
+        <v>24</v>
+      </c>
+      <c r="P478">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="479" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A479">
+        <v>3549</v>
+      </c>
+      <c r="B479">
+        <v>2</v>
+      </c>
+      <c r="C479">
+        <v>5</v>
+      </c>
+      <c r="D479">
+        <v>7</v>
+      </c>
+      <c r="E479">
+        <v>8</v>
+      </c>
+      <c r="F479">
+        <v>9</v>
+      </c>
+      <c r="G479">
+        <v>11</v>
+      </c>
+      <c r="H479">
+        <v>12</v>
+      </c>
+      <c r="I479">
+        <v>14</v>
+      </c>
+      <c r="J479">
+        <v>17</v>
+      </c>
+      <c r="K479">
+        <v>20</v>
+      </c>
+      <c r="L479">
+        <v>21</v>
+      </c>
+      <c r="M479">
+        <v>22</v>
+      </c>
+      <c r="N479">
+        <v>23</v>
+      </c>
+      <c r="O479">
+        <v>24</v>
+      </c>
+      <c r="P479">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="480" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A480">
+        <v>3550</v>
+      </c>
+      <c r="B480">
+        <v>1</v>
+      </c>
+      <c r="C480">
+        <v>4</v>
+      </c>
+      <c r="D480">
+        <v>6</v>
+      </c>
+      <c r="E480">
+        <v>7</v>
+      </c>
+      <c r="F480">
+        <v>8</v>
+      </c>
+      <c r="G480">
+        <v>12</v>
+      </c>
+      <c r="H480">
+        <v>13</v>
+      </c>
+      <c r="I480">
+        <v>15</v>
+      </c>
+      <c r="J480">
+        <v>16</v>
+      </c>
+      <c r="K480">
+        <v>18</v>
+      </c>
+      <c r="L480">
+        <v>19</v>
+      </c>
+      <c r="M480">
+        <v>20</v>
+      </c>
+      <c r="N480">
+        <v>22</v>
+      </c>
+      <c r="O480">
+        <v>23</v>
+      </c>
+      <c r="P480">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="481" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A481">
+        <v>3551</v>
+      </c>
+      <c r="B481">
+        <v>1</v>
+      </c>
+      <c r="C481">
+        <v>2</v>
+      </c>
+      <c r="D481">
+        <v>3</v>
+      </c>
+      <c r="E481">
+        <v>7</v>
+      </c>
+      <c r="F481">
+        <v>8</v>
+      </c>
+      <c r="G481">
+        <v>10</v>
+      </c>
+      <c r="H481">
+        <v>11</v>
+      </c>
+      <c r="I481">
+        <v>12</v>
+      </c>
+      <c r="J481">
+        <v>15</v>
+      </c>
+      <c r="K481">
+        <v>16</v>
+      </c>
+      <c r="L481">
+        <v>17</v>
+      </c>
+      <c r="M481">
+        <v>19</v>
+      </c>
+      <c r="N481">
+        <v>21</v>
+      </c>
+      <c r="O481">
+        <v>22</v>
+      </c>
+      <c r="P481">
+        <v>25</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100C92CDE8829F3C7438DCCB0991C30EAAE" ma:contentTypeVersion="3" ma:contentTypeDescription="Crie um novo documento." ma:contentTypeScope="" ma:versionID="36cf41eecaf38ba1d849a0c8dd067090">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="3e38fcf2-aa96-4a2c-865b-c3abba01ba51" xmlns:ns3="4455b8ba-124f-46d5-aaaa-9813efd83d1e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="023f68b2d27389a617bf935a3f0e17ad" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -24143,15 +24702,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -24163,6 +24713,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{82B637BD-743B-452C-A85E-33AF8B93F052}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{46C5B8C5-4575-4105-836C-9C4A6674A14B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -24182,14 +24740,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{82B637BD-743B-452C-A85E-33AF8B93F052}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0328C38C-FE97-4791-8469-4B5D9CCC5D08}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
AtualizaÃ§Ã£o dos dados dos resultados das loterias - LotofÃ¡cil, Lotomania, Mega-Sena, MilionÃ¡ria e Quina
</commit_message>
<xml_diff>
--- a/LoteriasExcel/Lotofacil_edt2.xlsx
+++ b/LoteriasExcel/Lotofacil_edt2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\Dropbox\! 000 ByPass\Pessoal\99_Loterias\0 - Loterias-Inteligentes\LoteriasExcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{690614F6-7722-428E-A2A5-5C56CF244FDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92AD381D-74D4-49A4-BEE6-08FAFDCB06E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="69915" yWindow="0" windowWidth="24690" windowHeight="10050" tabRatio="876" xr2:uid="{2663372B-AA50-4721-AD6B-5F0B8186ACF5}"/>
+    <workbookView xWindow="75975" yWindow="5760" windowWidth="19545" windowHeight="12000" tabRatio="876" xr2:uid="{2663372B-AA50-4721-AD6B-5F0B8186ACF5}"/>
   </bookViews>
   <sheets>
     <sheet name="LOTOFÁCIL" sheetId="3" r:id="rId1"/>
@@ -130,11 +130,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -455,11 +457,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69BEFC42-DD13-4DE0-B2AD-D0F44AF8189C}">
-  <dimension ref="A1:P481"/>
+  <dimension ref="A1:P492"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A463" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B471" sqref="B471:P481"/>
+      <pane ySplit="1" topLeftCell="A475" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B482" sqref="B482:P492"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -24520,21 +24522,562 @@
         <v>25</v>
       </c>
     </row>
+    <row r="482" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A482" s="2">
+        <v>3552</v>
+      </c>
+      <c r="B482" s="3">
+        <v>4</v>
+      </c>
+      <c r="C482" s="3">
+        <v>5</v>
+      </c>
+      <c r="D482" s="3">
+        <v>6</v>
+      </c>
+      <c r="E482" s="3">
+        <v>7</v>
+      </c>
+      <c r="F482" s="3">
+        <v>11</v>
+      </c>
+      <c r="G482" s="3">
+        <v>12</v>
+      </c>
+      <c r="H482" s="3">
+        <v>14</v>
+      </c>
+      <c r="I482" s="3">
+        <v>15</v>
+      </c>
+      <c r="J482" s="3">
+        <v>16</v>
+      </c>
+      <c r="K482" s="3">
+        <v>17</v>
+      </c>
+      <c r="L482" s="3">
+        <v>18</v>
+      </c>
+      <c r="M482" s="3">
+        <v>20</v>
+      </c>
+      <c r="N482" s="3">
+        <v>21</v>
+      </c>
+      <c r="O482" s="3">
+        <v>23</v>
+      </c>
+      <c r="P482" s="3">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="483" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A483" s="2">
+        <v>3553</v>
+      </c>
+      <c r="B483" s="3">
+        <v>1</v>
+      </c>
+      <c r="C483" s="3">
+        <v>2</v>
+      </c>
+      <c r="D483" s="3">
+        <v>3</v>
+      </c>
+      <c r="E483" s="3">
+        <v>7</v>
+      </c>
+      <c r="F483" s="3">
+        <v>8</v>
+      </c>
+      <c r="G483" s="3">
+        <v>9</v>
+      </c>
+      <c r="H483" s="3">
+        <v>12</v>
+      </c>
+      <c r="I483" s="3">
+        <v>13</v>
+      </c>
+      <c r="J483" s="3">
+        <v>16</v>
+      </c>
+      <c r="K483" s="3">
+        <v>17</v>
+      </c>
+      <c r="L483" s="3">
+        <v>19</v>
+      </c>
+      <c r="M483" s="3">
+        <v>21</v>
+      </c>
+      <c r="N483" s="3">
+        <v>22</v>
+      </c>
+      <c r="O483" s="3">
+        <v>23</v>
+      </c>
+      <c r="P483" s="3">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="484" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A484" s="2">
+        <v>3554</v>
+      </c>
+      <c r="B484" s="3">
+        <v>1</v>
+      </c>
+      <c r="C484" s="3">
+        <v>3</v>
+      </c>
+      <c r="D484" s="3">
+        <v>4</v>
+      </c>
+      <c r="E484" s="3">
+        <v>5</v>
+      </c>
+      <c r="F484" s="3">
+        <v>8</v>
+      </c>
+      <c r="G484" s="3">
+        <v>9</v>
+      </c>
+      <c r="H484" s="3">
+        <v>11</v>
+      </c>
+      <c r="I484" s="3">
+        <v>12</v>
+      </c>
+      <c r="J484" s="3">
+        <v>14</v>
+      </c>
+      <c r="K484" s="3">
+        <v>15</v>
+      </c>
+      <c r="L484" s="3">
+        <v>16</v>
+      </c>
+      <c r="M484" s="3">
+        <v>18</v>
+      </c>
+      <c r="N484" s="3">
+        <v>22</v>
+      </c>
+      <c r="O484" s="3">
+        <v>23</v>
+      </c>
+      <c r="P484" s="3">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="485" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A485" s="2">
+        <v>3555</v>
+      </c>
+      <c r="B485" s="3">
+        <v>1</v>
+      </c>
+      <c r="C485" s="3">
+        <v>2</v>
+      </c>
+      <c r="D485" s="3">
+        <v>3</v>
+      </c>
+      <c r="E485" s="3">
+        <v>4</v>
+      </c>
+      <c r="F485" s="3">
+        <v>7</v>
+      </c>
+      <c r="G485" s="3">
+        <v>8</v>
+      </c>
+      <c r="H485" s="3">
+        <v>10</v>
+      </c>
+      <c r="I485" s="3">
+        <v>13</v>
+      </c>
+      <c r="J485" s="3">
+        <v>14</v>
+      </c>
+      <c r="K485" s="3">
+        <v>15</v>
+      </c>
+      <c r="L485" s="3">
+        <v>18</v>
+      </c>
+      <c r="M485" s="3">
+        <v>19</v>
+      </c>
+      <c r="N485" s="3">
+        <v>20</v>
+      </c>
+      <c r="O485" s="3">
+        <v>23</v>
+      </c>
+      <c r="P485" s="3">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="486" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A486" s="2">
+        <v>3556</v>
+      </c>
+      <c r="B486" s="3">
+        <v>1</v>
+      </c>
+      <c r="C486" s="3">
+        <v>2</v>
+      </c>
+      <c r="D486" s="3">
+        <v>3</v>
+      </c>
+      <c r="E486" s="3">
+        <v>4</v>
+      </c>
+      <c r="F486" s="3">
+        <v>5</v>
+      </c>
+      <c r="G486" s="3">
+        <v>7</v>
+      </c>
+      <c r="H486" s="3">
+        <v>9</v>
+      </c>
+      <c r="I486" s="3">
+        <v>10</v>
+      </c>
+      <c r="J486" s="3">
+        <v>12</v>
+      </c>
+      <c r="K486" s="3">
+        <v>14</v>
+      </c>
+      <c r="L486" s="3">
+        <v>16</v>
+      </c>
+      <c r="M486" s="3">
+        <v>17</v>
+      </c>
+      <c r="N486" s="3">
+        <v>19</v>
+      </c>
+      <c r="O486" s="3">
+        <v>21</v>
+      </c>
+      <c r="P486" s="3">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="487" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A487" s="2">
+        <v>3557</v>
+      </c>
+      <c r="B487" s="3">
+        <v>5</v>
+      </c>
+      <c r="C487" s="3">
+        <v>6</v>
+      </c>
+      <c r="D487" s="3">
+        <v>7</v>
+      </c>
+      <c r="E487" s="3">
+        <v>9</v>
+      </c>
+      <c r="F487" s="3">
+        <v>10</v>
+      </c>
+      <c r="G487" s="3">
+        <v>13</v>
+      </c>
+      <c r="H487" s="3">
+        <v>14</v>
+      </c>
+      <c r="I487" s="3">
+        <v>15</v>
+      </c>
+      <c r="J487" s="3">
+        <v>16</v>
+      </c>
+      <c r="K487" s="3">
+        <v>17</v>
+      </c>
+      <c r="L487" s="3">
+        <v>19</v>
+      </c>
+      <c r="M487" s="3">
+        <v>20</v>
+      </c>
+      <c r="N487" s="3">
+        <v>21</v>
+      </c>
+      <c r="O487" s="3">
+        <v>22</v>
+      </c>
+      <c r="P487" s="3">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="488" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A488" s="2">
+        <v>3558</v>
+      </c>
+      <c r="B488" s="3">
+        <v>2</v>
+      </c>
+      <c r="C488" s="3">
+        <v>3</v>
+      </c>
+      <c r="D488" s="3">
+        <v>4</v>
+      </c>
+      <c r="E488" s="3">
+        <v>7</v>
+      </c>
+      <c r="F488" s="3">
+        <v>9</v>
+      </c>
+      <c r="G488" s="3">
+        <v>12</v>
+      </c>
+      <c r="H488" s="3">
+        <v>13</v>
+      </c>
+      <c r="I488" s="3">
+        <v>14</v>
+      </c>
+      <c r="J488" s="3">
+        <v>15</v>
+      </c>
+      <c r="K488" s="3">
+        <v>18</v>
+      </c>
+      <c r="L488" s="3">
+        <v>20</v>
+      </c>
+      <c r="M488" s="3">
+        <v>22</v>
+      </c>
+      <c r="N488" s="3">
+        <v>23</v>
+      </c>
+      <c r="O488" s="3">
+        <v>24</v>
+      </c>
+      <c r="P488" s="3">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="489" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A489" s="2">
+        <v>3559</v>
+      </c>
+      <c r="B489" s="3">
+        <v>1</v>
+      </c>
+      <c r="C489" s="3">
+        <v>2</v>
+      </c>
+      <c r="D489" s="3">
+        <v>6</v>
+      </c>
+      <c r="E489" s="3">
+        <v>8</v>
+      </c>
+      <c r="F489" s="3">
+        <v>9</v>
+      </c>
+      <c r="G489" s="3">
+        <v>10</v>
+      </c>
+      <c r="H489" s="3">
+        <v>11</v>
+      </c>
+      <c r="I489" s="3">
+        <v>13</v>
+      </c>
+      <c r="J489" s="3">
+        <v>14</v>
+      </c>
+      <c r="K489" s="3">
+        <v>15</v>
+      </c>
+      <c r="L489" s="3">
+        <v>16</v>
+      </c>
+      <c r="M489" s="3">
+        <v>19</v>
+      </c>
+      <c r="N489" s="3">
+        <v>20</v>
+      </c>
+      <c r="O489" s="3">
+        <v>24</v>
+      </c>
+      <c r="P489" s="3">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="490" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A490" s="2">
+        <v>3560</v>
+      </c>
+      <c r="B490" s="3">
+        <v>1</v>
+      </c>
+      <c r="C490" s="3">
+        <v>3</v>
+      </c>
+      <c r="D490" s="3">
+        <v>4</v>
+      </c>
+      <c r="E490" s="3">
+        <v>6</v>
+      </c>
+      <c r="F490" s="3">
+        <v>7</v>
+      </c>
+      <c r="G490" s="3">
+        <v>8</v>
+      </c>
+      <c r="H490" s="3">
+        <v>10</v>
+      </c>
+      <c r="I490" s="3">
+        <v>11</v>
+      </c>
+      <c r="J490" s="3">
+        <v>12</v>
+      </c>
+      <c r="K490" s="3">
+        <v>13</v>
+      </c>
+      <c r="L490" s="3">
+        <v>17</v>
+      </c>
+      <c r="M490" s="3">
+        <v>18</v>
+      </c>
+      <c r="N490" s="3">
+        <v>19</v>
+      </c>
+      <c r="O490" s="3">
+        <v>23</v>
+      </c>
+      <c r="P490" s="3">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="491" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A491" s="2">
+        <v>3561</v>
+      </c>
+      <c r="B491" s="3">
+        <v>1</v>
+      </c>
+      <c r="C491" s="3">
+        <v>2</v>
+      </c>
+      <c r="D491" s="3">
+        <v>4</v>
+      </c>
+      <c r="E491" s="3">
+        <v>5</v>
+      </c>
+      <c r="F491" s="3">
+        <v>6</v>
+      </c>
+      <c r="G491" s="3">
+        <v>7</v>
+      </c>
+      <c r="H491" s="3">
+        <v>8</v>
+      </c>
+      <c r="I491" s="3">
+        <v>10</v>
+      </c>
+      <c r="J491" s="3">
+        <v>15</v>
+      </c>
+      <c r="K491" s="3">
+        <v>16</v>
+      </c>
+      <c r="L491" s="3">
+        <v>17</v>
+      </c>
+      <c r="M491" s="3">
+        <v>18</v>
+      </c>
+      <c r="N491" s="3">
+        <v>20</v>
+      </c>
+      <c r="O491" s="3">
+        <v>21</v>
+      </c>
+      <c r="P491" s="3">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="492" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A492" s="2">
+        <v>3562</v>
+      </c>
+      <c r="B492" s="3">
+        <v>3</v>
+      </c>
+      <c r="C492" s="3">
+        <v>5</v>
+      </c>
+      <c r="D492" s="3">
+        <v>6</v>
+      </c>
+      <c r="E492" s="3">
+        <v>7</v>
+      </c>
+      <c r="F492" s="3">
+        <v>9</v>
+      </c>
+      <c r="G492" s="3">
+        <v>10</v>
+      </c>
+      <c r="H492" s="3">
+        <v>11</v>
+      </c>
+      <c r="I492" s="3">
+        <v>12</v>
+      </c>
+      <c r="J492" s="3">
+        <v>13</v>
+      </c>
+      <c r="K492" s="3">
+        <v>14</v>
+      </c>
+      <c r="L492" s="3">
+        <v>15</v>
+      </c>
+      <c r="M492" s="3">
+        <v>19</v>
+      </c>
+      <c r="N492" s="3">
+        <v>22</v>
+      </c>
+      <c r="O492" s="3">
+        <v>23</v>
+      </c>
+      <c r="P492" s="3">
+        <v>25</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100C92CDE8829F3C7438DCCB0991C30EAAE" ma:contentTypeVersion="3" ma:contentTypeDescription="Crie um novo documento." ma:contentTypeScope="" ma:versionID="36cf41eecaf38ba1d849a0c8dd067090">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="3e38fcf2-aa96-4a2c-865b-c3abba01ba51" xmlns:ns3="4455b8ba-124f-46d5-aaaa-9813efd83d1e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="023f68b2d27389a617bf935a3f0e17ad" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -24702,6 +25245,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -24713,14 +25265,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{82B637BD-743B-452C-A85E-33AF8B93F052}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{46C5B8C5-4575-4105-836C-9C4A6674A14B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -24740,6 +25284,14 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{82B637BD-743B-452C-A85E-33AF8B93F052}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0328C38C-FE97-4791-8469-4B5D9CCC5D08}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
AtualizaÃ§Ã£o dos resultados das loterias - dados mais recentes para o site
</commit_message>
<xml_diff>
--- a/LoteriasExcel/Lotofacil_edt2.xlsx
+++ b/LoteriasExcel/Lotofacil_edt2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\Dropbox\! 000 ByPass\Pessoal\99_Loterias\0 - Loterias-Inteligentes\LoteriasExcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92AD381D-74D4-49A4-BEE6-08FAFDCB06E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F52542F-5276-4D6C-A11F-E4F8502F2D67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="75975" yWindow="5760" windowWidth="19545" windowHeight="12000" tabRatio="876" xr2:uid="{2663372B-AA50-4721-AD6B-5F0B8186ACF5}"/>
+    <workbookView xWindow="58260" yWindow="660" windowWidth="19545" windowHeight="12000" tabRatio="876" xr2:uid="{2663372B-AA50-4721-AD6B-5F0B8186ACF5}"/>
   </bookViews>
   <sheets>
     <sheet name="LOTOFÁCIL" sheetId="3" r:id="rId1"/>
@@ -457,11 +457,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69BEFC42-DD13-4DE0-B2AD-D0F44AF8189C}">
-  <dimension ref="A1:P492"/>
+  <dimension ref="A1:P495"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A475" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B482" sqref="B482:P492"/>
+      <selection pane="bottomLeft" activeCell="B493" sqref="B493:P495"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -24523,552 +24523,702 @@
       </c>
     </row>
     <row r="482" spans="1:16" x14ac:dyDescent="0.4">
-      <c r="A482" s="2">
+      <c r="A482">
         <v>3552</v>
       </c>
-      <c r="B482" s="3">
-        <v>4</v>
-      </c>
-      <c r="C482" s="3">
-        <v>5</v>
-      </c>
-      <c r="D482" s="3">
-        <v>6</v>
-      </c>
-      <c r="E482" s="3">
-        <v>7</v>
-      </c>
-      <c r="F482" s="3">
-        <v>11</v>
-      </c>
-      <c r="G482" s="3">
-        <v>12</v>
-      </c>
-      <c r="H482" s="3">
-        <v>14</v>
-      </c>
-      <c r="I482" s="3">
-        <v>15</v>
-      </c>
-      <c r="J482" s="3">
-        <v>16</v>
-      </c>
-      <c r="K482" s="3">
-        <v>17</v>
-      </c>
-      <c r="L482" s="3">
-        <v>18</v>
-      </c>
-      <c r="M482" s="3">
-        <v>20</v>
-      </c>
-      <c r="N482" s="3">
-        <v>21</v>
-      </c>
-      <c r="O482" s="3">
-        <v>23</v>
-      </c>
-      <c r="P482" s="3">
+      <c r="B482">
+        <v>4</v>
+      </c>
+      <c r="C482">
+        <v>5</v>
+      </c>
+      <c r="D482">
+        <v>6</v>
+      </c>
+      <c r="E482">
+        <v>7</v>
+      </c>
+      <c r="F482">
+        <v>11</v>
+      </c>
+      <c r="G482">
+        <v>12</v>
+      </c>
+      <c r="H482">
+        <v>14</v>
+      </c>
+      <c r="I482">
+        <v>15</v>
+      </c>
+      <c r="J482">
+        <v>16</v>
+      </c>
+      <c r="K482">
+        <v>17</v>
+      </c>
+      <c r="L482">
+        <v>18</v>
+      </c>
+      <c r="M482">
+        <v>20</v>
+      </c>
+      <c r="N482">
+        <v>21</v>
+      </c>
+      <c r="O482">
+        <v>23</v>
+      </c>
+      <c r="P482">
         <v>25</v>
       </c>
     </row>
     <row r="483" spans="1:16" x14ac:dyDescent="0.4">
-      <c r="A483" s="2">
+      <c r="A483">
         <v>3553</v>
       </c>
-      <c r="B483" s="3">
-        <v>1</v>
-      </c>
-      <c r="C483" s="3">
-        <v>2</v>
-      </c>
-      <c r="D483" s="3">
-        <v>3</v>
-      </c>
-      <c r="E483" s="3">
-        <v>7</v>
-      </c>
-      <c r="F483" s="3">
-        <v>8</v>
-      </c>
-      <c r="G483" s="3">
-        <v>9</v>
-      </c>
-      <c r="H483" s="3">
-        <v>12</v>
-      </c>
-      <c r="I483" s="3">
-        <v>13</v>
-      </c>
-      <c r="J483" s="3">
-        <v>16</v>
-      </c>
-      <c r="K483" s="3">
-        <v>17</v>
-      </c>
-      <c r="L483" s="3">
-        <v>19</v>
-      </c>
-      <c r="M483" s="3">
-        <v>21</v>
-      </c>
-      <c r="N483" s="3">
-        <v>22</v>
-      </c>
-      <c r="O483" s="3">
-        <v>23</v>
-      </c>
-      <c r="P483" s="3">
+      <c r="B483">
+        <v>1</v>
+      </c>
+      <c r="C483">
+        <v>2</v>
+      </c>
+      <c r="D483">
+        <v>3</v>
+      </c>
+      <c r="E483">
+        <v>7</v>
+      </c>
+      <c r="F483">
+        <v>8</v>
+      </c>
+      <c r="G483">
+        <v>9</v>
+      </c>
+      <c r="H483">
+        <v>12</v>
+      </c>
+      <c r="I483">
+        <v>13</v>
+      </c>
+      <c r="J483">
+        <v>16</v>
+      </c>
+      <c r="K483">
+        <v>17</v>
+      </c>
+      <c r="L483">
+        <v>19</v>
+      </c>
+      <c r="M483">
+        <v>21</v>
+      </c>
+      <c r="N483">
+        <v>22</v>
+      </c>
+      <c r="O483">
+        <v>23</v>
+      </c>
+      <c r="P483">
         <v>24</v>
       </c>
     </row>
     <row r="484" spans="1:16" x14ac:dyDescent="0.4">
-      <c r="A484" s="2">
+      <c r="A484">
         <v>3554</v>
       </c>
-      <c r="B484" s="3">
-        <v>1</v>
-      </c>
-      <c r="C484" s="3">
-        <v>3</v>
-      </c>
-      <c r="D484" s="3">
-        <v>4</v>
-      </c>
-      <c r="E484" s="3">
-        <v>5</v>
-      </c>
-      <c r="F484" s="3">
-        <v>8</v>
-      </c>
-      <c r="G484" s="3">
-        <v>9</v>
-      </c>
-      <c r="H484" s="3">
-        <v>11</v>
-      </c>
-      <c r="I484" s="3">
-        <v>12</v>
-      </c>
-      <c r="J484" s="3">
-        <v>14</v>
-      </c>
-      <c r="K484" s="3">
-        <v>15</v>
-      </c>
-      <c r="L484" s="3">
-        <v>16</v>
-      </c>
-      <c r="M484" s="3">
-        <v>18</v>
-      </c>
-      <c r="N484" s="3">
-        <v>22</v>
-      </c>
-      <c r="O484" s="3">
-        <v>23</v>
-      </c>
-      <c r="P484" s="3">
+      <c r="B484">
+        <v>1</v>
+      </c>
+      <c r="C484">
+        <v>3</v>
+      </c>
+      <c r="D484">
+        <v>4</v>
+      </c>
+      <c r="E484">
+        <v>5</v>
+      </c>
+      <c r="F484">
+        <v>8</v>
+      </c>
+      <c r="G484">
+        <v>9</v>
+      </c>
+      <c r="H484">
+        <v>11</v>
+      </c>
+      <c r="I484">
+        <v>12</v>
+      </c>
+      <c r="J484">
+        <v>14</v>
+      </c>
+      <c r="K484">
+        <v>15</v>
+      </c>
+      <c r="L484">
+        <v>16</v>
+      </c>
+      <c r="M484">
+        <v>18</v>
+      </c>
+      <c r="N484">
+        <v>22</v>
+      </c>
+      <c r="O484">
+        <v>23</v>
+      </c>
+      <c r="P484">
         <v>25</v>
       </c>
     </row>
     <row r="485" spans="1:16" x14ac:dyDescent="0.4">
-      <c r="A485" s="2">
+      <c r="A485">
         <v>3555</v>
       </c>
-      <c r="B485" s="3">
-        <v>1</v>
-      </c>
-      <c r="C485" s="3">
-        <v>2</v>
-      </c>
-      <c r="D485" s="3">
-        <v>3</v>
-      </c>
-      <c r="E485" s="3">
-        <v>4</v>
-      </c>
-      <c r="F485" s="3">
-        <v>7</v>
-      </c>
-      <c r="G485" s="3">
-        <v>8</v>
-      </c>
-      <c r="H485" s="3">
-        <v>10</v>
-      </c>
-      <c r="I485" s="3">
-        <v>13</v>
-      </c>
-      <c r="J485" s="3">
-        <v>14</v>
-      </c>
-      <c r="K485" s="3">
-        <v>15</v>
-      </c>
-      <c r="L485" s="3">
-        <v>18</v>
-      </c>
-      <c r="M485" s="3">
-        <v>19</v>
-      </c>
-      <c r="N485" s="3">
-        <v>20</v>
-      </c>
-      <c r="O485" s="3">
-        <v>23</v>
-      </c>
-      <c r="P485" s="3">
+      <c r="B485">
+        <v>1</v>
+      </c>
+      <c r="C485">
+        <v>2</v>
+      </c>
+      <c r="D485">
+        <v>3</v>
+      </c>
+      <c r="E485">
+        <v>4</v>
+      </c>
+      <c r="F485">
+        <v>7</v>
+      </c>
+      <c r="G485">
+        <v>8</v>
+      </c>
+      <c r="H485">
+        <v>10</v>
+      </c>
+      <c r="I485">
+        <v>13</v>
+      </c>
+      <c r="J485">
+        <v>14</v>
+      </c>
+      <c r="K485">
+        <v>15</v>
+      </c>
+      <c r="L485">
+        <v>18</v>
+      </c>
+      <c r="M485">
+        <v>19</v>
+      </c>
+      <c r="N485">
+        <v>20</v>
+      </c>
+      <c r="O485">
+        <v>23</v>
+      </c>
+      <c r="P485">
         <v>24</v>
       </c>
     </row>
     <row r="486" spans="1:16" x14ac:dyDescent="0.4">
-      <c r="A486" s="2">
+      <c r="A486">
         <v>3556</v>
       </c>
-      <c r="B486" s="3">
-        <v>1</v>
-      </c>
-      <c r="C486" s="3">
-        <v>2</v>
-      </c>
-      <c r="D486" s="3">
-        <v>3</v>
-      </c>
-      <c r="E486" s="3">
-        <v>4</v>
-      </c>
-      <c r="F486" s="3">
-        <v>5</v>
-      </c>
-      <c r="G486" s="3">
-        <v>7</v>
-      </c>
-      <c r="H486" s="3">
-        <v>9</v>
-      </c>
-      <c r="I486" s="3">
-        <v>10</v>
-      </c>
-      <c r="J486" s="3">
-        <v>12</v>
-      </c>
-      <c r="K486" s="3">
-        <v>14</v>
-      </c>
-      <c r="L486" s="3">
-        <v>16</v>
-      </c>
-      <c r="M486" s="3">
-        <v>17</v>
-      </c>
-      <c r="N486" s="3">
-        <v>19</v>
-      </c>
-      <c r="O486" s="3">
-        <v>21</v>
-      </c>
-      <c r="P486" s="3">
+      <c r="B486">
+        <v>1</v>
+      </c>
+      <c r="C486">
+        <v>2</v>
+      </c>
+      <c r="D486">
+        <v>3</v>
+      </c>
+      <c r="E486">
+        <v>4</v>
+      </c>
+      <c r="F486">
+        <v>5</v>
+      </c>
+      <c r="G486">
+        <v>7</v>
+      </c>
+      <c r="H486">
+        <v>9</v>
+      </c>
+      <c r="I486">
+        <v>10</v>
+      </c>
+      <c r="J486">
+        <v>12</v>
+      </c>
+      <c r="K486">
+        <v>14</v>
+      </c>
+      <c r="L486">
+        <v>16</v>
+      </c>
+      <c r="M486">
+        <v>17</v>
+      </c>
+      <c r="N486">
+        <v>19</v>
+      </c>
+      <c r="O486">
+        <v>21</v>
+      </c>
+      <c r="P486">
         <v>23</v>
       </c>
     </row>
     <row r="487" spans="1:16" x14ac:dyDescent="0.4">
-      <c r="A487" s="2">
+      <c r="A487">
         <v>3557</v>
       </c>
-      <c r="B487" s="3">
-        <v>5</v>
-      </c>
-      <c r="C487" s="3">
-        <v>6</v>
-      </c>
-      <c r="D487" s="3">
-        <v>7</v>
-      </c>
-      <c r="E487" s="3">
-        <v>9</v>
-      </c>
-      <c r="F487" s="3">
-        <v>10</v>
-      </c>
-      <c r="G487" s="3">
-        <v>13</v>
-      </c>
-      <c r="H487" s="3">
-        <v>14</v>
-      </c>
-      <c r="I487" s="3">
-        <v>15</v>
-      </c>
-      <c r="J487" s="3">
-        <v>16</v>
-      </c>
-      <c r="K487" s="3">
-        <v>17</v>
-      </c>
-      <c r="L487" s="3">
-        <v>19</v>
-      </c>
-      <c r="M487" s="3">
-        <v>20</v>
-      </c>
-      <c r="N487" s="3">
-        <v>21</v>
-      </c>
-      <c r="O487" s="3">
-        <v>22</v>
-      </c>
-      <c r="P487" s="3">
+      <c r="B487">
+        <v>5</v>
+      </c>
+      <c r="C487">
+        <v>6</v>
+      </c>
+      <c r="D487">
+        <v>7</v>
+      </c>
+      <c r="E487">
+        <v>9</v>
+      </c>
+      <c r="F487">
+        <v>10</v>
+      </c>
+      <c r="G487">
+        <v>13</v>
+      </c>
+      <c r="H487">
+        <v>14</v>
+      </c>
+      <c r="I487">
+        <v>15</v>
+      </c>
+      <c r="J487">
+        <v>16</v>
+      </c>
+      <c r="K487">
+        <v>17</v>
+      </c>
+      <c r="L487">
+        <v>19</v>
+      </c>
+      <c r="M487">
+        <v>20</v>
+      </c>
+      <c r="N487">
+        <v>21</v>
+      </c>
+      <c r="O487">
+        <v>22</v>
+      </c>
+      <c r="P487">
         <v>24</v>
       </c>
     </row>
     <row r="488" spans="1:16" x14ac:dyDescent="0.4">
-      <c r="A488" s="2">
+      <c r="A488">
         <v>3558</v>
       </c>
-      <c r="B488" s="3">
-        <v>2</v>
-      </c>
-      <c r="C488" s="3">
-        <v>3</v>
-      </c>
-      <c r="D488" s="3">
-        <v>4</v>
-      </c>
-      <c r="E488" s="3">
-        <v>7</v>
-      </c>
-      <c r="F488" s="3">
-        <v>9</v>
-      </c>
-      <c r="G488" s="3">
-        <v>12</v>
-      </c>
-      <c r="H488" s="3">
-        <v>13</v>
-      </c>
-      <c r="I488" s="3">
-        <v>14</v>
-      </c>
-      <c r="J488" s="3">
-        <v>15</v>
-      </c>
-      <c r="K488" s="3">
-        <v>18</v>
-      </c>
-      <c r="L488" s="3">
-        <v>20</v>
-      </c>
-      <c r="M488" s="3">
-        <v>22</v>
-      </c>
-      <c r="N488" s="3">
-        <v>23</v>
-      </c>
-      <c r="O488" s="3">
-        <v>24</v>
-      </c>
-      <c r="P488" s="3">
+      <c r="B488">
+        <v>2</v>
+      </c>
+      <c r="C488">
+        <v>3</v>
+      </c>
+      <c r="D488">
+        <v>4</v>
+      </c>
+      <c r="E488">
+        <v>7</v>
+      </c>
+      <c r="F488">
+        <v>9</v>
+      </c>
+      <c r="G488">
+        <v>12</v>
+      </c>
+      <c r="H488">
+        <v>13</v>
+      </c>
+      <c r="I488">
+        <v>14</v>
+      </c>
+      <c r="J488">
+        <v>15</v>
+      </c>
+      <c r="K488">
+        <v>18</v>
+      </c>
+      <c r="L488">
+        <v>20</v>
+      </c>
+      <c r="M488">
+        <v>22</v>
+      </c>
+      <c r="N488">
+        <v>23</v>
+      </c>
+      <c r="O488">
+        <v>24</v>
+      </c>
+      <c r="P488">
         <v>25</v>
       </c>
     </row>
     <row r="489" spans="1:16" x14ac:dyDescent="0.4">
-      <c r="A489" s="2">
+      <c r="A489">
         <v>3559</v>
       </c>
-      <c r="B489" s="3">
-        <v>1</v>
-      </c>
-      <c r="C489" s="3">
-        <v>2</v>
-      </c>
-      <c r="D489" s="3">
-        <v>6</v>
-      </c>
-      <c r="E489" s="3">
-        <v>8</v>
-      </c>
-      <c r="F489" s="3">
-        <v>9</v>
-      </c>
-      <c r="G489" s="3">
-        <v>10</v>
-      </c>
-      <c r="H489" s="3">
-        <v>11</v>
-      </c>
-      <c r="I489" s="3">
-        <v>13</v>
-      </c>
-      <c r="J489" s="3">
-        <v>14</v>
-      </c>
-      <c r="K489" s="3">
-        <v>15</v>
-      </c>
-      <c r="L489" s="3">
-        <v>16</v>
-      </c>
-      <c r="M489" s="3">
-        <v>19</v>
-      </c>
-      <c r="N489" s="3">
-        <v>20</v>
-      </c>
-      <c r="O489" s="3">
-        <v>24</v>
-      </c>
-      <c r="P489" s="3">
+      <c r="B489">
+        <v>1</v>
+      </c>
+      <c r="C489">
+        <v>2</v>
+      </c>
+      <c r="D489">
+        <v>6</v>
+      </c>
+      <c r="E489">
+        <v>8</v>
+      </c>
+      <c r="F489">
+        <v>9</v>
+      </c>
+      <c r="G489">
+        <v>10</v>
+      </c>
+      <c r="H489">
+        <v>11</v>
+      </c>
+      <c r="I489">
+        <v>13</v>
+      </c>
+      <c r="J489">
+        <v>14</v>
+      </c>
+      <c r="K489">
+        <v>15</v>
+      </c>
+      <c r="L489">
+        <v>16</v>
+      </c>
+      <c r="M489">
+        <v>19</v>
+      </c>
+      <c r="N489">
+        <v>20</v>
+      </c>
+      <c r="O489">
+        <v>24</v>
+      </c>
+      <c r="P489">
         <v>25</v>
       </c>
     </row>
     <row r="490" spans="1:16" x14ac:dyDescent="0.4">
-      <c r="A490" s="2">
+      <c r="A490">
         <v>3560</v>
       </c>
-      <c r="B490" s="3">
-        <v>1</v>
-      </c>
-      <c r="C490" s="3">
-        <v>3</v>
-      </c>
-      <c r="D490" s="3">
-        <v>4</v>
-      </c>
-      <c r="E490" s="3">
-        <v>6</v>
-      </c>
-      <c r="F490" s="3">
-        <v>7</v>
-      </c>
-      <c r="G490" s="3">
-        <v>8</v>
-      </c>
-      <c r="H490" s="3">
-        <v>10</v>
-      </c>
-      <c r="I490" s="3">
-        <v>11</v>
-      </c>
-      <c r="J490" s="3">
-        <v>12</v>
-      </c>
-      <c r="K490" s="3">
-        <v>13</v>
-      </c>
-      <c r="L490" s="3">
-        <v>17</v>
-      </c>
-      <c r="M490" s="3">
-        <v>18</v>
-      </c>
-      <c r="N490" s="3">
-        <v>19</v>
-      </c>
-      <c r="O490" s="3">
-        <v>23</v>
-      </c>
-      <c r="P490" s="3">
+      <c r="B490">
+        <v>1</v>
+      </c>
+      <c r="C490">
+        <v>3</v>
+      </c>
+      <c r="D490">
+        <v>4</v>
+      </c>
+      <c r="E490">
+        <v>6</v>
+      </c>
+      <c r="F490">
+        <v>7</v>
+      </c>
+      <c r="G490">
+        <v>8</v>
+      </c>
+      <c r="H490">
+        <v>10</v>
+      </c>
+      <c r="I490">
+        <v>11</v>
+      </c>
+      <c r="J490">
+        <v>12</v>
+      </c>
+      <c r="K490">
+        <v>13</v>
+      </c>
+      <c r="L490">
+        <v>17</v>
+      </c>
+      <c r="M490">
+        <v>18</v>
+      </c>
+      <c r="N490">
+        <v>19</v>
+      </c>
+      <c r="O490">
+        <v>23</v>
+      </c>
+      <c r="P490">
         <v>24</v>
       </c>
     </row>
     <row r="491" spans="1:16" x14ac:dyDescent="0.4">
-      <c r="A491" s="2">
+      <c r="A491">
         <v>3561</v>
       </c>
-      <c r="B491" s="3">
-        <v>1</v>
-      </c>
-      <c r="C491" s="3">
-        <v>2</v>
-      </c>
-      <c r="D491" s="3">
-        <v>4</v>
-      </c>
-      <c r="E491" s="3">
-        <v>5</v>
-      </c>
-      <c r="F491" s="3">
-        <v>6</v>
-      </c>
-      <c r="G491" s="3">
-        <v>7</v>
-      </c>
-      <c r="H491" s="3">
-        <v>8</v>
-      </c>
-      <c r="I491" s="3">
-        <v>10</v>
-      </c>
-      <c r="J491" s="3">
-        <v>15</v>
-      </c>
-      <c r="K491" s="3">
-        <v>16</v>
-      </c>
-      <c r="L491" s="3">
-        <v>17</v>
-      </c>
-      <c r="M491" s="3">
-        <v>18</v>
-      </c>
-      <c r="N491" s="3">
-        <v>20</v>
-      </c>
-      <c r="O491" s="3">
-        <v>21</v>
-      </c>
-      <c r="P491" s="3">
+      <c r="B491">
+        <v>1</v>
+      </c>
+      <c r="C491">
+        <v>2</v>
+      </c>
+      <c r="D491">
+        <v>4</v>
+      </c>
+      <c r="E491">
+        <v>5</v>
+      </c>
+      <c r="F491">
+        <v>6</v>
+      </c>
+      <c r="G491">
+        <v>7</v>
+      </c>
+      <c r="H491">
+        <v>8</v>
+      </c>
+      <c r="I491">
+        <v>10</v>
+      </c>
+      <c r="J491">
+        <v>15</v>
+      </c>
+      <c r="K491">
+        <v>16</v>
+      </c>
+      <c r="L491">
+        <v>17</v>
+      </c>
+      <c r="M491">
+        <v>18</v>
+      </c>
+      <c r="N491">
+        <v>20</v>
+      </c>
+      <c r="O491">
+        <v>21</v>
+      </c>
+      <c r="P491">
         <v>25</v>
       </c>
     </row>
     <row r="492" spans="1:16" x14ac:dyDescent="0.4">
-      <c r="A492" s="2">
+      <c r="A492">
         <v>3562</v>
       </c>
-      <c r="B492" s="3">
-        <v>3</v>
-      </c>
-      <c r="C492" s="3">
-        <v>5</v>
-      </c>
-      <c r="D492" s="3">
-        <v>6</v>
-      </c>
-      <c r="E492" s="3">
-        <v>7</v>
-      </c>
-      <c r="F492" s="3">
-        <v>9</v>
-      </c>
-      <c r="G492" s="3">
-        <v>10</v>
-      </c>
-      <c r="H492" s="3">
-        <v>11</v>
-      </c>
-      <c r="I492" s="3">
-        <v>12</v>
-      </c>
-      <c r="J492" s="3">
-        <v>13</v>
-      </c>
-      <c r="K492" s="3">
-        <v>14</v>
-      </c>
-      <c r="L492" s="3">
-        <v>15</v>
-      </c>
-      <c r="M492" s="3">
-        <v>19</v>
-      </c>
-      <c r="N492" s="3">
-        <v>22</v>
-      </c>
-      <c r="O492" s="3">
-        <v>23</v>
-      </c>
-      <c r="P492" s="3">
+      <c r="B492">
+        <v>3</v>
+      </c>
+      <c r="C492">
+        <v>5</v>
+      </c>
+      <c r="D492">
+        <v>6</v>
+      </c>
+      <c r="E492">
+        <v>7</v>
+      </c>
+      <c r="F492">
+        <v>9</v>
+      </c>
+      <c r="G492">
+        <v>10</v>
+      </c>
+      <c r="H492">
+        <v>11</v>
+      </c>
+      <c r="I492">
+        <v>12</v>
+      </c>
+      <c r="J492">
+        <v>13</v>
+      </c>
+      <c r="K492">
+        <v>14</v>
+      </c>
+      <c r="L492">
+        <v>15</v>
+      </c>
+      <c r="M492">
+        <v>19</v>
+      </c>
+      <c r="N492">
+        <v>22</v>
+      </c>
+      <c r="O492">
+        <v>23</v>
+      </c>
+      <c r="P492">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="493" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A493" s="2">
+        <v>3563</v>
+      </c>
+      <c r="B493" s="3">
+        <v>1</v>
+      </c>
+      <c r="C493" s="3">
+        <v>3</v>
+      </c>
+      <c r="D493" s="3">
+        <v>4</v>
+      </c>
+      <c r="E493" s="3">
+        <v>9</v>
+      </c>
+      <c r="F493" s="3">
+        <v>10</v>
+      </c>
+      <c r="G493" s="3">
+        <v>11</v>
+      </c>
+      <c r="H493" s="3">
+        <v>12</v>
+      </c>
+      <c r="I493" s="3">
+        <v>13</v>
+      </c>
+      <c r="J493" s="3">
+        <v>15</v>
+      </c>
+      <c r="K493" s="3">
+        <v>17</v>
+      </c>
+      <c r="L493" s="3">
+        <v>19</v>
+      </c>
+      <c r="M493" s="3">
+        <v>20</v>
+      </c>
+      <c r="N493" s="3">
+        <v>21</v>
+      </c>
+      <c r="O493" s="3">
+        <v>23</v>
+      </c>
+      <c r="P493" s="3">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="494" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A494" s="2">
+        <v>3564</v>
+      </c>
+      <c r="B494" s="3">
+        <v>5</v>
+      </c>
+      <c r="C494" s="3">
+        <v>6</v>
+      </c>
+      <c r="D494" s="3">
+        <v>7</v>
+      </c>
+      <c r="E494" s="3">
+        <v>8</v>
+      </c>
+      <c r="F494" s="3">
+        <v>9</v>
+      </c>
+      <c r="G494" s="3">
+        <v>11</v>
+      </c>
+      <c r="H494" s="3">
+        <v>12</v>
+      </c>
+      <c r="I494" s="3">
+        <v>13</v>
+      </c>
+      <c r="J494" s="3">
+        <v>14</v>
+      </c>
+      <c r="K494" s="3">
+        <v>19</v>
+      </c>
+      <c r="L494" s="3">
+        <v>20</v>
+      </c>
+      <c r="M494" s="3">
+        <v>21</v>
+      </c>
+      <c r="N494" s="3">
+        <v>23</v>
+      </c>
+      <c r="O494" s="3">
+        <v>24</v>
+      </c>
+      <c r="P494" s="3">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="495" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A495" s="2">
+        <v>3565</v>
+      </c>
+      <c r="B495" s="3">
+        <v>1</v>
+      </c>
+      <c r="C495" s="3">
+        <v>4</v>
+      </c>
+      <c r="D495" s="3">
+        <v>10</v>
+      </c>
+      <c r="E495" s="3">
+        <v>11</v>
+      </c>
+      <c r="F495" s="3">
+        <v>13</v>
+      </c>
+      <c r="G495" s="3">
+        <v>16</v>
+      </c>
+      <c r="H495" s="3">
+        <v>17</v>
+      </c>
+      <c r="I495" s="3">
+        <v>18</v>
+      </c>
+      <c r="J495" s="3">
+        <v>19</v>
+      </c>
+      <c r="K495" s="3">
+        <v>20</v>
+      </c>
+      <c r="L495" s="3">
+        <v>21</v>
+      </c>
+      <c r="M495" s="3">
+        <v>22</v>
+      </c>
+      <c r="N495" s="3">
+        <v>23</v>
+      </c>
+      <c r="O495" s="3">
+        <v>24</v>
+      </c>
+      <c r="P495" s="3">
         <v>25</v>
       </c>
     </row>
@@ -25078,6 +25228,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100C92CDE8829F3C7438DCCB0991C30EAAE" ma:contentTypeVersion="3" ma:contentTypeDescription="Crie um novo documento." ma:contentTypeScope="" ma:versionID="36cf41eecaf38ba1d849a0c8dd067090">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="3e38fcf2-aa96-4a2c-865b-c3abba01ba51" xmlns:ns3="4455b8ba-124f-46d5-aaaa-9813efd83d1e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="023f68b2d27389a617bf935a3f0e17ad" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -25245,15 +25404,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -25265,6 +25415,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{82B637BD-743B-452C-A85E-33AF8B93F052}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{46C5B8C5-4575-4105-836C-9C4A6674A14B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -25284,14 +25442,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{82B637BD-743B-452C-A85E-33AF8B93F052}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0328C38C-FE97-4791-8469-4B5D9CCC5D08}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
atualizandpo resultados das loterias ca caixa no site
</commit_message>
<xml_diff>
--- a/LoteriasExcel/Lotofacil_edt2.xlsx
+++ b/LoteriasExcel/Lotofacil_edt2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\Dropbox\! 000 ByPass\Pessoal\99_Loterias\0 - Loterias-Inteligentes\LoteriasExcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F52542F-5276-4D6C-A11F-E4F8502F2D67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5981D75F-1BC3-46E7-ACE0-9A478883A65E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="58260" yWindow="660" windowWidth="19545" windowHeight="12000" tabRatio="876" xr2:uid="{2663372B-AA50-4721-AD6B-5F0B8186ACF5}"/>
+    <workbookView xWindow="74385" yWindow="225" windowWidth="20535" windowHeight="8940" tabRatio="876" xr2:uid="{2663372B-AA50-4721-AD6B-5F0B8186ACF5}"/>
   </bookViews>
   <sheets>
     <sheet name="LOTOFÁCIL" sheetId="3" r:id="rId1"/>
@@ -457,11 +457,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69BEFC42-DD13-4DE0-B2AD-D0F44AF8189C}">
-  <dimension ref="A1:P495"/>
+  <dimension ref="A1:P498"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A475" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B493" sqref="B493:P495"/>
+      <pane ySplit="1" topLeftCell="A484" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B496" sqref="B496:P498"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -25073,153 +25073,303 @@
       </c>
     </row>
     <row r="493" spans="1:16" x14ac:dyDescent="0.4">
-      <c r="A493" s="2">
+      <c r="A493">
         <v>3563</v>
       </c>
-      <c r="B493" s="3">
-        <v>1</v>
-      </c>
-      <c r="C493" s="3">
-        <v>3</v>
-      </c>
-      <c r="D493" s="3">
-        <v>4</v>
-      </c>
-      <c r="E493" s="3">
-        <v>9</v>
-      </c>
-      <c r="F493" s="3">
-        <v>10</v>
-      </c>
-      <c r="G493" s="3">
-        <v>11</v>
-      </c>
-      <c r="H493" s="3">
-        <v>12</v>
-      </c>
-      <c r="I493" s="3">
-        <v>13</v>
-      </c>
-      <c r="J493" s="3">
-        <v>15</v>
-      </c>
-      <c r="K493" s="3">
-        <v>17</v>
-      </c>
-      <c r="L493" s="3">
-        <v>19</v>
-      </c>
-      <c r="M493" s="3">
-        <v>20</v>
-      </c>
-      <c r="N493" s="3">
-        <v>21</v>
-      </c>
-      <c r="O493" s="3">
-        <v>23</v>
-      </c>
-      <c r="P493" s="3">
+      <c r="B493">
+        <v>1</v>
+      </c>
+      <c r="C493">
+        <v>3</v>
+      </c>
+      <c r="D493">
+        <v>4</v>
+      </c>
+      <c r="E493">
+        <v>9</v>
+      </c>
+      <c r="F493">
+        <v>10</v>
+      </c>
+      <c r="G493">
+        <v>11</v>
+      </c>
+      <c r="H493">
+        <v>12</v>
+      </c>
+      <c r="I493">
+        <v>13</v>
+      </c>
+      <c r="J493">
+        <v>15</v>
+      </c>
+      <c r="K493">
+        <v>17</v>
+      </c>
+      <c r="L493">
+        <v>19</v>
+      </c>
+      <c r="M493">
+        <v>20</v>
+      </c>
+      <c r="N493">
+        <v>21</v>
+      </c>
+      <c r="O493">
+        <v>23</v>
+      </c>
+      <c r="P493">
         <v>25</v>
       </c>
     </row>
     <row r="494" spans="1:16" x14ac:dyDescent="0.4">
-      <c r="A494" s="2">
+      <c r="A494">
         <v>3564</v>
       </c>
-      <c r="B494" s="3">
-        <v>5</v>
-      </c>
-      <c r="C494" s="3">
-        <v>6</v>
-      </c>
-      <c r="D494" s="3">
-        <v>7</v>
-      </c>
-      <c r="E494" s="3">
-        <v>8</v>
-      </c>
-      <c r="F494" s="3">
-        <v>9</v>
-      </c>
-      <c r="G494" s="3">
-        <v>11</v>
-      </c>
-      <c r="H494" s="3">
-        <v>12</v>
-      </c>
-      <c r="I494" s="3">
-        <v>13</v>
-      </c>
-      <c r="J494" s="3">
-        <v>14</v>
-      </c>
-      <c r="K494" s="3">
-        <v>19</v>
-      </c>
-      <c r="L494" s="3">
-        <v>20</v>
-      </c>
-      <c r="M494" s="3">
-        <v>21</v>
-      </c>
-      <c r="N494" s="3">
-        <v>23</v>
-      </c>
-      <c r="O494" s="3">
-        <v>24</v>
-      </c>
-      <c r="P494" s="3">
+      <c r="B494">
+        <v>5</v>
+      </c>
+      <c r="C494">
+        <v>6</v>
+      </c>
+      <c r="D494">
+        <v>7</v>
+      </c>
+      <c r="E494">
+        <v>8</v>
+      </c>
+      <c r="F494">
+        <v>9</v>
+      </c>
+      <c r="G494">
+        <v>11</v>
+      </c>
+      <c r="H494">
+        <v>12</v>
+      </c>
+      <c r="I494">
+        <v>13</v>
+      </c>
+      <c r="J494">
+        <v>14</v>
+      </c>
+      <c r="K494">
+        <v>19</v>
+      </c>
+      <c r="L494">
+        <v>20</v>
+      </c>
+      <c r="M494">
+        <v>21</v>
+      </c>
+      <c r="N494">
+        <v>23</v>
+      </c>
+      <c r="O494">
+        <v>24</v>
+      </c>
+      <c r="P494">
         <v>25</v>
       </c>
     </row>
     <row r="495" spans="1:16" x14ac:dyDescent="0.4">
-      <c r="A495" s="2">
+      <c r="A495">
         <v>3565</v>
       </c>
-      <c r="B495" s="3">
-        <v>1</v>
-      </c>
-      <c r="C495" s="3">
-        <v>4</v>
-      </c>
-      <c r="D495" s="3">
-        <v>10</v>
-      </c>
-      <c r="E495" s="3">
-        <v>11</v>
-      </c>
-      <c r="F495" s="3">
-        <v>13</v>
-      </c>
-      <c r="G495" s="3">
-        <v>16</v>
-      </c>
-      <c r="H495" s="3">
-        <v>17</v>
-      </c>
-      <c r="I495" s="3">
-        <v>18</v>
-      </c>
-      <c r="J495" s="3">
-        <v>19</v>
-      </c>
-      <c r="K495" s="3">
-        <v>20</v>
-      </c>
-      <c r="L495" s="3">
-        <v>21</v>
-      </c>
-      <c r="M495" s="3">
-        <v>22</v>
-      </c>
-      <c r="N495" s="3">
-        <v>23</v>
-      </c>
-      <c r="O495" s="3">
-        <v>24</v>
-      </c>
-      <c r="P495" s="3">
-        <v>25</v>
+      <c r="B495">
+        <v>1</v>
+      </c>
+      <c r="C495">
+        <v>4</v>
+      </c>
+      <c r="D495">
+        <v>10</v>
+      </c>
+      <c r="E495">
+        <v>11</v>
+      </c>
+      <c r="F495">
+        <v>13</v>
+      </c>
+      <c r="G495">
+        <v>16</v>
+      </c>
+      <c r="H495">
+        <v>17</v>
+      </c>
+      <c r="I495">
+        <v>18</v>
+      </c>
+      <c r="J495">
+        <v>19</v>
+      </c>
+      <c r="K495">
+        <v>20</v>
+      </c>
+      <c r="L495">
+        <v>21</v>
+      </c>
+      <c r="M495">
+        <v>22</v>
+      </c>
+      <c r="N495">
+        <v>23</v>
+      </c>
+      <c r="O495">
+        <v>24</v>
+      </c>
+      <c r="P495">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="496" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A496" s="2">
+        <v>3566</v>
+      </c>
+      <c r="B496" s="3">
+        <v>1</v>
+      </c>
+      <c r="C496" s="3">
+        <v>2</v>
+      </c>
+      <c r="D496" s="3">
+        <v>4</v>
+      </c>
+      <c r="E496" s="3">
+        <v>7</v>
+      </c>
+      <c r="F496" s="3">
+        <v>8</v>
+      </c>
+      <c r="G496" s="3">
+        <v>12</v>
+      </c>
+      <c r="H496" s="3">
+        <v>13</v>
+      </c>
+      <c r="I496" s="3">
+        <v>14</v>
+      </c>
+      <c r="J496" s="3">
+        <v>15</v>
+      </c>
+      <c r="K496" s="3">
+        <v>17</v>
+      </c>
+      <c r="L496" s="3">
+        <v>20</v>
+      </c>
+      <c r="M496" s="3">
+        <v>21</v>
+      </c>
+      <c r="N496" s="3">
+        <v>22</v>
+      </c>
+      <c r="O496" s="3">
+        <v>23</v>
+      </c>
+      <c r="P496" s="3">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="497" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A497" s="2">
+        <v>3567</v>
+      </c>
+      <c r="B497" s="3">
+        <v>1</v>
+      </c>
+      <c r="C497" s="3">
+        <v>2</v>
+      </c>
+      <c r="D497" s="3">
+        <v>4</v>
+      </c>
+      <c r="E497" s="3">
+        <v>8</v>
+      </c>
+      <c r="F497" s="3">
+        <v>9</v>
+      </c>
+      <c r="G497" s="3">
+        <v>10</v>
+      </c>
+      <c r="H497" s="3">
+        <v>11</v>
+      </c>
+      <c r="I497" s="3">
+        <v>12</v>
+      </c>
+      <c r="J497" s="3">
+        <v>14</v>
+      </c>
+      <c r="K497" s="3">
+        <v>15</v>
+      </c>
+      <c r="L497" s="3">
+        <v>18</v>
+      </c>
+      <c r="M497" s="3">
+        <v>19</v>
+      </c>
+      <c r="N497" s="3">
+        <v>20</v>
+      </c>
+      <c r="O497" s="3">
+        <v>24</v>
+      </c>
+      <c r="P497" s="3">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="498" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A498" s="2">
+        <v>3568</v>
+      </c>
+      <c r="B498" s="3">
+        <v>1</v>
+      </c>
+      <c r="C498" s="3">
+        <v>2</v>
+      </c>
+      <c r="D498" s="3">
+        <v>4</v>
+      </c>
+      <c r="E498" s="3">
+        <v>5</v>
+      </c>
+      <c r="F498" s="3">
+        <v>6</v>
+      </c>
+      <c r="G498" s="3">
+        <v>7</v>
+      </c>
+      <c r="H498" s="3">
+        <v>8</v>
+      </c>
+      <c r="I498" s="3">
+        <v>10</v>
+      </c>
+      <c r="J498" s="3">
+        <v>11</v>
+      </c>
+      <c r="K498" s="3">
+        <v>13</v>
+      </c>
+      <c r="L498" s="3">
+        <v>18</v>
+      </c>
+      <c r="M498" s="3">
+        <v>19</v>
+      </c>
+      <c r="N498" s="3">
+        <v>20</v>
+      </c>
+      <c r="O498" s="3">
+        <v>22</v>
+      </c>
+      <c r="P498" s="3">
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -25228,15 +25378,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100C92CDE8829F3C7438DCCB0991C30EAAE" ma:contentTypeVersion="3" ma:contentTypeDescription="Crie um novo documento." ma:contentTypeScope="" ma:versionID="36cf41eecaf38ba1d849a0c8dd067090">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="3e38fcf2-aa96-4a2c-865b-c3abba01ba51" xmlns:ns3="4455b8ba-124f-46d5-aaaa-9813efd83d1e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="023f68b2d27389a617bf935a3f0e17ad" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -25404,6 +25545,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -25415,14 +25565,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{82B637BD-743B-452C-A85E-33AF8B93F052}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{46C5B8C5-4575-4105-836C-9C4A6674A14B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -25442,6 +25584,14 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{82B637BD-743B-452C-A85E-33AF8B93F052}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0328C38C-FE97-4791-8469-4B5D9CCC5D08}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Atualiza planilhas com concursos mais recentes
</commit_message>
<xml_diff>
--- a/LoteriasExcel/Lotofacil_edt2.xlsx
+++ b/LoteriasExcel/Lotofacil_edt2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\Dropbox\! 000 ByPass\Pessoal\99_Loterias\0 - Loterias-Inteligentes\LoteriasExcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5981D75F-1BC3-46E7-ACE0-9A478883A65E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D423847F-26AC-4F36-9199-BF2B07F3448D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="74385" yWindow="225" windowWidth="20535" windowHeight="8940" tabRatio="876" xr2:uid="{2663372B-AA50-4721-AD6B-5F0B8186ACF5}"/>
+    <workbookView xWindow="57525" yWindow="1380" windowWidth="19740" windowHeight="16020" tabRatio="876" xr2:uid="{2663372B-AA50-4721-AD6B-5F0B8186ACF5}"/>
   </bookViews>
   <sheets>
     <sheet name="LOTOFÁCIL" sheetId="3" r:id="rId1"/>
@@ -104,7 +104,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -114,6 +114,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFA55592"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -130,13 +148,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -457,11 +478,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69BEFC42-DD13-4DE0-B2AD-D0F44AF8189C}">
-  <dimension ref="A1:P498"/>
+  <dimension ref="A1:P516"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A484" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B496" sqref="B496:P498"/>
+      <selection pane="bottomLeft" activeCell="H521" sqref="H521"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -25223,153 +25244,1053 @@
       </c>
     </row>
     <row r="496" spans="1:16" x14ac:dyDescent="0.4">
-      <c r="A496" s="2">
+      <c r="A496">
         <v>3566</v>
       </c>
-      <c r="B496" s="3">
-        <v>1</v>
-      </c>
-      <c r="C496" s="3">
-        <v>2</v>
-      </c>
-      <c r="D496" s="3">
-        <v>4</v>
-      </c>
-      <c r="E496" s="3">
-        <v>7</v>
-      </c>
-      <c r="F496" s="3">
-        <v>8</v>
-      </c>
-      <c r="G496" s="3">
-        <v>12</v>
-      </c>
-      <c r="H496" s="3">
-        <v>13</v>
-      </c>
-      <c r="I496" s="3">
-        <v>14</v>
-      </c>
-      <c r="J496" s="3">
-        <v>15</v>
-      </c>
-      <c r="K496" s="3">
-        <v>17</v>
-      </c>
-      <c r="L496" s="3">
-        <v>20</v>
-      </c>
-      <c r="M496" s="3">
-        <v>21</v>
-      </c>
-      <c r="N496" s="3">
-        <v>22</v>
-      </c>
-      <c r="O496" s="3">
-        <v>23</v>
-      </c>
-      <c r="P496" s="3">
+      <c r="B496">
+        <v>1</v>
+      </c>
+      <c r="C496">
+        <v>2</v>
+      </c>
+      <c r="D496">
+        <v>4</v>
+      </c>
+      <c r="E496">
+        <v>7</v>
+      </c>
+      <c r="F496">
+        <v>8</v>
+      </c>
+      <c r="G496">
+        <v>12</v>
+      </c>
+      <c r="H496">
+        <v>13</v>
+      </c>
+      <c r="I496">
+        <v>14</v>
+      </c>
+      <c r="J496">
+        <v>15</v>
+      </c>
+      <c r="K496">
+        <v>17</v>
+      </c>
+      <c r="L496">
+        <v>20</v>
+      </c>
+      <c r="M496">
+        <v>21</v>
+      </c>
+      <c r="N496">
+        <v>22</v>
+      </c>
+      <c r="O496">
+        <v>23</v>
+      </c>
+      <c r="P496">
         <v>24</v>
       </c>
     </row>
     <row r="497" spans="1:16" x14ac:dyDescent="0.4">
-      <c r="A497" s="2">
+      <c r="A497">
         <v>3567</v>
       </c>
-      <c r="B497" s="3">
-        <v>1</v>
-      </c>
-      <c r="C497" s="3">
-        <v>2</v>
-      </c>
-      <c r="D497" s="3">
-        <v>4</v>
-      </c>
-      <c r="E497" s="3">
-        <v>8</v>
-      </c>
-      <c r="F497" s="3">
-        <v>9</v>
-      </c>
-      <c r="G497" s="3">
-        <v>10</v>
-      </c>
-      <c r="H497" s="3">
-        <v>11</v>
-      </c>
-      <c r="I497" s="3">
-        <v>12</v>
-      </c>
-      <c r="J497" s="3">
-        <v>14</v>
-      </c>
-      <c r="K497" s="3">
-        <v>15</v>
-      </c>
-      <c r="L497" s="3">
-        <v>18</v>
-      </c>
-      <c r="M497" s="3">
-        <v>19</v>
-      </c>
-      <c r="N497" s="3">
-        <v>20</v>
-      </c>
-      <c r="O497" s="3">
-        <v>24</v>
-      </c>
-      <c r="P497" s="3">
+      <c r="B497">
+        <v>1</v>
+      </c>
+      <c r="C497">
+        <v>2</v>
+      </c>
+      <c r="D497">
+        <v>4</v>
+      </c>
+      <c r="E497">
+        <v>8</v>
+      </c>
+      <c r="F497">
+        <v>9</v>
+      </c>
+      <c r="G497">
+        <v>10</v>
+      </c>
+      <c r="H497">
+        <v>11</v>
+      </c>
+      <c r="I497">
+        <v>12</v>
+      </c>
+      <c r="J497">
+        <v>14</v>
+      </c>
+      <c r="K497">
+        <v>15</v>
+      </c>
+      <c r="L497">
+        <v>18</v>
+      </c>
+      <c r="M497">
+        <v>19</v>
+      </c>
+      <c r="N497">
+        <v>20</v>
+      </c>
+      <c r="O497">
+        <v>24</v>
+      </c>
+      <c r="P497">
         <v>25</v>
       </c>
     </row>
     <row r="498" spans="1:16" x14ac:dyDescent="0.4">
-      <c r="A498" s="2">
+      <c r="A498">
         <v>3568</v>
       </c>
-      <c r="B498" s="3">
-        <v>1</v>
-      </c>
-      <c r="C498" s="3">
-        <v>2</v>
-      </c>
-      <c r="D498" s="3">
-        <v>4</v>
-      </c>
-      <c r="E498" s="3">
-        <v>5</v>
-      </c>
-      <c r="F498" s="3">
-        <v>6</v>
-      </c>
-      <c r="G498" s="3">
-        <v>7</v>
-      </c>
-      <c r="H498" s="3">
-        <v>8</v>
-      </c>
-      <c r="I498" s="3">
-        <v>10</v>
-      </c>
-      <c r="J498" s="3">
-        <v>11</v>
-      </c>
-      <c r="K498" s="3">
-        <v>13</v>
-      </c>
-      <c r="L498" s="3">
-        <v>18</v>
-      </c>
-      <c r="M498" s="3">
-        <v>19</v>
-      </c>
-      <c r="N498" s="3">
-        <v>20</v>
-      </c>
-      <c r="O498" s="3">
-        <v>22</v>
-      </c>
-      <c r="P498" s="3">
-        <v>24</v>
+      <c r="B498" s="2">
+        <v>1</v>
+      </c>
+      <c r="C498" s="2">
+        <v>2</v>
+      </c>
+      <c r="D498" s="2">
+        <v>4</v>
+      </c>
+      <c r="E498" s="2">
+        <v>5</v>
+      </c>
+      <c r="F498" s="2">
+        <v>6</v>
+      </c>
+      <c r="G498" s="5">
+        <v>7</v>
+      </c>
+      <c r="H498" s="5">
+        <v>8</v>
+      </c>
+      <c r="I498" s="5">
+        <v>10</v>
+      </c>
+      <c r="J498" s="5">
+        <v>11</v>
+      </c>
+      <c r="K498" s="5">
+        <v>13</v>
+      </c>
+      <c r="L498" s="6">
+        <v>18</v>
+      </c>
+      <c r="M498" s="6">
+        <v>19</v>
+      </c>
+      <c r="N498" s="6">
+        <v>20</v>
+      </c>
+      <c r="O498" s="6">
+        <v>22</v>
+      </c>
+      <c r="P498" s="6">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="499" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A499" s="3">
+        <v>3569</v>
+      </c>
+      <c r="B499" s="4">
+        <v>1</v>
+      </c>
+      <c r="C499" s="4">
+        <v>2</v>
+      </c>
+      <c r="D499" s="4">
+        <v>3</v>
+      </c>
+      <c r="E499" s="4">
+        <v>4</v>
+      </c>
+      <c r="F499" s="4">
+        <v>5</v>
+      </c>
+      <c r="G499" s="4">
+        <v>6</v>
+      </c>
+      <c r="H499" s="4">
+        <v>8</v>
+      </c>
+      <c r="I499" s="4">
+        <v>10</v>
+      </c>
+      <c r="J499" s="4">
+        <v>14</v>
+      </c>
+      <c r="K499" s="4">
+        <v>15</v>
+      </c>
+      <c r="L499" s="4">
+        <v>17</v>
+      </c>
+      <c r="M499" s="4">
+        <v>18</v>
+      </c>
+      <c r="N499" s="4">
+        <v>19</v>
+      </c>
+      <c r="O499" s="4">
+        <v>20</v>
+      </c>
+      <c r="P499" s="4">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="500" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A500" s="3">
+        <v>3570</v>
+      </c>
+      <c r="B500" s="4">
+        <v>1</v>
+      </c>
+      <c r="C500" s="4">
+        <v>2</v>
+      </c>
+      <c r="D500" s="4">
+        <v>3</v>
+      </c>
+      <c r="E500" s="4">
+        <v>5</v>
+      </c>
+      <c r="F500" s="4">
+        <v>6</v>
+      </c>
+      <c r="G500" s="4">
+        <v>10</v>
+      </c>
+      <c r="H500" s="4">
+        <v>11</v>
+      </c>
+      <c r="I500" s="4">
+        <v>13</v>
+      </c>
+      <c r="J500" s="4">
+        <v>15</v>
+      </c>
+      <c r="K500" s="4">
+        <v>18</v>
+      </c>
+      <c r="L500" s="4">
+        <v>19</v>
+      </c>
+      <c r="M500" s="4">
+        <v>20</v>
+      </c>
+      <c r="N500" s="4">
+        <v>21</v>
+      </c>
+      <c r="O500" s="4">
+        <v>22</v>
+      </c>
+      <c r="P500" s="4">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="501" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A501" s="3">
+        <v>3571</v>
+      </c>
+      <c r="B501" s="4">
+        <v>2</v>
+      </c>
+      <c r="C501" s="4">
+        <v>3</v>
+      </c>
+      <c r="D501" s="4">
+        <v>4</v>
+      </c>
+      <c r="E501" s="4">
+        <v>5</v>
+      </c>
+      <c r="F501" s="4">
+        <v>6</v>
+      </c>
+      <c r="G501" s="4">
+        <v>8</v>
+      </c>
+      <c r="H501" s="4">
+        <v>11</v>
+      </c>
+      <c r="I501" s="4">
+        <v>12</v>
+      </c>
+      <c r="J501" s="4">
+        <v>13</v>
+      </c>
+      <c r="K501" s="4">
+        <v>14</v>
+      </c>
+      <c r="L501" s="4">
+        <v>17</v>
+      </c>
+      <c r="M501" s="4">
+        <v>20</v>
+      </c>
+      <c r="N501" s="4">
+        <v>22</v>
+      </c>
+      <c r="O501" s="4">
+        <v>24</v>
+      </c>
+      <c r="P501" s="4">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="502" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A502" s="3">
+        <v>3572</v>
+      </c>
+      <c r="B502" s="4">
+        <v>1</v>
+      </c>
+      <c r="C502" s="4">
+        <v>2</v>
+      </c>
+      <c r="D502" s="4">
+        <v>4</v>
+      </c>
+      <c r="E502" s="4">
+        <v>5</v>
+      </c>
+      <c r="F502" s="4">
+        <v>7</v>
+      </c>
+      <c r="G502" s="4">
+        <v>10</v>
+      </c>
+      <c r="H502" s="4">
+        <v>12</v>
+      </c>
+      <c r="I502" s="4">
+        <v>14</v>
+      </c>
+      <c r="J502" s="4">
+        <v>15</v>
+      </c>
+      <c r="K502" s="4">
+        <v>16</v>
+      </c>
+      <c r="L502" s="4">
+        <v>17</v>
+      </c>
+      <c r="M502" s="4">
+        <v>18</v>
+      </c>
+      <c r="N502" s="4">
+        <v>19</v>
+      </c>
+      <c r="O502" s="4">
+        <v>22</v>
+      </c>
+      <c r="P502" s="4">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="503" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A503" s="3">
+        <v>3573</v>
+      </c>
+      <c r="B503" s="4">
+        <v>1</v>
+      </c>
+      <c r="C503" s="4">
+        <v>2</v>
+      </c>
+      <c r="D503" s="4">
+        <v>7</v>
+      </c>
+      <c r="E503" s="4">
+        <v>8</v>
+      </c>
+      <c r="F503" s="4">
+        <v>10</v>
+      </c>
+      <c r="G503" s="4">
+        <v>11</v>
+      </c>
+      <c r="H503" s="4">
+        <v>12</v>
+      </c>
+      <c r="I503" s="4">
+        <v>14</v>
+      </c>
+      <c r="J503" s="4">
+        <v>15</v>
+      </c>
+      <c r="K503" s="4">
+        <v>16</v>
+      </c>
+      <c r="L503" s="4">
+        <v>17</v>
+      </c>
+      <c r="M503" s="4">
+        <v>20</v>
+      </c>
+      <c r="N503" s="4">
+        <v>22</v>
+      </c>
+      <c r="O503" s="4">
+        <v>23</v>
+      </c>
+      <c r="P503" s="4">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="504" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A504" s="3">
+        <v>3574</v>
+      </c>
+      <c r="B504" s="4">
+        <v>1</v>
+      </c>
+      <c r="C504" s="4">
+        <v>3</v>
+      </c>
+      <c r="D504" s="4">
+        <v>4</v>
+      </c>
+      <c r="E504" s="4">
+        <v>5</v>
+      </c>
+      <c r="F504" s="4">
+        <v>6</v>
+      </c>
+      <c r="G504" s="4">
+        <v>8</v>
+      </c>
+      <c r="H504" s="4">
+        <v>12</v>
+      </c>
+      <c r="I504" s="4">
+        <v>13</v>
+      </c>
+      <c r="J504" s="4">
+        <v>15</v>
+      </c>
+      <c r="K504" s="4">
+        <v>16</v>
+      </c>
+      <c r="L504" s="4">
+        <v>17</v>
+      </c>
+      <c r="M504" s="4">
+        <v>18</v>
+      </c>
+      <c r="N504" s="4">
+        <v>20</v>
+      </c>
+      <c r="O504" s="4">
+        <v>21</v>
+      </c>
+      <c r="P504" s="4">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="505" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A505" s="3">
+        <v>3575</v>
+      </c>
+      <c r="B505" s="4">
+        <v>2</v>
+      </c>
+      <c r="C505" s="4">
+        <v>4</v>
+      </c>
+      <c r="D505" s="4">
+        <v>5</v>
+      </c>
+      <c r="E505" s="4">
+        <v>7</v>
+      </c>
+      <c r="F505" s="4">
+        <v>8</v>
+      </c>
+      <c r="G505" s="4">
+        <v>9</v>
+      </c>
+      <c r="H505" s="4">
+        <v>10</v>
+      </c>
+      <c r="I505" s="4">
+        <v>12</v>
+      </c>
+      <c r="J505" s="4">
+        <v>13</v>
+      </c>
+      <c r="K505" s="4">
+        <v>14</v>
+      </c>
+      <c r="L505" s="4">
+        <v>15</v>
+      </c>
+      <c r="M505" s="4">
+        <v>17</v>
+      </c>
+      <c r="N505" s="4">
+        <v>21</v>
+      </c>
+      <c r="O505" s="4">
+        <v>22</v>
+      </c>
+      <c r="P505" s="4">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="506" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A506" s="3">
+        <v>3576</v>
+      </c>
+      <c r="B506" s="4">
+        <v>1</v>
+      </c>
+      <c r="C506" s="4">
+        <v>2</v>
+      </c>
+      <c r="D506" s="4">
+        <v>3</v>
+      </c>
+      <c r="E506" s="4">
+        <v>5</v>
+      </c>
+      <c r="F506" s="4">
+        <v>7</v>
+      </c>
+      <c r="G506" s="4">
+        <v>8</v>
+      </c>
+      <c r="H506" s="4">
+        <v>10</v>
+      </c>
+      <c r="I506" s="4">
+        <v>13</v>
+      </c>
+      <c r="J506" s="4">
+        <v>16</v>
+      </c>
+      <c r="K506" s="4">
+        <v>18</v>
+      </c>
+      <c r="L506" s="4">
+        <v>19</v>
+      </c>
+      <c r="M506" s="4">
+        <v>21</v>
+      </c>
+      <c r="N506" s="4">
+        <v>22</v>
+      </c>
+      <c r="O506" s="4">
+        <v>23</v>
+      </c>
+      <c r="P506" s="4">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="507" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A507" s="3">
+        <v>3577</v>
+      </c>
+      <c r="B507" s="4">
+        <v>1</v>
+      </c>
+      <c r="C507" s="4">
+        <v>2</v>
+      </c>
+      <c r="D507" s="4">
+        <v>4</v>
+      </c>
+      <c r="E507" s="4">
+        <v>5</v>
+      </c>
+      <c r="F507" s="4">
+        <v>6</v>
+      </c>
+      <c r="G507" s="4">
+        <v>8</v>
+      </c>
+      <c r="H507" s="4">
+        <v>9</v>
+      </c>
+      <c r="I507" s="4">
+        <v>10</v>
+      </c>
+      <c r="J507" s="4">
+        <v>12</v>
+      </c>
+      <c r="K507" s="4">
+        <v>16</v>
+      </c>
+      <c r="L507" s="4">
+        <v>18</v>
+      </c>
+      <c r="M507" s="4">
+        <v>20</v>
+      </c>
+      <c r="N507" s="4">
+        <v>23</v>
+      </c>
+      <c r="O507" s="4">
+        <v>24</v>
+      </c>
+      <c r="P507" s="4">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="508" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A508" s="3">
+        <v>3578</v>
+      </c>
+      <c r="B508" s="4">
+        <v>2</v>
+      </c>
+      <c r="C508" s="4">
+        <v>3</v>
+      </c>
+      <c r="D508" s="4">
+        <v>4</v>
+      </c>
+      <c r="E508" s="4">
+        <v>5</v>
+      </c>
+      <c r="F508" s="4">
+        <v>6</v>
+      </c>
+      <c r="G508" s="4">
+        <v>7</v>
+      </c>
+      <c r="H508" s="4">
+        <v>9</v>
+      </c>
+      <c r="I508" s="4">
+        <v>10</v>
+      </c>
+      <c r="J508" s="4">
+        <v>14</v>
+      </c>
+      <c r="K508" s="4">
+        <v>17</v>
+      </c>
+      <c r="L508" s="4">
+        <v>19</v>
+      </c>
+      <c r="M508" s="4">
+        <v>20</v>
+      </c>
+      <c r="N508" s="4">
+        <v>22</v>
+      </c>
+      <c r="O508" s="4">
+        <v>23</v>
+      </c>
+      <c r="P508" s="4">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="509" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A509" s="3">
+        <v>3579</v>
+      </c>
+      <c r="B509" s="4">
+        <v>1</v>
+      </c>
+      <c r="C509" s="4">
+        <v>2</v>
+      </c>
+      <c r="D509" s="4">
+        <v>3</v>
+      </c>
+      <c r="E509" s="4">
+        <v>4</v>
+      </c>
+      <c r="F509" s="4">
+        <v>8</v>
+      </c>
+      <c r="G509" s="4">
+        <v>10</v>
+      </c>
+      <c r="H509" s="4">
+        <v>11</v>
+      </c>
+      <c r="I509" s="4">
+        <v>13</v>
+      </c>
+      <c r="J509" s="4">
+        <v>15</v>
+      </c>
+      <c r="K509" s="4">
+        <v>17</v>
+      </c>
+      <c r="L509" s="4">
+        <v>19</v>
+      </c>
+      <c r="M509" s="4">
+        <v>20</v>
+      </c>
+      <c r="N509" s="4">
+        <v>21</v>
+      </c>
+      <c r="O509" s="4">
+        <v>23</v>
+      </c>
+      <c r="P509" s="4">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="510" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A510" s="3">
+        <v>3580</v>
+      </c>
+      <c r="B510" s="4">
+        <v>1</v>
+      </c>
+      <c r="C510" s="4">
+        <v>4</v>
+      </c>
+      <c r="D510" s="4">
+        <v>5</v>
+      </c>
+      <c r="E510" s="4">
+        <v>6</v>
+      </c>
+      <c r="F510" s="4">
+        <v>8</v>
+      </c>
+      <c r="G510" s="4">
+        <v>9</v>
+      </c>
+      <c r="H510" s="4">
+        <v>12</v>
+      </c>
+      <c r="I510" s="4">
+        <v>13</v>
+      </c>
+      <c r="J510" s="4">
+        <v>15</v>
+      </c>
+      <c r="K510" s="4">
+        <v>16</v>
+      </c>
+      <c r="L510" s="4">
+        <v>19</v>
+      </c>
+      <c r="M510" s="4">
+        <v>20</v>
+      </c>
+      <c r="N510" s="4">
+        <v>21</v>
+      </c>
+      <c r="O510" s="4">
+        <v>23</v>
+      </c>
+      <c r="P510" s="4">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="511" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A511" s="3">
+        <v>3581</v>
+      </c>
+      <c r="B511" s="4">
+        <v>2</v>
+      </c>
+      <c r="C511" s="4">
+        <v>3</v>
+      </c>
+      <c r="D511" s="4">
+        <v>4</v>
+      </c>
+      <c r="E511" s="4">
+        <v>5</v>
+      </c>
+      <c r="F511" s="4">
+        <v>6</v>
+      </c>
+      <c r="G511" s="4">
+        <v>7</v>
+      </c>
+      <c r="H511" s="4">
+        <v>8</v>
+      </c>
+      <c r="I511" s="4">
+        <v>10</v>
+      </c>
+      <c r="J511" s="4">
+        <v>12</v>
+      </c>
+      <c r="K511" s="4">
+        <v>15</v>
+      </c>
+      <c r="L511" s="4">
+        <v>16</v>
+      </c>
+      <c r="M511" s="4">
+        <v>17</v>
+      </c>
+      <c r="N511" s="4">
+        <v>20</v>
+      </c>
+      <c r="O511" s="4">
+        <v>22</v>
+      </c>
+      <c r="P511" s="4">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="512" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A512" s="3">
+        <v>3582</v>
+      </c>
+      <c r="B512" s="4">
+        <v>2</v>
+      </c>
+      <c r="C512" s="4">
+        <v>5</v>
+      </c>
+      <c r="D512" s="4">
+        <v>6</v>
+      </c>
+      <c r="E512" s="4">
+        <v>7</v>
+      </c>
+      <c r="F512" s="4">
+        <v>8</v>
+      </c>
+      <c r="G512" s="4">
+        <v>9</v>
+      </c>
+      <c r="H512" s="4">
+        <v>10</v>
+      </c>
+      <c r="I512" s="4">
+        <v>11</v>
+      </c>
+      <c r="J512" s="4">
+        <v>12</v>
+      </c>
+      <c r="K512" s="4">
+        <v>13</v>
+      </c>
+      <c r="L512" s="4">
+        <v>16</v>
+      </c>
+      <c r="M512" s="4">
+        <v>18</v>
+      </c>
+      <c r="N512" s="4">
+        <v>23</v>
+      </c>
+      <c r="O512" s="4">
+        <v>24</v>
+      </c>
+      <c r="P512" s="4">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="513" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A513" s="3">
+        <v>3583</v>
+      </c>
+      <c r="B513" s="4">
+        <v>2</v>
+      </c>
+      <c r="C513" s="4">
+        <v>3</v>
+      </c>
+      <c r="D513" s="4">
+        <v>4</v>
+      </c>
+      <c r="E513" s="4">
+        <v>6</v>
+      </c>
+      <c r="F513" s="4">
+        <v>9</v>
+      </c>
+      <c r="G513" s="4">
+        <v>10</v>
+      </c>
+      <c r="H513" s="4">
+        <v>12</v>
+      </c>
+      <c r="I513" s="4">
+        <v>13</v>
+      </c>
+      <c r="J513" s="4">
+        <v>14</v>
+      </c>
+      <c r="K513" s="4">
+        <v>15</v>
+      </c>
+      <c r="L513" s="4">
+        <v>21</v>
+      </c>
+      <c r="M513" s="4">
+        <v>22</v>
+      </c>
+      <c r="N513" s="4">
+        <v>23</v>
+      </c>
+      <c r="O513" s="4">
+        <v>24</v>
+      </c>
+      <c r="P513" s="4">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="514" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A514" s="3">
+        <v>3584</v>
+      </c>
+      <c r="B514" s="4">
+        <v>1</v>
+      </c>
+      <c r="C514" s="4">
+        <v>2</v>
+      </c>
+      <c r="D514" s="4">
+        <v>4</v>
+      </c>
+      <c r="E514" s="4">
+        <v>7</v>
+      </c>
+      <c r="F514" s="4">
+        <v>8</v>
+      </c>
+      <c r="G514" s="4">
+        <v>9</v>
+      </c>
+      <c r="H514" s="4">
+        <v>13</v>
+      </c>
+      <c r="I514" s="4">
+        <v>15</v>
+      </c>
+      <c r="J514" s="4">
+        <v>16</v>
+      </c>
+      <c r="K514" s="4">
+        <v>17</v>
+      </c>
+      <c r="L514" s="4">
+        <v>18</v>
+      </c>
+      <c r="M514" s="4">
+        <v>20</v>
+      </c>
+      <c r="N514" s="4">
+        <v>21</v>
+      </c>
+      <c r="O514" s="4">
+        <v>23</v>
+      </c>
+      <c r="P514" s="4">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="515" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A515" s="3">
+        <v>3585</v>
+      </c>
+      <c r="B515" s="4">
+        <v>1</v>
+      </c>
+      <c r="C515" s="4">
+        <v>2</v>
+      </c>
+      <c r="D515" s="4">
+        <v>4</v>
+      </c>
+      <c r="E515" s="4">
+        <v>8</v>
+      </c>
+      <c r="F515" s="4">
+        <v>9</v>
+      </c>
+      <c r="G515" s="4">
+        <v>10</v>
+      </c>
+      <c r="H515" s="4">
+        <v>13</v>
+      </c>
+      <c r="I515" s="4">
+        <v>16</v>
+      </c>
+      <c r="J515" s="4">
+        <v>17</v>
+      </c>
+      <c r="K515" s="4">
+        <v>19</v>
+      </c>
+      <c r="L515" s="4">
+        <v>20</v>
+      </c>
+      <c r="M515" s="4">
+        <v>21</v>
+      </c>
+      <c r="N515" s="4">
+        <v>22</v>
+      </c>
+      <c r="O515" s="4">
+        <v>23</v>
+      </c>
+      <c r="P515" s="4">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="516" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A516" s="3">
+        <v>3586</v>
+      </c>
+      <c r="B516" s="4">
+        <v>1</v>
+      </c>
+      <c r="C516" s="4">
+        <v>2</v>
+      </c>
+      <c r="D516" s="4">
+        <v>6</v>
+      </c>
+      <c r="E516" s="4">
+        <v>10</v>
+      </c>
+      <c r="F516" s="4">
+        <v>11</v>
+      </c>
+      <c r="G516" s="4">
+        <v>12</v>
+      </c>
+      <c r="H516" s="4">
+        <v>13</v>
+      </c>
+      <c r="I516" s="4">
+        <v>14</v>
+      </c>
+      <c r="J516" s="4">
+        <v>15</v>
+      </c>
+      <c r="K516" s="4">
+        <v>17</v>
+      </c>
+      <c r="L516" s="4">
+        <v>18</v>
+      </c>
+      <c r="M516" s="4">
+        <v>21</v>
+      </c>
+      <c r="N516" s="4">
+        <v>22</v>
+      </c>
+      <c r="O516" s="4">
+        <v>24</v>
+      </c>
+      <c r="P516" s="4">
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -25378,6 +26299,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100C92CDE8829F3C7438DCCB0991C30EAAE" ma:contentTypeVersion="3" ma:contentTypeDescription="Crie um novo documento." ma:contentTypeScope="" ma:versionID="36cf41eecaf38ba1d849a0c8dd067090">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="3e38fcf2-aa96-4a2c-865b-c3abba01ba51" xmlns:ns3="4455b8ba-124f-46d5-aaaa-9813efd83d1e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="023f68b2d27389a617bf935a3f0e17ad" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -25545,15 +26475,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -25565,6 +26486,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{82B637BD-743B-452C-A85E-33AF8B93F052}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{46C5B8C5-4575-4105-836C-9C4A6674A14B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -25584,14 +26513,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{82B637BD-743B-452C-A85E-33AF8B93F052}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0328C38C-FE97-4791-8469-4B5D9CCC5D08}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
atualizando arquivos dados xlsx loterias
</commit_message>
<xml_diff>
--- a/LoteriasExcel/Lotofacil_edt2.xlsx
+++ b/LoteriasExcel/Lotofacil_edt2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29725"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\Dropbox\! 000 ByPass\Pessoal\99_Loterias\0 - Loterias-Inteligentes\LoteriasExcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2189B7F7-F9A5-436F-BF63-8D9E901457C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{340A7A47-225E-4B71-B5CA-459FE5A61885}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57615" yWindow="1275" windowWidth="19125" windowHeight="16920" tabRatio="876" xr2:uid="{2663372B-AA50-4721-AD6B-5F0B8186ACF5}"/>
+    <workbookView xWindow="78510" yWindow="735" windowWidth="17280" windowHeight="18765" tabRatio="876" xr2:uid="{2663372B-AA50-4721-AD6B-5F0B8186ACF5}"/>
   </bookViews>
   <sheets>
     <sheet name="LOTOFÁCIL" sheetId="3" r:id="rId1"/>
@@ -476,11 +476,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69BEFC42-DD13-4DE0-B2AD-D0F44AF8189C}">
-  <dimension ref="A1:P529"/>
+  <dimension ref="A1:P541"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A508" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P529" sqref="P529"/>
+      <selection pane="bottomLeft" activeCell="B530" sqref="B530:P541"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -26941,12 +26941,622 @@
         <v>24</v>
       </c>
     </row>
+    <row r="530" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A530">
+        <v>3600</v>
+      </c>
+      <c r="B530">
+        <v>3</v>
+      </c>
+      <c r="C530">
+        <v>4</v>
+      </c>
+      <c r="D530">
+        <v>5</v>
+      </c>
+      <c r="E530">
+        <v>6</v>
+      </c>
+      <c r="F530">
+        <v>7</v>
+      </c>
+      <c r="G530">
+        <v>8</v>
+      </c>
+      <c r="H530">
+        <v>9</v>
+      </c>
+      <c r="I530">
+        <v>11</v>
+      </c>
+      <c r="J530">
+        <v>12</v>
+      </c>
+      <c r="K530">
+        <v>16</v>
+      </c>
+      <c r="L530">
+        <v>17</v>
+      </c>
+      <c r="M530">
+        <v>20</v>
+      </c>
+      <c r="N530">
+        <v>21</v>
+      </c>
+      <c r="O530">
+        <v>22</v>
+      </c>
+      <c r="P530">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="531" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A531">
+        <v>3601</v>
+      </c>
+      <c r="B531">
+        <v>2</v>
+      </c>
+      <c r="C531">
+        <v>3</v>
+      </c>
+      <c r="D531">
+        <v>4</v>
+      </c>
+      <c r="E531">
+        <v>6</v>
+      </c>
+      <c r="F531">
+        <v>7</v>
+      </c>
+      <c r="G531">
+        <v>8</v>
+      </c>
+      <c r="H531">
+        <v>9</v>
+      </c>
+      <c r="I531">
+        <v>11</v>
+      </c>
+      <c r="J531">
+        <v>16</v>
+      </c>
+      <c r="K531">
+        <v>17</v>
+      </c>
+      <c r="L531">
+        <v>20</v>
+      </c>
+      <c r="M531">
+        <v>21</v>
+      </c>
+      <c r="N531">
+        <v>23</v>
+      </c>
+      <c r="O531">
+        <v>24</v>
+      </c>
+      <c r="P531">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="532" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A532">
+        <v>3602</v>
+      </c>
+      <c r="B532">
+        <v>1</v>
+      </c>
+      <c r="C532">
+        <v>2</v>
+      </c>
+      <c r="D532">
+        <v>3</v>
+      </c>
+      <c r="E532">
+        <v>4</v>
+      </c>
+      <c r="F532">
+        <v>5</v>
+      </c>
+      <c r="G532">
+        <v>6</v>
+      </c>
+      <c r="H532">
+        <v>8</v>
+      </c>
+      <c r="I532">
+        <v>9</v>
+      </c>
+      <c r="J532">
+        <v>15</v>
+      </c>
+      <c r="K532">
+        <v>18</v>
+      </c>
+      <c r="L532">
+        <v>19</v>
+      </c>
+      <c r="M532">
+        <v>20</v>
+      </c>
+      <c r="N532">
+        <v>22</v>
+      </c>
+      <c r="O532">
+        <v>23</v>
+      </c>
+      <c r="P532">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="533" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A533">
+        <v>3603</v>
+      </c>
+      <c r="B533">
+        <v>2</v>
+      </c>
+      <c r="C533">
+        <v>4</v>
+      </c>
+      <c r="D533">
+        <v>5</v>
+      </c>
+      <c r="E533">
+        <v>9</v>
+      </c>
+      <c r="F533">
+        <v>10</v>
+      </c>
+      <c r="G533">
+        <v>11</v>
+      </c>
+      <c r="H533">
+        <v>12</v>
+      </c>
+      <c r="I533">
+        <v>14</v>
+      </c>
+      <c r="J533">
+        <v>15</v>
+      </c>
+      <c r="K533">
+        <v>17</v>
+      </c>
+      <c r="L533">
+        <v>19</v>
+      </c>
+      <c r="M533">
+        <v>20</v>
+      </c>
+      <c r="N533">
+        <v>21</v>
+      </c>
+      <c r="O533">
+        <v>22</v>
+      </c>
+      <c r="P533">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="534" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A534">
+        <v>3604</v>
+      </c>
+      <c r="B534">
+        <v>1</v>
+      </c>
+      <c r="C534">
+        <v>2</v>
+      </c>
+      <c r="D534">
+        <v>3</v>
+      </c>
+      <c r="E534">
+        <v>6</v>
+      </c>
+      <c r="F534">
+        <v>7</v>
+      </c>
+      <c r="G534">
+        <v>8</v>
+      </c>
+      <c r="H534">
+        <v>11</v>
+      </c>
+      <c r="I534">
+        <v>13</v>
+      </c>
+      <c r="J534">
+        <v>15</v>
+      </c>
+      <c r="K534">
+        <v>16</v>
+      </c>
+      <c r="L534">
+        <v>19</v>
+      </c>
+      <c r="M534">
+        <v>21</v>
+      </c>
+      <c r="N534">
+        <v>22</v>
+      </c>
+      <c r="O534">
+        <v>23</v>
+      </c>
+      <c r="P534">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="535" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A535">
+        <v>3605</v>
+      </c>
+      <c r="B535">
+        <v>1</v>
+      </c>
+      <c r="C535">
+        <v>3</v>
+      </c>
+      <c r="D535">
+        <v>4</v>
+      </c>
+      <c r="E535">
+        <v>7</v>
+      </c>
+      <c r="F535">
+        <v>10</v>
+      </c>
+      <c r="G535">
+        <v>12</v>
+      </c>
+      <c r="H535">
+        <v>13</v>
+      </c>
+      <c r="I535">
+        <v>14</v>
+      </c>
+      <c r="J535">
+        <v>19</v>
+      </c>
+      <c r="K535">
+        <v>20</v>
+      </c>
+      <c r="L535">
+        <v>21</v>
+      </c>
+      <c r="M535">
+        <v>22</v>
+      </c>
+      <c r="N535">
+        <v>23</v>
+      </c>
+      <c r="O535">
+        <v>24</v>
+      </c>
+      <c r="P535">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="536" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A536">
+        <v>3606</v>
+      </c>
+      <c r="B536">
+        <v>2</v>
+      </c>
+      <c r="C536">
+        <v>3</v>
+      </c>
+      <c r="D536">
+        <v>6</v>
+      </c>
+      <c r="E536">
+        <v>7</v>
+      </c>
+      <c r="F536">
+        <v>9</v>
+      </c>
+      <c r="G536">
+        <v>11</v>
+      </c>
+      <c r="H536">
+        <v>12</v>
+      </c>
+      <c r="I536">
+        <v>14</v>
+      </c>
+      <c r="J536">
+        <v>15</v>
+      </c>
+      <c r="K536">
+        <v>17</v>
+      </c>
+      <c r="L536">
+        <v>19</v>
+      </c>
+      <c r="M536">
+        <v>20</v>
+      </c>
+      <c r="N536">
+        <v>21</v>
+      </c>
+      <c r="O536">
+        <v>23</v>
+      </c>
+      <c r="P536">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="537" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A537">
+        <v>3607</v>
+      </c>
+      <c r="B537">
+        <v>1</v>
+      </c>
+      <c r="C537">
+        <v>2</v>
+      </c>
+      <c r="D537">
+        <v>4</v>
+      </c>
+      <c r="E537">
+        <v>5</v>
+      </c>
+      <c r="F537">
+        <v>6</v>
+      </c>
+      <c r="G537">
+        <v>8</v>
+      </c>
+      <c r="H537">
+        <v>9</v>
+      </c>
+      <c r="I537">
+        <v>13</v>
+      </c>
+      <c r="J537">
+        <v>14</v>
+      </c>
+      <c r="K537">
+        <v>15</v>
+      </c>
+      <c r="L537">
+        <v>16</v>
+      </c>
+      <c r="M537">
+        <v>18</v>
+      </c>
+      <c r="N537">
+        <v>19</v>
+      </c>
+      <c r="O537">
+        <v>20</v>
+      </c>
+      <c r="P537">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="538" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A538">
+        <v>3608</v>
+      </c>
+      <c r="B538">
+        <v>2</v>
+      </c>
+      <c r="C538">
+        <v>5</v>
+      </c>
+      <c r="D538">
+        <v>6</v>
+      </c>
+      <c r="E538">
+        <v>8</v>
+      </c>
+      <c r="F538">
+        <v>9</v>
+      </c>
+      <c r="G538">
+        <v>11</v>
+      </c>
+      <c r="H538">
+        <v>14</v>
+      </c>
+      <c r="I538">
+        <v>16</v>
+      </c>
+      <c r="J538">
+        <v>17</v>
+      </c>
+      <c r="K538">
+        <v>18</v>
+      </c>
+      <c r="L538">
+        <v>19</v>
+      </c>
+      <c r="M538">
+        <v>20</v>
+      </c>
+      <c r="N538">
+        <v>22</v>
+      </c>
+      <c r="O538">
+        <v>23</v>
+      </c>
+      <c r="P538">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="539" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A539">
+        <v>3609</v>
+      </c>
+      <c r="B539">
+        <v>2</v>
+      </c>
+      <c r="C539">
+        <v>5</v>
+      </c>
+      <c r="D539">
+        <v>6</v>
+      </c>
+      <c r="E539">
+        <v>8</v>
+      </c>
+      <c r="F539">
+        <v>9</v>
+      </c>
+      <c r="G539">
+        <v>10</v>
+      </c>
+      <c r="H539">
+        <v>11</v>
+      </c>
+      <c r="I539">
+        <v>12</v>
+      </c>
+      <c r="J539">
+        <v>13</v>
+      </c>
+      <c r="K539">
+        <v>17</v>
+      </c>
+      <c r="L539">
+        <v>19</v>
+      </c>
+      <c r="M539">
+        <v>20</v>
+      </c>
+      <c r="N539">
+        <v>22</v>
+      </c>
+      <c r="O539">
+        <v>24</v>
+      </c>
+      <c r="P539">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="540" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A540">
+        <v>3610</v>
+      </c>
+      <c r="B540">
+        <v>1</v>
+      </c>
+      <c r="C540">
+        <v>3</v>
+      </c>
+      <c r="D540">
+        <v>5</v>
+      </c>
+      <c r="E540">
+        <v>7</v>
+      </c>
+      <c r="F540">
+        <v>8</v>
+      </c>
+      <c r="G540">
+        <v>10</v>
+      </c>
+      <c r="H540">
+        <v>13</v>
+      </c>
+      <c r="I540">
+        <v>14</v>
+      </c>
+      <c r="J540">
+        <v>17</v>
+      </c>
+      <c r="K540">
+        <v>20</v>
+      </c>
+      <c r="L540">
+        <v>21</v>
+      </c>
+      <c r="M540">
+        <v>22</v>
+      </c>
+      <c r="N540">
+        <v>23</v>
+      </c>
+      <c r="O540">
+        <v>24</v>
+      </c>
+      <c r="P540">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="541" spans="1:16" x14ac:dyDescent="0.4">
+      <c r="A541">
+        <v>3611</v>
+      </c>
+      <c r="B541">
+        <v>1</v>
+      </c>
+      <c r="C541">
+        <v>2</v>
+      </c>
+      <c r="D541">
+        <v>3</v>
+      </c>
+      <c r="E541">
+        <v>4</v>
+      </c>
+      <c r="F541">
+        <v>5</v>
+      </c>
+      <c r="G541">
+        <v>6</v>
+      </c>
+      <c r="H541">
+        <v>10</v>
+      </c>
+      <c r="I541">
+        <v>11</v>
+      </c>
+      <c r="J541">
+        <v>12</v>
+      </c>
+      <c r="K541">
+        <v>14</v>
+      </c>
+      <c r="L541">
+        <v>15</v>
+      </c>
+      <c r="M541">
+        <v>17</v>
+      </c>
+      <c r="N541">
+        <v>18</v>
+      </c>
+      <c r="O541">
+        <v>19</v>
+      </c>
+      <c r="P541">
+        <v>25</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <PublishingExpirationDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <PublishingStartDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <AtualizadoPeloTimerJobEm xmlns="4455b8ba-124f-46d5-aaaa-9813efd83d1e">2025-08-17T04:03:58+00:00</AtualizadoPeloTimerJobEm>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100C92CDE8829F3C7438DCCB0991C30EAAE" ma:contentTypeVersion="3" ma:contentTypeDescription="Crie um novo documento." ma:contentTypeScope="" ma:versionID="36cf41eecaf38ba1d849a0c8dd067090">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="3e38fcf2-aa96-4a2c-865b-c3abba01ba51" xmlns:ns3="4455b8ba-124f-46d5-aaaa-9813efd83d1e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="023f68b2d27389a617bf935a3f0e17ad" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -27114,16 +27724,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <PublishingExpirationDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <PublishingStartDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <AtualizadoPeloTimerJobEm xmlns="4455b8ba-124f-46d5-aaaa-9813efd83d1e">2025-08-17T04:03:58+00:00</AtualizadoPeloTimerJobEm>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -27134,6 +27734,17 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0328C38C-FE97-4791-8469-4B5D9CCC5D08}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="4455b8ba-124f-46d5-aaaa-9813efd83d1e"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{46C5B8C5-4575-4105-836C-9C4A6674A14B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -27153,17 +27764,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0328C38C-FE97-4791-8469-4B5D9CCC5D08}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="4455b8ba-124f-46d5-aaaa-9813efd83d1e"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{82B637BD-743B-452C-A85E-33AF8B93F052}">
   <ds:schemaRefs>

</xml_diff>